<commit_message>
added more models and updated using odds at 3pm
</commit_message>
<xml_diff>
--- a/data/data_wc2014.xlsx
+++ b/data/data_wc2014.xlsx
@@ -395,12 +395,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -437,11 +431,17 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1496,7 @@
       </c>
     </row>
     <row r="4" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35">
+      <c r="B4" s="32">
         <v>1</v>
       </c>
       <c r="C4" s="10">
@@ -1570,15 +1570,15 @@
         <f>U4-V4</f>
         <v>4</v>
       </c>
-      <c r="Y4" s="20" t="s">
+      <c r="Y4" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="Z4" s="21" t="s">
+      <c r="Z4" s="34" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5" s="35">
+      <c r="B5" s="32">
         <v>2</v>
       </c>
       <c r="C5" s="10">
@@ -1600,13 +1600,13 @@
         <v>30</v>
       </c>
       <c r="I5" s="16">
-        <v>2.25</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="J5" s="16">
-        <v>3.2</v>
+        <v>3.95</v>
       </c>
       <c r="K5" s="16">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="L5" s="16">
         <f>VLOOKUP($D5,'538'!$B$3:$F$34,3,FALSE)</f>
@@ -1652,11 +1652,11 @@
         <f t="shared" ref="W5:W22" si="1">U5-V5</f>
         <v>1</v>
       </c>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="21"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="34"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="35">
+      <c r="B6" s="32">
         <v>3</v>
       </c>
       <c r="C6" s="10">
@@ -1678,13 +1678,13 @@
         <v>25</v>
       </c>
       <c r="I6" s="16">
-        <v>1.8</v>
+        <v>1.87</v>
       </c>
       <c r="J6" s="16">
-        <v>3.4</v>
+        <v>5.5</v>
       </c>
       <c r="K6" s="16">
-        <v>5.5</v>
+        <v>3.45</v>
       </c>
       <c r="L6" s="16">
         <f>VLOOKUP($D6,'538'!$B$3:$F$34,3,FALSE)</f>
@@ -1730,11 +1730,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="21"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="34"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="35">
+      <c r="B7" s="32">
         <v>4</v>
       </c>
       <c r="C7" s="10">
@@ -1756,13 +1756,13 @@
         <v>19</v>
       </c>
       <c r="I7" s="16">
-        <v>1.44</v>
+        <v>1.51</v>
       </c>
       <c r="J7" s="16">
-        <v>4.5</v>
+        <v>9.4</v>
       </c>
       <c r="K7" s="16">
-        <v>10</v>
+        <v>4.3</v>
       </c>
       <c r="L7" s="16">
         <f>VLOOKUP($D7,'538'!$B$3:$F$34,3,FALSE)</f>
@@ -1808,11 +1808,11 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="21"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="34"/>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="35">
+      <c r="B8" s="32">
         <v>5</v>
       </c>
       <c r="C8" s="8">
@@ -1886,12 +1886,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Z8" s="34" t="s">
+      <c r="Z8" s="35" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="35">
+      <c r="B9" s="32">
         <v>6</v>
       </c>
       <c r="C9" s="8">
@@ -1965,10 +1965,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Z9" s="34"/>
+      <c r="Z9" s="35"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="35">
+      <c r="B10" s="32">
         <v>7</v>
       </c>
       <c r="C10" s="8">
@@ -2042,10 +2042,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z10" s="34"/>
+      <c r="Z10" s="35"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B11" s="35">
+      <c r="B11" s="32">
         <v>8</v>
       </c>
       <c r="C11" s="8">
@@ -2119,10 +2119,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z11" s="34"/>
+      <c r="Z11" s="35"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B12" s="35">
+      <c r="B12" s="32">
         <v>9</v>
       </c>
       <c r="C12" s="8">
@@ -2198,7 +2198,7 @@
       </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="35">
+      <c r="B13" s="32">
         <v>10</v>
       </c>
       <c r="C13" s="8">
@@ -2274,7 +2274,7 @@
       </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="35">
+      <c r="B14" s="32">
         <v>11</v>
       </c>
       <c r="C14" s="8">
@@ -2350,7 +2350,7 @@
       </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B15" s="35">
+      <c r="B15" s="32">
         <v>12</v>
       </c>
       <c r="C15" s="8">
@@ -2426,7 +2426,7 @@
       </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B16" s="35">
+      <c r="B16" s="32">
         <v>13</v>
       </c>
       <c r="C16" s="8">
@@ -2502,7 +2502,7 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
+      <c r="B17" s="32">
         <v>14</v>
       </c>
       <c r="C17" s="8">
@@ -2578,7 +2578,7 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="35">
+      <c r="B18" s="32">
         <v>15</v>
       </c>
       <c r="C18" s="8">
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B19" s="35">
+      <c r="B19" s="32">
         <v>16</v>
       </c>
       <c r="C19" s="8">
@@ -2730,7 +2730,7 @@
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B20" s="35">
+      <c r="B20" s="32">
         <v>17</v>
       </c>
       <c r="C20" s="8">
@@ -2806,7 +2806,7 @@
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B21" s="35">
+      <c r="B21" s="32">
         <v>18</v>
       </c>
       <c r="C21" s="8">
@@ -2882,7 +2882,7 @@
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B22" s="35">
+      <c r="B22" s="32">
         <v>19</v>
       </c>
       <c r="C22" s="8"/>
@@ -2932,7 +2932,7 @@
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="35">
+      <c r="B23" s="32">
         <v>20</v>
       </c>
       <c r="C23" s="8"/>
@@ -2982,7 +2982,7 @@
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="35">
+      <c r="B24" s="32">
         <v>21</v>
       </c>
       <c r="C24" s="8"/>
@@ -3032,7 +3032,7 @@
       </c>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B25" s="35">
+      <c r="B25" s="32">
         <v>22</v>
       </c>
       <c r="C25" s="8"/>
@@ -3082,7 +3082,7 @@
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B26" s="35">
+      <c r="B26" s="32">
         <v>23</v>
       </c>
       <c r="C26" s="8"/>
@@ -3132,7 +3132,7 @@
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B27" s="35">
+      <c r="B27" s="32">
         <v>24</v>
       </c>
       <c r="C27" s="8"/>
@@ -3182,7 +3182,7 @@
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B28" s="35">
+      <c r="B28" s="32">
         <v>25</v>
       </c>
       <c r="C28" s="8"/>
@@ -3232,7 +3232,7 @@
       </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="35">
+      <c r="B29" s="32">
         <v>26</v>
       </c>
       <c r="C29" s="8"/>
@@ -3282,7 +3282,7 @@
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="35">
+      <c r="B30" s="32">
         <v>27</v>
       </c>
       <c r="C30" s="8"/>
@@ -3332,7 +3332,7 @@
       </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B31" s="35">
+      <c r="B31" s="32">
         <v>28</v>
       </c>
       <c r="C31" s="8"/>
@@ -3382,7 +3382,7 @@
       </c>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="35">
+      <c r="B32" s="32">
         <v>29</v>
       </c>
       <c r="C32" s="8"/>
@@ -3432,7 +3432,7 @@
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B33" s="35">
+      <c r="B33" s="32">
         <v>30</v>
       </c>
       <c r="C33" s="8"/>
@@ -3482,7 +3482,7 @@
       </c>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="35">
+      <c r="B34" s="32">
         <v>31</v>
       </c>
       <c r="C34" s="8"/>
@@ -3532,7 +3532,7 @@
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="35">
+      <c r="B35" s="32">
         <v>32</v>
       </c>
       <c r="C35" s="8"/>
@@ -3582,7 +3582,7 @@
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B36" s="35">
+      <c r="B36" s="32">
         <v>33</v>
       </c>
       <c r="C36" s="8"/>
@@ -3632,7 +3632,7 @@
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="35">
+      <c r="B37" s="32">
         <v>34</v>
       </c>
       <c r="C37" s="8"/>
@@ -3682,7 +3682,7 @@
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="35">
+      <c r="B38" s="32">
         <v>35</v>
       </c>
       <c r="C38" s="8"/>
@@ -3732,7 +3732,7 @@
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="35">
+      <c r="B39" s="32">
         <v>36</v>
       </c>
       <c r="C39" s="8"/>
@@ -3782,7 +3782,7 @@
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="35">
+      <c r="B40" s="32">
         <v>37</v>
       </c>
       <c r="C40" s="8"/>
@@ -3832,7 +3832,7 @@
       </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="35">
+      <c r="B41" s="32">
         <v>38</v>
       </c>
       <c r="C41" s="8"/>
@@ -3882,7 +3882,7 @@
       </c>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42" s="35">
+      <c r="B42" s="32">
         <v>39</v>
       </c>
       <c r="C42" s="8"/>
@@ -3932,7 +3932,7 @@
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B43" s="35">
+      <c r="B43" s="32">
         <v>40</v>
       </c>
       <c r="C43" s="8"/>
@@ -3982,7 +3982,7 @@
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="35">
+      <c r="B44" s="32">
         <v>41</v>
       </c>
       <c r="C44" s="8"/>
@@ -4032,7 +4032,7 @@
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" s="35">
+      <c r="B45" s="32">
         <v>42</v>
       </c>
       <c r="C45" s="8"/>
@@ -4082,7 +4082,7 @@
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B46" s="35">
+      <c r="B46" s="32">
         <v>43</v>
       </c>
       <c r="C46" s="8"/>
@@ -4132,7 +4132,7 @@
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B47" s="35">
+      <c r="B47" s="32">
         <v>44</v>
       </c>
       <c r="C47" s="8"/>
@@ -4182,7 +4182,7 @@
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B48" s="35">
+      <c r="B48" s="32">
         <v>45</v>
       </c>
       <c r="C48" s="8"/>
@@ -4232,7 +4232,7 @@
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49" s="35">
+      <c r="B49" s="32">
         <v>46</v>
       </c>
       <c r="C49" s="8"/>
@@ -4282,7 +4282,7 @@
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50" s="35">
+      <c r="B50" s="32">
         <v>47</v>
       </c>
       <c r="C50" s="8"/>
@@ -4332,7 +4332,7 @@
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B51" s="35">
+      <c r="B51" s="32">
         <v>48</v>
       </c>
       <c r="C51" s="8"/>
@@ -4382,7 +4382,7 @@
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52" s="35">
+      <c r="B52" s="32">
         <v>49</v>
       </c>
       <c r="C52" s="8"/>
@@ -4432,7 +4432,7 @@
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B53" s="35">
+      <c r="B53" s="32">
         <v>50</v>
       </c>
       <c r="C53" s="8"/>
@@ -4482,7 +4482,7 @@
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B54" s="35">
+      <c r="B54" s="32">
         <v>51</v>
       </c>
       <c r="C54" s="8"/>
@@ -4532,7 +4532,7 @@
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B55" s="35">
+      <c r="B55" s="32">
         <v>52</v>
       </c>
       <c r="C55" s="8"/>
@@ -4582,7 +4582,7 @@
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B56" s="35">
+      <c r="B56" s="32">
         <v>53</v>
       </c>
       <c r="C56" s="8"/>
@@ -4632,7 +4632,7 @@
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B57" s="35">
+      <c r="B57" s="32">
         <v>54</v>
       </c>
       <c r="C57" s="8"/>
@@ -4682,7 +4682,7 @@
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B58" s="35">
+      <c r="B58" s="32">
         <v>55</v>
       </c>
       <c r="C58" s="8"/>
@@ -4732,7 +4732,7 @@
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B59" s="35">
+      <c r="B59" s="32">
         <v>56</v>
       </c>
       <c r="C59" s="8"/>
@@ -4782,7 +4782,7 @@
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B60" s="35">
+      <c r="B60" s="32">
         <v>57</v>
       </c>
       <c r="C60" s="8"/>
@@ -4832,7 +4832,7 @@
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B61" s="35">
+      <c r="B61" s="32">
         <v>58</v>
       </c>
       <c r="C61" s="8"/>
@@ -4882,7 +4882,7 @@
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B62" s="35">
+      <c r="B62" s="32">
         <v>59</v>
       </c>
       <c r="C62" s="8"/>
@@ -4932,7 +4932,7 @@
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B63" s="35">
+      <c r="B63" s="32">
         <v>60</v>
       </c>
       <c r="C63" s="8"/>
@@ -4982,7 +4982,7 @@
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B64" s="35">
+      <c r="B64" s="32">
         <v>61</v>
       </c>
       <c r="C64" s="8"/>
@@ -5032,7 +5032,7 @@
       </c>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B65" s="35">
+      <c r="B65" s="32">
         <v>62</v>
       </c>
       <c r="C65" s="8"/>
@@ -5082,7 +5082,7 @@
       </c>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B66" s="35">
+      <c r="B66" s="32">
         <v>63</v>
       </c>
       <c r="C66" s="8"/>
@@ -5132,7 +5132,7 @@
       </c>
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B67" s="35">
+      <c r="B67" s="32">
         <v>64</v>
       </c>
       <c r="C67" s="8"/>
@@ -5284,1549 +5284,1549 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+      <c r="A2" s="20">
         <f>Main!C4</f>
         <v>41802</v>
       </c>
-      <c r="B2" s="23" t="str">
+      <c r="B2" s="21" t="str">
         <f>Main!D4</f>
         <v>Brazil</v>
       </c>
-      <c r="C2" s="23" t="str">
+      <c r="C2" s="21" t="str">
         <f>Main!E4</f>
         <v>Croatia</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="22">
         <f>Main!F4</f>
         <v>88</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="22">
         <f>Main!G4</f>
         <v>3</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="22">
         <f>Main!H4</f>
         <v>10</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="23">
         <f>Main!I4</f>
         <v>1.33</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="23">
         <f>Main!J4</f>
         <v>5</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="23">
         <f>Main!K4</f>
         <v>13</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2" s="23">
         <f>Main!L4</f>
         <v>91.8</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="23">
         <f>Main!M4</f>
         <v>3.4</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="23">
         <f>Main!N4</f>
         <v>0.5</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="23">
         <f>Main!O4</f>
         <v>75.7</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="23">
         <f>Main!P4</f>
         <v>1.8</v>
       </c>
-      <c r="O2" s="25">
+      <c r="O2" s="23">
         <f>Main!Q4</f>
         <v>0.9</v>
       </c>
-      <c r="P2" s="24">
+      <c r="P2" s="22">
         <f>Main!R4</f>
         <v>3</v>
       </c>
-      <c r="Q2" s="24">
+      <c r="Q2" s="22">
         <f>Main!S4</f>
         <v>1</v>
       </c>
-      <c r="R2" s="24">
+      <c r="R2" s="22">
         <f>Main!T4</f>
         <v>2</v>
       </c>
-      <c r="S2" s="24">
+      <c r="S2" s="22">
         <f>Main!U4</f>
         <v>4</v>
       </c>
-      <c r="T2" s="24">
+      <c r="T2" s="22">
         <f>Main!V4</f>
         <v>0</v>
       </c>
-      <c r="U2" s="24">
+      <c r="U2" s="22">
         <f>Main!W4</f>
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
+      <c r="A3" s="24">
         <f>Main!C5</f>
         <v>41803</v>
       </c>
-      <c r="B3" s="27" t="str">
+      <c r="B3" s="25" t="str">
         <f>Main!D5</f>
         <v>Mexico</v>
       </c>
-      <c r="C3" s="27" t="str">
+      <c r="C3" s="25" t="str">
         <f>Main!E5</f>
         <v>Cameroon</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="26">
         <f>Main!F5</f>
         <v>43</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="26">
         <f>Main!G5</f>
         <v>27</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="26">
         <f>Main!H5</f>
         <v>30</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="27">
         <f>Main!I5</f>
-        <v>2.25</v>
-      </c>
-      <c r="H3" s="29">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="H3" s="27">
         <f>Main!J5</f>
-        <v>3.2</v>
-      </c>
-      <c r="I3" s="29">
+        <v>3.95</v>
+      </c>
+      <c r="I3" s="27">
         <f>Main!K5</f>
-        <v>3.75</v>
-      </c>
-      <c r="J3" s="29">
+        <v>3.25</v>
+      </c>
+      <c r="J3" s="27">
         <f>Main!L5</f>
         <v>77</v>
       </c>
-      <c r="K3" s="29">
+      <c r="K3" s="27">
         <f>Main!M5</f>
         <v>1.6</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="27">
         <f>Main!N5</f>
         <v>0.7</v>
       </c>
-      <c r="M3" s="29">
+      <c r="M3" s="27">
         <f>Main!O5</f>
         <v>71.3</v>
       </c>
-      <c r="N3" s="29">
+      <c r="N3" s="27">
         <f>Main!P5</f>
         <v>1.5</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="27">
         <f>Main!Q5</f>
         <v>1</v>
       </c>
-      <c r="P3" s="28">
+      <c r="P3" s="26">
         <f>Main!R5</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="28">
+      <c r="Q3" s="26">
         <f>Main!S5</f>
         <v>0</v>
       </c>
-      <c r="R3" s="28">
+      <c r="R3" s="26">
         <f>Main!T5</f>
         <v>1</v>
       </c>
-      <c r="S3" s="28">
+      <c r="S3" s="26">
         <f>Main!U5</f>
         <v>1</v>
       </c>
-      <c r="T3" s="28">
+      <c r="T3" s="26">
         <f>Main!V5</f>
         <v>0</v>
       </c>
-      <c r="U3" s="28">
+      <c r="U3" s="26">
         <f>Main!W5</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="24">
         <f>Main!C6</f>
         <v>41803</v>
       </c>
-      <c r="B4" s="27" t="str">
+      <c r="B4" s="25" t="str">
         <f>Main!D6</f>
         <v>Spain</v>
       </c>
-      <c r="C4" s="27" t="str">
+      <c r="C4" s="25" t="str">
         <f>Main!E6</f>
         <v>Netherlands</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="26">
         <f>Main!F6</f>
         <v>53</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="26">
         <f>Main!G6</f>
         <v>21</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="26">
         <f>Main!H6</f>
         <v>25</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="27">
         <f>Main!I6</f>
-        <v>1.8</v>
-      </c>
-      <c r="H4" s="29">
+        <v>1.87</v>
+      </c>
+      <c r="H4" s="27">
         <f>Main!J6</f>
-        <v>3.4</v>
-      </c>
-      <c r="I4" s="29">
+        <v>5.5</v>
+      </c>
+      <c r="I4" s="27">
         <f>Main!K6</f>
-        <v>5.5</v>
-      </c>
-      <c r="J4" s="29">
+        <v>3.45</v>
+      </c>
+      <c r="J4" s="27">
         <f>Main!L6</f>
         <v>89.1</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="27">
         <f>Main!M6</f>
         <v>2.7</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="27">
         <f>Main!N6</f>
         <v>0.4</v>
       </c>
-      <c r="M4" s="29">
+      <c r="M4" s="27">
         <f>Main!O6</f>
         <v>82.5</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="27">
         <f>Main!P6</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="27">
         <f>Main!Q6</f>
         <v>0.8</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="26">
         <f>Main!R6</f>
         <v>1</v>
       </c>
-      <c r="Q4" s="28">
+      <c r="Q4" s="26">
         <f>Main!S6</f>
         <v>0</v>
       </c>
-      <c r="R4" s="28">
+      <c r="R4" s="26">
         <f>Main!T6</f>
         <v>1</v>
       </c>
-      <c r="S4" s="28">
+      <c r="S4" s="26">
         <f>Main!U6</f>
         <v>1</v>
       </c>
-      <c r="T4" s="28">
+      <c r="T4" s="26">
         <f>Main!V6</f>
         <v>0</v>
       </c>
-      <c r="U4" s="28">
+      <c r="U4" s="26">
         <f>Main!W6</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
+      <c r="A5" s="24">
         <f>Main!C7</f>
         <v>41803</v>
       </c>
-      <c r="B5" s="27" t="str">
+      <c r="B5" s="25" t="str">
         <f>Main!D7</f>
         <v>Chile</v>
       </c>
-      <c r="C5" s="27" t="str">
+      <c r="C5" s="25" t="str">
         <f>Main!E7</f>
         <v>Australia</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="26">
         <f>Main!F7</f>
         <v>72</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="26">
         <f>Main!G7</f>
         <v>9</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="26">
         <f>Main!H7</f>
         <v>19</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="27">
         <f>Main!I7</f>
-        <v>1.44</v>
-      </c>
-      <c r="H5" s="29">
+        <v>1.51</v>
+      </c>
+      <c r="H5" s="27">
         <f>Main!J7</f>
-        <v>4.5</v>
-      </c>
-      <c r="I5" s="29">
+        <v>9.4</v>
+      </c>
+      <c r="I5" s="27">
         <f>Main!K7</f>
-        <v>10</v>
-      </c>
-      <c r="J5" s="29">
+        <v>4.3</v>
+      </c>
+      <c r="J5" s="27">
         <f>Main!L7</f>
         <v>86.7</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="27">
         <f>Main!M7</f>
         <v>2.7</v>
       </c>
-      <c r="L5" s="29">
+      <c r="L5" s="27">
         <f>Main!N7</f>
         <v>0.7</v>
       </c>
-      <c r="M5" s="29">
+      <c r="M5" s="27">
         <f>Main!O7</f>
         <v>69.5</v>
       </c>
-      <c r="N5" s="29">
+      <c r="N5" s="27">
         <f>Main!P7</f>
         <v>1.6</v>
       </c>
-      <c r="O5" s="29">
+      <c r="O5" s="27">
         <f>Main!Q7</f>
         <v>1.2</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="26">
         <f>Main!R7</f>
         <v>2</v>
       </c>
-      <c r="Q5" s="28">
+      <c r="Q5" s="26">
         <f>Main!S7</f>
         <v>0</v>
       </c>
-      <c r="R5" s="28">
+      <c r="R5" s="26">
         <f>Main!T7</f>
         <v>2</v>
       </c>
-      <c r="S5" s="28">
+      <c r="S5" s="26">
         <f>Main!U7</f>
         <v>2</v>
       </c>
-      <c r="T5" s="28">
+      <c r="T5" s="26">
         <f>Main!V7</f>
         <v>0</v>
       </c>
-      <c r="U5" s="28">
+      <c r="U5" s="26">
         <f>Main!W7</f>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="28">
         <f>Main!C8</f>
         <v>41804</v>
       </c>
-      <c r="B6" s="31" t="str">
+      <c r="B6" s="29" t="str">
         <f>Main!D8</f>
         <v>Colombia</v>
       </c>
-      <c r="C6" s="31" t="str">
+      <c r="C6" s="29" t="str">
         <f>Main!E8</f>
         <v>Greece</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="30">
         <f>Main!F8</f>
         <v>54</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="30">
         <f>Main!G8</f>
         <v>19</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="30">
         <f>Main!H8</f>
         <v>27</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="31">
         <f>Main!I8</f>
         <v>1.85</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="31">
         <f>Main!J8</f>
         <v>3.3</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="31">
         <f>Main!K8</f>
         <v>5</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="31">
         <f>Main!L8</f>
         <v>85.8</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="31">
         <f>Main!M8</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="L6" s="33">
+      <c r="L6" s="31">
         <f>Main!N8</f>
         <v>0.5</v>
       </c>
-      <c r="M6" s="33">
+      <c r="M6" s="31">
         <f>Main!O8</f>
         <v>76.8</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6" s="31">
         <f>Main!P8</f>
         <v>1.3</v>
       </c>
-      <c r="O6" s="33">
+      <c r="O6" s="31">
         <f>Main!Q8</f>
         <v>0.5</v>
       </c>
-      <c r="P6" s="32">
+      <c r="P6" s="30">
         <f>Main!R8</f>
         <v>1</v>
       </c>
-      <c r="Q6" s="32">
+      <c r="Q6" s="30">
         <f>Main!S8</f>
         <v>0</v>
       </c>
-      <c r="R6" s="32">
+      <c r="R6" s="30">
         <f>Main!T8</f>
         <v>1</v>
       </c>
-      <c r="S6" s="32">
+      <c r="S6" s="30">
         <f>Main!U8</f>
         <v>1</v>
       </c>
-      <c r="T6" s="32">
+      <c r="T6" s="30">
         <f>Main!V8</f>
         <v>0</v>
       </c>
-      <c r="U6" s="32">
+      <c r="U6" s="30">
         <f>Main!W8</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
+      <c r="A7" s="28">
         <f>Main!C9</f>
         <v>41804</v>
       </c>
-      <c r="B7" s="31" t="str">
+      <c r="B7" s="29" t="str">
         <f>Main!D9</f>
         <v>Uruguay</v>
       </c>
-      <c r="C7" s="31" t="str">
+      <c r="C7" s="29" t="str">
         <f>Main!E9</f>
         <v>Costa Rica</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="30">
         <f>Main!F9</f>
         <v>54</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="30">
         <f>Main!G9</f>
         <v>19</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="30">
         <f>Main!H9</f>
         <v>27</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="31">
         <f>Main!I9</f>
         <v>1.44</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="31">
         <f>Main!J9</f>
         <v>4.5</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="31">
         <f>Main!K9</f>
         <v>9</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="31">
         <f>Main!L9</f>
         <v>83.3</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="31">
         <f>Main!M9</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="31">
         <f>Main!N9</f>
         <v>0.7</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="31">
         <f>Main!O9</f>
         <v>74.099999999999994</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="31">
         <f>Main!P9</f>
         <v>1.3</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="31">
         <f>Main!Q9</f>
         <v>0.7</v>
       </c>
-      <c r="P7" s="32">
+      <c r="P7" s="30">
         <f>Main!R9</f>
         <v>2</v>
       </c>
-      <c r="Q7" s="32">
+      <c r="Q7" s="30">
         <f>Main!S9</f>
         <v>0</v>
       </c>
-      <c r="R7" s="32">
+      <c r="R7" s="30">
         <f>Main!T9</f>
         <v>2</v>
       </c>
-      <c r="S7" s="32">
+      <c r="S7" s="30">
         <f>Main!U9</f>
         <v>2</v>
       </c>
-      <c r="T7" s="32">
+      <c r="T7" s="30">
         <f>Main!V9</f>
         <v>0</v>
       </c>
-      <c r="U7" s="32">
+      <c r="U7" s="30">
         <f>Main!W9</f>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
+      <c r="A8" s="28">
         <f>Main!C10</f>
         <v>41804</v>
       </c>
-      <c r="B8" s="31" t="str">
+      <c r="B8" s="29" t="str">
         <f>Main!D10</f>
         <v>England</v>
       </c>
-      <c r="C8" s="31" t="str">
+      <c r="C8" s="29" t="str">
         <f>Main!E10</f>
         <v>Italy</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="30">
         <f>Main!F10</f>
         <v>43</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="30">
         <f>Main!G10</f>
         <v>28</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="30">
         <f>Main!H10</f>
         <v>29</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="31">
         <f>Main!I10</f>
         <v>2.9</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="31">
         <f>Main!J10</f>
         <v>3</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="31">
         <f>Main!K10</f>
         <v>2.8</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="31">
         <f>Main!L10</f>
         <v>83.2</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="31">
         <f>Main!M10</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="31">
         <f>Main!N10</f>
         <v>0.7</v>
       </c>
-      <c r="M8" s="33">
+      <c r="M8" s="31">
         <f>Main!O10</f>
         <v>79.5</v>
       </c>
-      <c r="N8" s="33">
+      <c r="N8" s="31">
         <f>Main!P10</f>
         <v>2</v>
       </c>
-      <c r="O8" s="33">
+      <c r="O8" s="31">
         <f>Main!Q10</f>
         <v>0.8</v>
       </c>
-      <c r="P8" s="32">
+      <c r="P8" s="30">
         <f>Main!R10</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="32">
+      <c r="Q8" s="30">
         <f>Main!S10</f>
         <v>0</v>
       </c>
-      <c r="R8" s="32">
+      <c r="R8" s="30">
         <f>Main!T10</f>
         <v>0</v>
       </c>
-      <c r="S8" s="32">
+      <c r="S8" s="30">
         <f>Main!U10</f>
         <v>0</v>
       </c>
-      <c r="T8" s="32">
+      <c r="T8" s="30">
         <f>Main!V10</f>
         <v>0</v>
       </c>
-      <c r="U8" s="32">
+      <c r="U8" s="30">
         <f>Main!W10</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="28">
         <f>Main!C11</f>
         <v>41805</v>
       </c>
-      <c r="B9" s="31" t="str">
+      <c r="B9" s="29" t="str">
         <f>Main!D11</f>
         <v>Ivory Cost</v>
       </c>
-      <c r="C9" s="31" t="str">
+      <c r="C9" s="29" t="str">
         <f>Main!E11</f>
         <v>Japan</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="30">
         <f>Main!F11</f>
         <v>47</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="30">
         <f>Main!G11</f>
         <v>25</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="30">
         <f>Main!H11</f>
         <v>27</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="31">
         <f>Main!I11</f>
         <v>2.5</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="31">
         <f>Main!J11</f>
         <v>3</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="31">
         <f>Main!K11</f>
         <v>3</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="31">
         <f>Main!L11</f>
         <v>78.900000000000006</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K9" s="31">
         <f>Main!M11</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="31">
         <f>Main!N11</f>
         <v>1</v>
       </c>
-      <c r="M9" s="33">
+      <c r="M9" s="31">
         <f>Main!O11</f>
         <v>73.5</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="31">
         <f>Main!P11</f>
         <v>2.1</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="31">
         <f>Main!Q11</f>
         <v>1.3</v>
       </c>
-      <c r="P9" s="32">
+      <c r="P9" s="30">
         <f>Main!R11</f>
         <v>1</v>
       </c>
-      <c r="Q9" s="32">
+      <c r="Q9" s="30">
         <f>Main!S11</f>
         <v>1</v>
       </c>
-      <c r="R9" s="32">
+      <c r="R9" s="30">
         <f>Main!T11</f>
         <v>0</v>
       </c>
-      <c r="S9" s="32">
+      <c r="S9" s="30">
         <f>Main!U11</f>
         <v>1</v>
       </c>
-      <c r="T9" s="32">
+      <c r="T9" s="30">
         <f>Main!V11</f>
         <v>1</v>
       </c>
-      <c r="U9" s="32">
+      <c r="U9" s="30">
         <f>Main!W11</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
+      <c r="A10" s="28">
         <f>Main!C12</f>
         <v>41805</v>
       </c>
-      <c r="B10" s="31" t="str">
+      <c r="B10" s="29" t="str">
         <f>Main!D12</f>
         <v>Switzerland</v>
       </c>
-      <c r="C10" s="31" t="str">
+      <c r="C10" s="29" t="str">
         <f>Main!E12</f>
         <v>Ecuador</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="30">
         <f>Main!F12</f>
         <v>31</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="30">
         <f>Main!G12</f>
         <v>40</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="30">
         <f>Main!H12</f>
         <v>29</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="31">
         <f>Main!I12</f>
         <v>2.5</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="31">
         <f>Main!J12</f>
         <v>3.1</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="31">
         <f>Main!K12</f>
         <v>3.2</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="31">
         <f>Main!L12</f>
         <v>78</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="31">
         <f>Main!M12</f>
         <v>2</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="31">
         <f>Main!N12</f>
         <v>0.9</v>
       </c>
-      <c r="M10" s="33">
+      <c r="M10" s="31">
         <f>Main!O12</f>
         <v>80.7</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="31">
         <f>Main!P12</f>
         <v>2</v>
       </c>
-      <c r="O10" s="33">
+      <c r="O10" s="31">
         <f>Main!Q12</f>
         <v>0.8</v>
       </c>
-      <c r="P10" s="32">
+      <c r="P10" s="30">
         <f>Main!R12</f>
         <v>1</v>
       </c>
-      <c r="Q10" s="32">
+      <c r="Q10" s="30">
         <f>Main!S12</f>
         <v>1</v>
       </c>
-      <c r="R10" s="32">
+      <c r="R10" s="30">
         <f>Main!T12</f>
         <v>0</v>
       </c>
-      <c r="S10" s="32">
+      <c r="S10" s="30">
         <f>Main!U12</f>
         <v>1</v>
       </c>
-      <c r="T10" s="32">
+      <c r="T10" s="30">
         <f>Main!V12</f>
         <v>1</v>
       </c>
-      <c r="U10" s="32">
+      <c r="U10" s="30">
         <f>Main!W12</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="30">
+      <c r="A11" s="28">
         <f>Main!C13</f>
         <v>41805</v>
       </c>
-      <c r="B11" s="31" t="str">
+      <c r="B11" s="29" t="str">
         <f>Main!D13</f>
         <v>France</v>
       </c>
-      <c r="C11" s="31" t="str">
+      <c r="C11" s="29" t="str">
         <f>Main!E13</f>
         <v>Honduras</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="30">
         <f>Main!F13</f>
         <v>67</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="30">
         <f>Main!G13</f>
         <v>12</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="30">
         <f>Main!H13</f>
         <v>21</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="31">
         <f>Main!I13</f>
         <v>1.36</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="31">
         <f>Main!J13</f>
         <v>4.8</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="31">
         <f>Main!K13</f>
         <v>13</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="31">
         <f>Main!L13</f>
         <v>86.1</v>
       </c>
-      <c r="K11" s="33">
+      <c r="K11" s="31">
         <f>Main!M13</f>
         <v>2.5</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="31">
         <f>Main!N13</f>
         <v>0.6</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="31">
         <f>Main!O13</f>
         <v>69.599999999999994</v>
       </c>
-      <c r="N11" s="33">
+      <c r="N11" s="31">
         <f>Main!P13</f>
         <v>1.6</v>
       </c>
-      <c r="O11" s="33">
+      <c r="O11" s="31">
         <f>Main!Q13</f>
         <v>1.2</v>
       </c>
-      <c r="P11" s="32">
+      <c r="P11" s="30">
         <f>Main!R13</f>
         <v>1</v>
       </c>
-      <c r="Q11" s="32">
+      <c r="Q11" s="30">
         <f>Main!S13</f>
         <v>0</v>
       </c>
-      <c r="R11" s="32">
+      <c r="R11" s="30">
         <f>Main!T13</f>
         <v>1</v>
       </c>
-      <c r="S11" s="32">
+      <c r="S11" s="30">
         <f>Main!U13</f>
         <v>1</v>
       </c>
-      <c r="T11" s="32">
+      <c r="T11" s="30">
         <f>Main!V13</f>
         <v>0</v>
       </c>
-      <c r="U11" s="32">
+      <c r="U11" s="30">
         <f>Main!W13</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="28">
         <f>Main!C14</f>
         <v>41805</v>
       </c>
-      <c r="B12" s="31" t="str">
+      <c r="B12" s="29" t="str">
         <f>Main!D14</f>
         <v>Argentina</v>
       </c>
-      <c r="C12" s="31" t="str">
+      <c r="C12" s="29" t="str">
         <f>Main!E14</f>
         <v>Bosnia-Herzegovina</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="30">
         <f>Main!F14</f>
         <v>62</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="30">
         <f>Main!G14</f>
         <v>15</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="30">
         <f>Main!H14</f>
         <v>22</v>
       </c>
-      <c r="G12" s="33">
+      <c r="G12" s="31">
         <f>Main!I14</f>
         <v>1.44</v>
       </c>
-      <c r="H12" s="33">
+      <c r="H12" s="31">
         <f>Main!J14</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="31">
         <f>Main!K14</f>
         <v>8.5</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="31">
         <f>Main!L14</f>
         <v>90</v>
       </c>
-      <c r="K12" s="33">
+      <c r="K12" s="31">
         <f>Main!M14</f>
         <v>2.9</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="31">
         <f>Main!N14</f>
         <v>0.4</v>
       </c>
-      <c r="M12" s="33">
+      <c r="M12" s="31">
         <f>Main!O14</f>
         <v>80.3</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="31">
         <f>Main!P14</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="O12" s="33">
+      <c r="O12" s="31">
         <f>Main!Q14</f>
         <v>1</v>
       </c>
-      <c r="P12" s="32">
+      <c r="P12" s="30">
         <f>Main!R14</f>
         <v>2</v>
       </c>
-      <c r="Q12" s="32">
+      <c r="Q12" s="30">
         <f>Main!S14</f>
         <v>0</v>
       </c>
-      <c r="R12" s="32">
+      <c r="R12" s="30">
         <f>Main!T14</f>
         <v>2</v>
       </c>
-      <c r="S12" s="32">
+      <c r="S12" s="30">
         <f>Main!U14</f>
         <v>2</v>
       </c>
-      <c r="T12" s="32">
+      <c r="T12" s="30">
         <f>Main!V14</f>
         <v>0</v>
       </c>
-      <c r="U12" s="32">
+      <c r="U12" s="30">
         <f>Main!W14</f>
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="28">
         <f>Main!C15</f>
         <v>41806</v>
       </c>
-      <c r="B13" s="31" t="str">
+      <c r="B13" s="29" t="str">
         <f>Main!D15</f>
         <v>Germany</v>
       </c>
-      <c r="C13" s="31" t="str">
+      <c r="C13" s="29" t="str">
         <f>Main!E15</f>
         <v>Portugal</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="30">
         <f>Main!F15</f>
         <v>60</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="30">
         <f>Main!G15</f>
         <v>17</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="30">
         <f>Main!H15</f>
         <v>23</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="31">
         <f>Main!I15</f>
         <v>2.15</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="31">
         <f>Main!J15</f>
         <v>3.3</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="31">
         <f>Main!K15</f>
         <v>3.75</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="31">
         <f>Main!L15</f>
         <v>88.9</v>
       </c>
-      <c r="K13" s="33">
+      <c r="K13" s="31">
         <f>Main!M15</f>
         <v>3.2</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13" s="31">
         <f>Main!N15</f>
         <v>0.8</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="31">
         <f>Main!O15</f>
         <v>81</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="31">
         <f>Main!P15</f>
         <v>2.1</v>
       </c>
-      <c r="O13" s="33">
+      <c r="O13" s="31">
         <f>Main!Q15</f>
         <v>0.8</v>
       </c>
-      <c r="P13" s="32">
+      <c r="P13" s="30">
         <f>Main!R15</f>
         <v>1</v>
       </c>
-      <c r="Q13" s="32">
+      <c r="Q13" s="30">
         <f>Main!S15</f>
         <v>0</v>
       </c>
-      <c r="R13" s="32">
+      <c r="R13" s="30">
         <f>Main!T15</f>
         <v>1</v>
       </c>
-      <c r="S13" s="32">
+      <c r="S13" s="30">
         <f>Main!U15</f>
         <v>1</v>
       </c>
-      <c r="T13" s="32">
+      <c r="T13" s="30">
         <f>Main!V15</f>
         <v>0</v>
       </c>
-      <c r="U13" s="32">
+      <c r="U13" s="30">
         <f>Main!W15</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="28">
         <f>Main!C16</f>
         <v>41806</v>
       </c>
-      <c r="B14" s="31" t="str">
+      <c r="B14" s="29" t="str">
         <f>Main!D16</f>
         <v>Iran</v>
       </c>
-      <c r="C14" s="31" t="str">
+      <c r="C14" s="29" t="str">
         <f>Main!E16</f>
         <v>Nigeria</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="30">
         <f>Main!F16</f>
         <v>27</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="30">
         <f>Main!G16</f>
         <v>42</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="30">
         <f>Main!H16</f>
         <v>31</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="31">
         <f>Main!I16</f>
         <v>3.6</v>
       </c>
-      <c r="H14" s="33">
+      <c r="H14" s="31">
         <f>Main!J16</f>
         <v>3.1</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="31">
         <f>Main!K16</f>
         <v>2.25</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="31">
         <f>Main!L16</f>
         <v>70.599999999999994</v>
       </c>
-      <c r="K14" s="33">
+      <c r="K14" s="31">
         <f>Main!M16</f>
         <v>1.3</v>
       </c>
-      <c r="L14" s="33">
+      <c r="L14" s="31">
         <f>Main!N16</f>
         <v>0.9</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M14" s="31">
         <f>Main!O16</f>
         <v>75.2</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="31">
         <f>Main!P16</f>
         <v>1.7</v>
       </c>
-      <c r="O14" s="33">
+      <c r="O14" s="31">
         <f>Main!Q16</f>
         <v>0.9</v>
       </c>
-      <c r="P14" s="32">
+      <c r="P14" s="30">
         <f>Main!R16</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="32">
+      <c r="Q14" s="30">
         <f>Main!S16</f>
         <v>0</v>
       </c>
-      <c r="R14" s="32">
+      <c r="R14" s="30">
         <f>Main!T16</f>
         <v>0</v>
       </c>
-      <c r="S14" s="32">
+      <c r="S14" s="30">
         <f>Main!U16</f>
         <v>0</v>
       </c>
-      <c r="T14" s="32">
+      <c r="T14" s="30">
         <f>Main!V16</f>
         <v>0</v>
       </c>
-      <c r="U14" s="32">
+      <c r="U14" s="30">
         <f>Main!W16</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="A15" s="28">
         <f>Main!C17</f>
         <v>41806</v>
       </c>
-      <c r="B15" s="31" t="str">
+      <c r="B15" s="29" t="str">
         <f>Main!D17</f>
         <v>Ghana</v>
       </c>
-      <c r="C15" s="31" t="str">
+      <c r="C15" s="29" t="str">
         <f>Main!E17</f>
         <v>USA</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="30">
         <f>Main!F17</f>
         <v>35</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="30">
         <f>Main!G17</f>
         <v>36</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="30">
         <f>Main!H17</f>
         <v>29</v>
       </c>
-      <c r="G15" s="33">
+      <c r="G15" s="31">
         <f>Main!I17</f>
         <v>2.6</v>
       </c>
-      <c r="H15" s="33">
+      <c r="H15" s="31">
         <f>Main!J17</f>
         <v>3.1</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="31">
         <f>Main!K17</f>
         <v>3.1</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="31">
         <f>Main!L17</f>
         <v>77.2</v>
       </c>
-      <c r="K15" s="33">
+      <c r="K15" s="31">
         <f>Main!M17</f>
         <v>1.9</v>
       </c>
-      <c r="L15" s="33">
+      <c r="L15" s="31">
         <f>Main!N17</f>
         <v>0.9</v>
       </c>
-      <c r="M15" s="33">
+      <c r="M15" s="31">
         <f>Main!O17</f>
         <v>77.400000000000006</v>
       </c>
-      <c r="N15" s="33">
+      <c r="N15" s="31">
         <f>Main!P17</f>
         <v>2</v>
       </c>
-      <c r="O15" s="33">
+      <c r="O15" s="31">
         <f>Main!Q17</f>
         <v>1</v>
       </c>
-      <c r="P15" s="32">
+      <c r="P15" s="30">
         <f>Main!R17</f>
         <v>1</v>
       </c>
-      <c r="Q15" s="32">
+      <c r="Q15" s="30">
         <f>Main!S17</f>
         <v>1</v>
       </c>
-      <c r="R15" s="32">
+      <c r="R15" s="30">
         <f>Main!T17</f>
         <v>0</v>
       </c>
-      <c r="S15" s="32">
+      <c r="S15" s="30">
         <f>Main!U17</f>
         <v>1</v>
       </c>
-      <c r="T15" s="32">
+      <c r="T15" s="30">
         <f>Main!V17</f>
         <v>1</v>
       </c>
-      <c r="U15" s="32">
+      <c r="U15" s="30">
         <f>Main!W17</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="28">
         <f>Main!C18</f>
         <v>41807</v>
       </c>
-      <c r="B16" s="31" t="str">
+      <c r="B16" s="29" t="str">
         <f>Main!D18</f>
         <v>Belgium</v>
       </c>
-      <c r="C16" s="31" t="str">
+      <c r="C16" s="29" t="str">
         <f>Main!E18</f>
         <v>Algeria</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="30">
         <f>Main!F18</f>
         <v>64</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="30">
         <f>Main!G18</f>
         <v>12</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="30">
         <f>Main!H18</f>
         <v>23</v>
       </c>
-      <c r="G16" s="33">
+      <c r="G16" s="31">
         <f>Main!I18</f>
         <v>1.5</v>
       </c>
-      <c r="H16" s="33">
+      <c r="H16" s="31">
         <f>Main!J18</f>
         <v>4.3</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="31">
         <f>Main!K18</f>
         <v>8</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J16" s="31">
         <f>Main!L18</f>
         <v>82</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K16" s="31">
         <f>Main!M18</f>
         <v>2.1</v>
       </c>
-      <c r="L16" s="33">
+      <c r="L16" s="31">
         <f>Main!N18</f>
         <v>0.7</v>
       </c>
-      <c r="M16" s="33">
+      <c r="M16" s="31">
         <f>Main!O18</f>
         <v>63.4</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N16" s="31">
         <f>Main!P18</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O16" s="33">
+      <c r="O16" s="31">
         <f>Main!Q18</f>
         <v>1.2</v>
       </c>
-      <c r="P16" s="32">
+      <c r="P16" s="30">
         <f>Main!R18</f>
         <v>1</v>
       </c>
-      <c r="Q16" s="32">
+      <c r="Q16" s="30">
         <f>Main!S18</f>
         <v>0</v>
       </c>
-      <c r="R16" s="32">
+      <c r="R16" s="30">
         <f>Main!T18</f>
         <v>1</v>
       </c>
-      <c r="S16" s="32">
+      <c r="S16" s="30">
         <f>Main!U18</f>
         <v>1</v>
       </c>
-      <c r="T16" s="32">
+      <c r="T16" s="30">
         <f>Main!V18</f>
         <v>0</v>
       </c>
-      <c r="U16" s="32">
+      <c r="U16" s="30">
         <f>Main!W18</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
+      <c r="A17" s="28">
         <f>Main!C19</f>
         <v>41807</v>
       </c>
-      <c r="B17" s="31" t="str">
+      <c r="B17" s="29" t="str">
         <f>Main!D19</f>
         <v>Russia</v>
       </c>
-      <c r="C17" s="31" t="str">
+      <c r="C17" s="29" t="str">
         <f>Main!E19</f>
         <v>S Korea</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="30">
         <f>Main!F19</f>
         <v>46</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="30">
         <f>Main!G19</f>
         <v>25</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="30">
         <f>Main!H19</f>
         <v>29</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="31">
         <f>Main!I19</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H17" s="31">
         <f>Main!J19</f>
         <v>3.1</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="31">
         <f>Main!K19</f>
         <v>3.6</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="31">
         <f>Main!L19</f>
         <v>79</v>
       </c>
-      <c r="K17" s="33">
+      <c r="K17" s="31">
         <f>Main!M19</f>
         <v>1.7</v>
       </c>
-      <c r="L17" s="33">
+      <c r="L17" s="31">
         <f>Main!N19</f>
         <v>0.6</v>
       </c>
-      <c r="M17" s="33">
+      <c r="M17" s="31">
         <f>Main!O19</f>
         <v>72.400000000000006</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N17" s="31">
         <f>Main!P19</f>
         <v>1.7</v>
       </c>
-      <c r="O17" s="33">
+      <c r="O17" s="31">
         <f>Main!Q19</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="P17" s="32">
+      <c r="P17" s="30">
         <f>Main!R19</f>
         <v>1</v>
       </c>
-      <c r="Q17" s="32">
+      <c r="Q17" s="30">
         <f>Main!S19</f>
         <v>0</v>
       </c>
-      <c r="R17" s="32">
+      <c r="R17" s="30">
         <f>Main!T19</f>
         <v>1</v>
       </c>
-      <c r="S17" s="32">
+      <c r="S17" s="30">
         <f>Main!U19</f>
         <v>1</v>
       </c>
-      <c r="T17" s="32">
+      <c r="T17" s="30">
         <f>Main!V19</f>
         <v>0</v>
       </c>
-      <c r="U17" s="32">
+      <c r="U17" s="30">
         <f>Main!W19</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="28">
         <f>Main!C20</f>
         <v>41808</v>
       </c>
-      <c r="B18" s="31" t="str">
+      <c r="B18" s="29" t="str">
         <f>Main!D20</f>
         <v>Australia</v>
       </c>
-      <c r="C18" s="31" t="str">
+      <c r="C18" s="29" t="str">
         <f>Main!E20</f>
         <v>Netherlands</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="30">
         <f>Main!F20</f>
         <v>15</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="30">
         <f>Main!G20</f>
         <v>61</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="30">
         <f>Main!H20</f>
         <v>24</v>
       </c>
-      <c r="G18" s="33">
+      <c r="G18" s="31">
         <f>Main!I20</f>
         <v>10</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="31">
         <f>Main!J20</f>
         <v>5</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="31">
         <f>Main!K20</f>
         <v>1.3</v>
       </c>
-      <c r="J18" s="33">
+      <c r="J18" s="31">
         <f>Main!L20</f>
         <v>69.5</v>
       </c>
-      <c r="K18" s="33">
+      <c r="K18" s="31">
         <f>Main!M20</f>
         <v>1.6</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="31">
         <f>Main!N20</f>
         <v>1.2</v>
       </c>
-      <c r="M18" s="33">
+      <c r="M18" s="31">
         <f>Main!O20</f>
         <v>82.5</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="31">
         <f>Main!P20</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="O18" s="33">
+      <c r="O18" s="31">
         <f>Main!Q20</f>
         <v>0.8</v>
       </c>
-      <c r="P18" s="32">
+      <c r="P18" s="30">
         <f>Main!R20</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="32">
+      <c r="Q18" s="30">
         <f>Main!S20</f>
         <v>2</v>
       </c>
-      <c r="R18" s="32">
+      <c r="R18" s="30">
         <f>Main!T20</f>
         <v>-2</v>
       </c>
-      <c r="S18" s="32">
+      <c r="S18" s="30">
         <f>Main!U20</f>
         <v>0</v>
       </c>
-      <c r="T18" s="32">
+      <c r="T18" s="30">
         <f>Main!V20</f>
         <v>2</v>
       </c>
-      <c r="U18" s="32">
+      <c r="U18" s="30">
         <f>Main!W20</f>
         <v>-2</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="A19" s="28">
         <f>Main!C21</f>
         <v>41808</v>
       </c>
-      <c r="B19" s="31" t="str">
+      <c r="B19" s="29" t="str">
         <f>Main!D21</f>
         <v>Spain</v>
       </c>
-      <c r="C19" s="31" t="str">
+      <c r="C19" s="29" t="str">
         <f>Main!E21</f>
         <v>Chile</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="30">
         <f>Main!F21</f>
         <v>42</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="30">
         <f>Main!G21</f>
         <v>31</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="30">
         <f>Main!H21</f>
         <v>27</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="31">
         <f>Main!I21</f>
         <v>1.72</v>
       </c>
-      <c r="H19" s="33">
+      <c r="H19" s="31">
         <f>Main!J21</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="31">
         <f>Main!K21</f>
         <v>5</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="31">
         <f>Main!L21</f>
         <v>89.1</v>
       </c>
-      <c r="K19" s="33">
+      <c r="K19" s="31">
         <f>Main!M21</f>
         <v>2.7</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="31">
         <f>Main!N21</f>
         <v>0.4</v>
       </c>
-      <c r="M19" s="33">
+      <c r="M19" s="31">
         <f>Main!O21</f>
         <v>86.7</v>
       </c>
-      <c r="N19" s="33">
+      <c r="N19" s="31">
         <f>Main!P21</f>
         <v>2.7</v>
       </c>
-      <c r="O19" s="33">
+      <c r="O19" s="31">
         <f>Main!Q21</f>
         <v>0.7</v>
       </c>
-      <c r="P19" s="32">
+      <c r="P19" s="30">
         <f>Main!R21</f>
         <v>1</v>
       </c>
-      <c r="Q19" s="32">
+      <c r="Q19" s="30">
         <f>Main!S21</f>
         <v>0</v>
       </c>
-      <c r="R19" s="32">
+      <c r="R19" s="30">
         <f>Main!T21</f>
         <v>1</v>
       </c>
-      <c r="S19" s="32">
+      <c r="S19" s="30">
         <f>Main!U21</f>
         <v>1</v>
       </c>
-      <c r="T19" s="32">
+      <c r="T19" s="30">
         <f>Main!V21</f>
         <v>0</v>
       </c>
-      <c r="U19" s="32">
+      <c r="U19" s="30">
         <f>Main!W21</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Predictions for 23-26/6 (leaving UK for a week)
</commit_message>
<xml_diff>
--- a/data/data_wc2014.xlsx
+++ b/data/data_wc2014.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="96">
   <si>
     <t>Team</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>predict</t>
-  </si>
-  <si>
-    <t>future</t>
   </si>
   <si>
     <t>Bosnia</t>
@@ -1550,6 +1547,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1557,15 +1563,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2000,7 +1997,7 @@
       <c r="E2" s="191"/>
       <c r="F2" s="192"/>
       <c r="G2" s="193" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="194"/>
       <c r="I2" s="194"/>
@@ -3043,16 +3040,16 @@
         <v>4</v>
       </c>
       <c r="I3" s="142" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="138" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="122" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="138" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3" s="122" t="s">
+      <c r="L3" s="123" t="s">
         <v>66</v>
-      </c>
-      <c r="L3" s="123" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:1024">
@@ -3792,7 +3789,7 @@
     </row>
     <row r="25" spans="2:12">
       <c r="B25" s="110" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>8</v>
@@ -4177,17 +4174,17 @@
     </row>
     <row r="37" spans="2:12">
       <c r="B37" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="2:12">
       <c r="B38" s="162" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="2:12">
       <c r="B39" s="163" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -4211,10 +4208,10 @@
   <dimension ref="A1:AMP51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="O28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="T28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V35" sqref="V35"/>
+      <selection pane="bottomRight" activeCell="AQ51" sqref="AQ51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4366,57 +4363,57 @@
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2" s="196">
+      <c r="F2" s="199">
         <v>538</v>
       </c>
-      <c r="G2" s="197"/>
-      <c r="H2" s="198"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="201"/>
       <c r="I2" s="193" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J2" s="194"/>
       <c r="K2" s="195"/>
-      <c r="L2" s="196">
+      <c r="L2" s="199">
         <v>538</v>
       </c>
-      <c r="M2" s="197"/>
-      <c r="N2" s="197"/>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="198"/>
-      <c r="R2" s="196" t="s">
-        <v>70</v>
-      </c>
-      <c r="S2" s="197"/>
-      <c r="T2" s="197"/>
-      <c r="U2" s="196" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" s="197"/>
-      <c r="W2" s="197"/>
-      <c r="X2" s="196" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y2" s="197"/>
-      <c r="Z2" s="197"/>
-      <c r="AA2" s="197"/>
-      <c r="AB2" s="197"/>
-      <c r="AC2" s="198"/>
-      <c r="AD2" s="196" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE2" s="197"/>
-      <c r="AF2" s="198"/>
-      <c r="AG2" s="199" t="s">
+      <c r="M2" s="200"/>
+      <c r="N2" s="200"/>
+      <c r="O2" s="200"/>
+      <c r="P2" s="200"/>
+      <c r="Q2" s="201"/>
+      <c r="R2" s="199" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="200"/>
+      <c r="T2" s="200"/>
+      <c r="U2" s="199" t="s">
+        <v>69</v>
+      </c>
+      <c r="V2" s="200"/>
+      <c r="W2" s="200"/>
+      <c r="X2" s="199" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y2" s="200"/>
+      <c r="Z2" s="200"/>
+      <c r="AA2" s="200"/>
+      <c r="AB2" s="200"/>
+      <c r="AC2" s="201"/>
+      <c r="AD2" s="199" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="200"/>
+      <c r="AF2" s="201"/>
+      <c r="AG2" s="196" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH2" s="197"/>
+      <c r="AI2" s="198"/>
+      <c r="AJ2" s="196" t="s">
         <v>85</v>
       </c>
-      <c r="AH2" s="200"/>
-      <c r="AI2" s="201"/>
-      <c r="AJ2" s="199" t="s">
-        <v>86</v>
-      </c>
-      <c r="AK2" s="200"/>
-      <c r="AL2" s="201"/>
+      <c r="AK2" s="197"/>
+      <c r="AL2" s="198"/>
       <c r="AM2"/>
       <c r="AO2" s="2">
         <f>MIN(AO4:AO510)</f>
@@ -4442,22 +4439,22 @@
         <v>47</v>
       </c>
       <c r="F3" s="85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G3" s="86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H3" s="87" t="s">
         <v>48</v>
       </c>
       <c r="I3" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="89" t="s">
-        <v>91</v>
-      </c>
       <c r="K3" s="90" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L3" s="88" t="s">
         <v>49</v>
@@ -4478,49 +4475,49 @@
         <v>54</v>
       </c>
       <c r="R3" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="S3" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="S3" s="86" t="s">
+      <c r="T3" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="T3" s="86" t="s">
+      <c r="U3" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="V3" s="86" t="s">
+        <v>92</v>
+      </c>
+      <c r="W3" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="X3" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="U3" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="V3" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="W3" s="86" t="s">
+      <c r="Y3" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z3" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA3" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB3" s="97" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC3" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD3" s="91" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE3" s="92" t="s">
         <v>94</v>
       </c>
-      <c r="X3" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y3" s="97" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z3" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA3" s="85" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB3" s="97" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC3" s="87" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD3" s="91" t="s">
+      <c r="AF3" s="93" t="s">
         <v>87</v>
-      </c>
-      <c r="AE3" s="92" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF3" s="93" t="s">
-        <v>88</v>
       </c>
       <c r="AG3" s="146" t="s">
         <v>55</v>
@@ -4529,7 +4526,7 @@
         <v>56</v>
       </c>
       <c r="AI3" s="148" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AJ3" s="104" t="s">
         <v>57</v>
@@ -5986,7 +5983,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" s="22">
         <v>62</v>
@@ -8560,7 +8557,7 @@
         <v>35</v>
       </c>
       <c r="E32" s="57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F32" s="24">
         <v>26</v>
@@ -8696,102 +8693,102 @@
       <c r="B33" s="43">
         <v>30</v>
       </c>
-      <c r="C33" s="48">
+      <c r="C33" s="47">
         <v>41812</v>
       </c>
-      <c r="D33" s="53" t="s">
+      <c r="D33" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="58" t="s">
+      <c r="E33" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="26">
+      <c r="F33" s="24">
         <v>43</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="12">
         <v>28</v>
       </c>
-      <c r="H33" s="27">
+      <c r="H33" s="25">
         <v>29</v>
       </c>
-      <c r="I33" s="37">
+      <c r="I33" s="35">
         <v>52.2</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33" s="13">
         <v>31.3</v>
       </c>
-      <c r="K33" s="38">
+      <c r="K33" s="36">
         <v>16.5</v>
       </c>
-      <c r="L33" s="37">
+      <c r="L33" s="35">
         <f>VLOOKUP($D33,'538'!$B$4:$F$35,3,0)</f>
         <v>82</v>
       </c>
-      <c r="M33" s="9">
+      <c r="M33" s="13">
         <f>VLOOKUP($D33,'538'!$B$4:$F$35,4,0)</f>
         <v>2.1</v>
       </c>
-      <c r="N33" s="38">
+      <c r="N33" s="36">
         <f>VLOOKUP($D33,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="O33" s="19">
+      <c r="O33" s="18">
         <f>VLOOKUP($E33,'538'!$B$4:$F$35,3,0)</f>
         <v>79</v>
       </c>
-      <c r="P33" s="9">
+      <c r="P33" s="13">
         <f>VLOOKUP($E33,'538'!$B$4:$F$35,4,0)</f>
         <v>1.7</v>
       </c>
-      <c r="Q33" s="64">
+      <c r="Q33" s="63">
         <f>VLOOKUP($E33,'538'!$B$4:$F$35,5,0)</f>
         <v>0.6</v>
       </c>
-      <c r="R33" s="26">
+      <c r="R33" s="24">
         <f>VLOOKUP($D33,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.6</v>
       </c>
-      <c r="S33" s="8">
+      <c r="S33" s="12">
         <f>VLOOKUP($D33,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="T33" s="8">
+      <c r="T33" s="12">
         <f>VLOOKUP($D33,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.3</v>
       </c>
-      <c r="U33" s="26">
+      <c r="U33" s="24">
         <f>VLOOKUP($E33,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>2.1</v>
       </c>
-      <c r="V33" s="8">
+      <c r="V33" s="12">
         <f>VLOOKUP($E33,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>3.1</v>
       </c>
-      <c r="W33" s="8">
+      <c r="W33" s="12">
         <f>VLOOKUP($E33,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>2.6</v>
       </c>
-      <c r="X33" s="26">
+      <c r="X33" s="24">
         <f>VLOOKUP($D33,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="Y33" s="102">
+      <c r="Y33" s="101">
         <f>VLOOKUP($D33,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="Z33" s="27">
+      <c r="Z33" s="25">
         <f>VLOOKUP($D33,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="AA33" s="26">
+      <c r="AA33" s="24">
         <f>VLOOKUP($E33,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="AB33" s="102">
+      <c r="AB33" s="101">
         <f>VLOOKUP($E33,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="AC33" s="27">
+      <c r="AC33" s="25">
         <f>VLOOKUP($E33,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>4</v>
       </c>
@@ -8824,7 +8821,7 @@
         <v>0.71</v>
       </c>
       <c r="AM33" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO33" s="2">
         <f t="shared" si="0"/>
@@ -8839,102 +8836,102 @@
       <c r="B34" s="43">
         <v>31</v>
       </c>
-      <c r="C34" s="48">
+      <c r="C34" s="47">
         <v>41812</v>
       </c>
-      <c r="D34" s="53" t="s">
+      <c r="D34" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="58" t="s">
+      <c r="E34" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="26">
+      <c r="F34" s="24">
         <v>45</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="12">
         <v>25</v>
       </c>
-      <c r="H34" s="27">
+      <c r="H34" s="25">
         <v>30</v>
       </c>
-      <c r="I34" s="37">
+      <c r="I34" s="35">
         <v>41.6</v>
       </c>
-      <c r="J34" s="9">
+      <c r="J34" s="13">
         <v>29</v>
       </c>
-      <c r="K34" s="38">
+      <c r="K34" s="36">
         <v>29.4</v>
       </c>
-      <c r="L34" s="37">
+      <c r="L34" s="35">
         <f>VLOOKUP($D34,'538'!$B$4:$F$35,3,0)</f>
         <v>72.400000000000006</v>
       </c>
-      <c r="M34" s="9">
+      <c r="M34" s="13">
         <f>VLOOKUP($D34,'538'!$B$4:$F$35,4,0)</f>
         <v>1.7</v>
       </c>
-      <c r="N34" s="38">
+      <c r="N34" s="36">
         <f>VLOOKUP($D34,'538'!$B$4:$F$35,5,0)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O34" s="19">
+      <c r="O34" s="18">
         <f>VLOOKUP($E34,'538'!$B$4:$F$35,3,0)</f>
         <v>63.4</v>
       </c>
-      <c r="P34" s="9">
+      <c r="P34" s="13">
         <f>VLOOKUP($E34,'538'!$B$4:$F$35,4,0)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q34" s="64">
+      <c r="Q34" s="63">
         <f>VLOOKUP($E34,'538'!$B$4:$F$35,5,0)</f>
         <v>1.2</v>
       </c>
-      <c r="R34" s="26">
+      <c r="R34" s="24">
         <f>VLOOKUP($D34,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>1.9</v>
       </c>
-      <c r="S34" s="8">
+      <c r="S34" s="12">
         <f>VLOOKUP($D34,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>1.4</v>
       </c>
-      <c r="T34" s="8">
+      <c r="T34" s="12">
         <f>VLOOKUP($D34,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>1.5</v>
       </c>
-      <c r="U34" s="26">
+      <c r="U34" s="24">
         <f>VLOOKUP($E34,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>1.4</v>
       </c>
-      <c r="V34" s="8">
+      <c r="V34" s="12">
         <f>VLOOKUP($E34,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>1.3</v>
       </c>
-      <c r="W34" s="8">
+      <c r="W34" s="12">
         <f>VLOOKUP($E34,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>1.3</v>
       </c>
-      <c r="X34" s="26">
+      <c r="X34" s="24">
         <f>VLOOKUP($D34,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>57</v>
       </c>
-      <c r="Y34" s="102">
+      <c r="Y34" s="101">
         <f>VLOOKUP($D34,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="Z34" s="27">
+      <c r="Z34" s="25">
         <f>VLOOKUP($D34,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="AA34" s="26">
+      <c r="AA34" s="24">
         <f>VLOOKUP($E34,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>22</v>
       </c>
-      <c r="AB34" s="102">
+      <c r="AB34" s="101">
         <f>VLOOKUP($E34,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="AC34" s="27">
+      <c r="AC34" s="25">
         <f>VLOOKUP($E34,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>32</v>
       </c>
@@ -8948,14 +8945,14 @@
         <v>3.1</v>
       </c>
       <c r="AG34" s="183">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH34" s="184">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AI34" s="151">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="AJ34" s="156">
         <v>1.2</v>
@@ -8967,7 +8964,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="AM34" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO34" s="2">
         <f t="shared" si="0"/>
@@ -8982,102 +8979,102 @@
       <c r="B35" s="43">
         <v>32</v>
       </c>
-      <c r="C35" s="48">
+      <c r="C35" s="47">
         <v>41812</v>
       </c>
-      <c r="D35" s="53" t="s">
+      <c r="D35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="58" t="s">
+      <c r="E35" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="26">
+      <c r="F35" s="24">
         <v>29</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="12">
         <v>42</v>
       </c>
-      <c r="H35" s="27">
+      <c r="H35" s="25">
         <v>29</v>
       </c>
-      <c r="I35" s="37">
+      <c r="I35" s="35">
         <v>21.3</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="13">
         <v>24.3</v>
       </c>
-      <c r="K35" s="38">
+      <c r="K35" s="36">
         <v>54.4</v>
       </c>
-      <c r="L35" s="37">
+      <c r="L35" s="35">
         <f>VLOOKUP($D35,'538'!$B$4:$F$35,3,0)</f>
         <v>77.400000000000006</v>
       </c>
-      <c r="M35" s="9">
+      <c r="M35" s="13">
         <f>VLOOKUP($D35,'538'!$B$4:$F$35,4,0)</f>
         <v>2</v>
       </c>
-      <c r="N35" s="38">
+      <c r="N35" s="36">
         <f>VLOOKUP($D35,'538'!$B$4:$F$35,5,0)</f>
         <v>1</v>
       </c>
-      <c r="O35" s="19">
+      <c r="O35" s="18">
         <f>VLOOKUP($E35,'538'!$B$4:$F$35,3,0)</f>
         <v>81</v>
       </c>
-      <c r="P35" s="9">
+      <c r="P35" s="13">
         <f>VLOOKUP($E35,'538'!$B$4:$F$35,4,0)</f>
         <v>2.1</v>
       </c>
-      <c r="Q35" s="64">
+      <c r="Q35" s="63">
         <f>VLOOKUP($E35,'538'!$B$4:$F$35,5,0)</f>
         <v>0.8</v>
       </c>
-      <c r="R35" s="26">
+      <c r="R35" s="24">
         <f>VLOOKUP($D35,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.6</v>
       </c>
-      <c r="S35" s="8">
+      <c r="S35" s="12">
         <f>VLOOKUP($D35,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>1.7</v>
       </c>
-      <c r="T35" s="8">
+      <c r="T35" s="12">
         <f>VLOOKUP($D35,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>2.6</v>
       </c>
-      <c r="U35" s="26">
+      <c r="U35" s="24">
         <f>VLOOKUP($E35,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="V35" s="8">
+      <c r="V35" s="12">
         <f>VLOOKUP($E35,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="W35" s="8">
+      <c r="W35" s="12">
         <f>VLOOKUP($E35,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.2</v>
       </c>
-      <c r="X35" s="26">
+      <c r="X35" s="24">
         <f>VLOOKUP($D35,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>13</v>
       </c>
-      <c r="Y35" s="102">
+      <c r="Y35" s="101">
         <f>VLOOKUP($D35,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="Z35" s="27">
+      <c r="Z35" s="25">
         <f>VLOOKUP($D35,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="AA35" s="26">
+      <c r="AA35" s="24">
         <f>VLOOKUP($E35,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="AB35" s="102">
+      <c r="AB35" s="101">
         <f>VLOOKUP($E35,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="AC35" s="27">
+      <c r="AC35" s="25">
         <f>VLOOKUP($E35,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>3</v>
       </c>
@@ -9091,10 +9088,10 @@
         <v>1.7</v>
       </c>
       <c r="AG35" s="183">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH35" s="184">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI35" s="151">
         <f t="shared" si="2"/>
@@ -9110,7 +9107,7 @@
         <v>-0.04</v>
       </c>
       <c r="AM35" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO35" s="2">
         <f t="shared" si="0"/>
@@ -9225,13 +9222,13 @@
         <v>3</v>
       </c>
       <c r="AD36" s="173">
-        <v>2.2999999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="AE36" s="174">
         <v>3.4</v>
       </c>
       <c r="AF36" s="175">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="AG36" s="183">
         <v>1</v>
@@ -9250,11 +9247,11 @@
         <v>0</v>
       </c>
       <c r="AL36" s="158">
-        <f t="shared" ref="AL33:AL51" si="3">AJ36-AK36</f>
+        <f t="shared" ref="AL36:AL51" si="3">AJ36-AK36</f>
         <v>0</v>
       </c>
       <c r="AM36" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO36" s="2">
         <f t="shared" si="0"/>
@@ -9369,13 +9366,13 @@
         <v>1</v>
       </c>
       <c r="AD37" s="173">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AE37" s="174">
-        <v>6</v>
+        <v>4.75</v>
       </c>
       <c r="AF37" s="175">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="AG37" s="183">
         <v>0</v>
@@ -9398,7 +9395,7 @@
         <v>0</v>
       </c>
       <c r="AM37" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO37" s="2">
         <f t="shared" si="0"/>
@@ -9516,10 +9513,10 @@
         <v>23</v>
       </c>
       <c r="AE38" s="174">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="AF38" s="175">
-        <v>1.18</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="AG38" s="183">
         <v>0</v>
@@ -9542,7 +9539,7 @@
         <v>0</v>
       </c>
       <c r="AM38" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO38" s="2">
         <f t="shared" si="0"/>
@@ -9657,13 +9654,13 @@
         <v>8</v>
       </c>
       <c r="AD39" s="173">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="AE39" s="174">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="AF39" s="175">
-        <v>2.87</v>
+        <v>2.7</v>
       </c>
       <c r="AG39" s="183">
         <v>1</v>
@@ -9686,7 +9683,7 @@
         <v>0</v>
       </c>
       <c r="AM39" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO39" s="2">
         <f t="shared" si="0"/>
@@ -9801,13 +9798,13 @@
         <v>1</v>
       </c>
       <c r="AD40" s="173">
-        <v>7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AE40" s="174">
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="AF40" s="175">
-        <v>1.44</v>
+        <v>1.83</v>
       </c>
       <c r="AG40" s="183">
         <v>0</v>
@@ -9830,7 +9827,7 @@
         <v>0</v>
       </c>
       <c r="AM40" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO40" s="2">
         <f t="shared" si="0"/>
@@ -9945,13 +9942,13 @@
         <v>1</v>
       </c>
       <c r="AD41" s="173">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="AE41" s="174">
-        <v>3.25</v>
+        <v>3.1</v>
       </c>
       <c r="AF41" s="175">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="AG41" s="183">
         <v>1</v>
@@ -9974,7 +9971,7 @@
         <v>0</v>
       </c>
       <c r="AM41" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO41" s="2">
         <f t="shared" si="0"/>
@@ -10089,13 +10086,13 @@
         <v>16</v>
       </c>
       <c r="AD42" s="173">
-        <v>4.3</v>
+        <v>3</v>
       </c>
       <c r="AE42" s="174">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="AF42" s="175">
-        <v>1.8</v>
+        <v>2.37</v>
       </c>
       <c r="AG42" s="183">
         <v>1</v>
@@ -10118,7 +10115,7 @@
         <v>0</v>
       </c>
       <c r="AM42" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO42" s="2">
         <f t="shared" si="0"/>
@@ -10233,13 +10230,13 @@
         <v>32</v>
       </c>
       <c r="AD43" s="173">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="AE43" s="174">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="AF43" s="175">
-        <v>2.2999999999999998</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="AG43" s="183">
         <v>1</v>
@@ -10262,7 +10259,7 @@
         <v>0</v>
       </c>
       <c r="AM43" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO43" s="2">
         <f t="shared" si="0"/>
@@ -10377,13 +10374,13 @@
         <v>1</v>
       </c>
       <c r="AD44" s="173">
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="AE44" s="174">
-        <v>4.5</v>
+        <v>3.8</v>
       </c>
       <c r="AF44" s="175">
-        <v>1.36</v>
+        <v>1.55</v>
       </c>
       <c r="AG44" s="183">
         <v>0</v>
@@ -10406,7 +10403,7 @@
         <v>0</v>
       </c>
       <c r="AM44" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO44" s="2">
         <f t="shared" si="0"/>
@@ -10425,7 +10422,7 @@
         <v>41815</v>
       </c>
       <c r="D45" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E45" s="58" t="s">
         <v>40</v>
@@ -10521,13 +10518,13 @@
         <v>32</v>
       </c>
       <c r="AD45" s="173">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="AE45" s="174">
+        <v>3.1</v>
+      </c>
+      <c r="AF45" s="175">
         <v>3.6</v>
-      </c>
-      <c r="AF45" s="175">
-        <v>6</v>
       </c>
       <c r="AG45" s="183">
         <v>1</v>
@@ -10550,7 +10547,7 @@
         <v>0</v>
       </c>
       <c r="AM45" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO45" s="2">
         <f t="shared" si="0"/>
@@ -10665,13 +10662,13 @@
         <v>1</v>
       </c>
       <c r="AD46" s="173">
-        <v>3.75</v>
+        <v>4.5</v>
       </c>
       <c r="AE46" s="174">
         <v>3.5</v>
       </c>
       <c r="AF46" s="175">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="AG46" s="183">
         <v>0</v>
@@ -10694,7 +10691,7 @@
         <v>0</v>
       </c>
       <c r="AM46" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO46" s="2">
         <f t="shared" si="0"/>
@@ -10809,13 +10806,13 @@
         <v>8</v>
       </c>
       <c r="AD47" s="173">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="AE47" s="174">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="AF47" s="175">
-        <v>1.57</v>
+        <v>1.44</v>
       </c>
       <c r="AG47" s="183">
         <v>1</v>
@@ -10838,7 +10835,7 @@
         <v>0</v>
       </c>
       <c r="AM47" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO47" s="2">
         <f t="shared" si="0"/>
@@ -10953,13 +10950,13 @@
         <v>8</v>
       </c>
       <c r="AD48" s="173">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="AE48" s="174">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="AF48" s="175">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="AG48" s="183">
         <v>1</v>
@@ -10982,7 +10979,7 @@
         <v>0</v>
       </c>
       <c r="AM48" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO48" s="2">
         <f t="shared" si="0"/>
@@ -11097,13 +11094,13 @@
         <v>1</v>
       </c>
       <c r="AD49" s="173">
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="AE49" s="174">
-        <v>4.4000000000000004</v>
+        <v>2.5</v>
       </c>
       <c r="AF49" s="175">
-        <v>1.4</v>
+        <v>1.72</v>
       </c>
       <c r="AG49" s="183">
         <v>0</v>
@@ -11126,7 +11123,7 @@
         <v>0</v>
       </c>
       <c r="AM49" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO49" s="2">
         <f t="shared" si="0"/>
@@ -11241,13 +11238,13 @@
         <v>4</v>
       </c>
       <c r="AD50" s="173">
-        <v>6</v>
+        <v>3.8</v>
       </c>
       <c r="AE50" s="174">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="AF50" s="175">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="AG50" s="183">
         <v>0</v>
@@ -11270,7 +11267,7 @@
         <v>0</v>
       </c>
       <c r="AM50" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO50" s="2">
         <f t="shared" si="0"/>
@@ -11385,13 +11382,13 @@
         <v>4</v>
       </c>
       <c r="AD51" s="176">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="AE51" s="177">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="AF51" s="178">
-        <v>1.61</v>
+        <v>1.8</v>
       </c>
       <c r="AG51" s="185">
         <v>0</v>
@@ -11414,7 +11411,7 @@
         <v>0</v>
       </c>
       <c r="AM51" s="68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO51" s="2">
         <f t="shared" si="0"/>
@@ -16110,7 +16107,7 @@
       </c>
       <c r="AK31" s="188" t="str">
         <f>Main!AM33</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="32" spans="1:37">
@@ -16236,15 +16233,15 @@
       </c>
       <c r="AE32" s="183">
         <f>Main!AG34</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF32" s="184">
         <f>Main!AH34</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG32" s="151">
         <f>Main!AI34</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="AH32" s="156">
         <f>Main!AJ34</f>
@@ -16260,7 +16257,7 @@
       </c>
       <c r="AK32" s="188" t="str">
         <f>Main!AM34</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="33" spans="1:37">
@@ -16386,11 +16383,11 @@
       </c>
       <c r="AE33" s="183">
         <f>Main!AG35</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF33" s="184">
         <f>Main!AH35</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG33" s="151">
         <f>Main!AI35</f>
@@ -16410,7 +16407,7 @@
       </c>
       <c r="AK33" s="188" t="str">
         <f>Main!AM35</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="34" spans="1:37">
@@ -16524,7 +16521,7 @@
       </c>
       <c r="AB34" s="173">
         <f>Main!AD36</f>
-        <v>2.2999999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="AC34" s="174">
         <f>Main!AE36</f>
@@ -16532,7 +16529,7 @@
       </c>
       <c r="AD34" s="175">
         <f>Main!AF36</f>
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="AE34" s="183">
         <f>Main!AG36</f>
@@ -16560,7 +16557,7 @@
       </c>
       <c r="AK34" s="188" t="str">
         <f>Main!AM36</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="35" spans="1:37">
@@ -16674,15 +16671,15 @@
       </c>
       <c r="AB35" s="173">
         <f>Main!AD37</f>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AC35" s="174">
         <f>Main!AE37</f>
-        <v>6</v>
+        <v>4.75</v>
       </c>
       <c r="AD35" s="175">
         <f>Main!AF37</f>
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="AE35" s="183">
         <f>Main!AG37</f>
@@ -16710,7 +16707,7 @@
       </c>
       <c r="AK35" s="188" t="str">
         <f>Main!AM37</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="36" spans="1:37">
@@ -16828,11 +16825,11 @@
       </c>
       <c r="AC36" s="174">
         <f>Main!AE38</f>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="AD36" s="175">
         <f>Main!AF38</f>
-        <v>1.18</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="AE36" s="183">
         <f>Main!AG38</f>
@@ -16860,7 +16857,7 @@
       </c>
       <c r="AK36" s="188" t="str">
         <f>Main!AM38</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="37" spans="1:37">
@@ -16974,15 +16971,15 @@
       </c>
       <c r="AB37" s="173">
         <f>Main!AD39</f>
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="AC37" s="174">
         <f>Main!AE39</f>
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="AD37" s="175">
         <f>Main!AF39</f>
-        <v>2.87</v>
+        <v>2.7</v>
       </c>
       <c r="AE37" s="183">
         <f>Main!AG39</f>
@@ -17010,7 +17007,7 @@
       </c>
       <c r="AK37" s="188" t="str">
         <f>Main!AM39</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="38" spans="1:37">
@@ -17124,15 +17121,15 @@
       </c>
       <c r="AB38" s="173">
         <f>Main!AD40</f>
-        <v>7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AC38" s="174">
         <f>Main!AE40</f>
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="AD38" s="175">
         <f>Main!AF40</f>
-        <v>1.44</v>
+        <v>1.83</v>
       </c>
       <c r="AE38" s="183">
         <f>Main!AG40</f>
@@ -17160,7 +17157,7 @@
       </c>
       <c r="AK38" s="188" t="str">
         <f>Main!AM40</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="39" spans="1:37">
@@ -17274,15 +17271,15 @@
       </c>
       <c r="AB39" s="173">
         <f>Main!AD41</f>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="AC39" s="174">
         <f>Main!AE41</f>
-        <v>3.25</v>
+        <v>3.1</v>
       </c>
       <c r="AD39" s="175">
         <f>Main!AF41</f>
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="AE39" s="183">
         <f>Main!AG41</f>
@@ -17310,7 +17307,7 @@
       </c>
       <c r="AK39" s="188" t="str">
         <f>Main!AM41</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="40" spans="1:37">
@@ -17424,15 +17421,15 @@
       </c>
       <c r="AB40" s="173">
         <f>Main!AD42</f>
-        <v>4.3</v>
+        <v>3</v>
       </c>
       <c r="AC40" s="174">
         <f>Main!AE42</f>
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="AD40" s="175">
         <f>Main!AF42</f>
-        <v>1.8</v>
+        <v>2.37</v>
       </c>
       <c r="AE40" s="183">
         <f>Main!AG42</f>
@@ -17460,7 +17457,7 @@
       </c>
       <c r="AK40" s="188" t="str">
         <f>Main!AM42</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="41" spans="1:37">
@@ -17574,15 +17571,15 @@
       </c>
       <c r="AB41" s="173">
         <f>Main!AD43</f>
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="AC41" s="174">
         <f>Main!AE43</f>
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="AD41" s="175">
         <f>Main!AF43</f>
-        <v>2.2999999999999998</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="AE41" s="183">
         <f>Main!AG43</f>
@@ -17610,7 +17607,7 @@
       </c>
       <c r="AK41" s="188" t="str">
         <f>Main!AM43</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="42" spans="1:37">
@@ -17724,15 +17721,15 @@
       </c>
       <c r="AB42" s="173">
         <f>Main!AD44</f>
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="AC42" s="174">
         <f>Main!AE44</f>
-        <v>4.5</v>
+        <v>3.8</v>
       </c>
       <c r="AD42" s="175">
         <f>Main!AF44</f>
-        <v>1.36</v>
+        <v>1.55</v>
       </c>
       <c r="AE42" s="183">
         <f>Main!AG44</f>
@@ -17760,7 +17757,7 @@
       </c>
       <c r="AK42" s="188" t="str">
         <f>Main!AM44</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="43" spans="1:37">
@@ -17874,15 +17871,15 @@
       </c>
       <c r="AB43" s="173">
         <f>Main!AD45</f>
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="AC43" s="174">
         <f>Main!AE45</f>
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="AD43" s="175">
         <f>Main!AF45</f>
-        <v>6</v>
+        <v>3.6</v>
       </c>
       <c r="AE43" s="183">
         <f>Main!AG45</f>
@@ -17910,7 +17907,7 @@
       </c>
       <c r="AK43" s="188" t="str">
         <f>Main!AM45</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="44" spans="1:37">
@@ -18024,7 +18021,7 @@
       </c>
       <c r="AB44" s="173">
         <f>Main!AD46</f>
-        <v>3.75</v>
+        <v>4.5</v>
       </c>
       <c r="AC44" s="174">
         <f>Main!AE46</f>
@@ -18032,7 +18029,7 @@
       </c>
       <c r="AD44" s="175">
         <f>Main!AF46</f>
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="AE44" s="183">
         <f>Main!AG46</f>
@@ -18060,7 +18057,7 @@
       </c>
       <c r="AK44" s="188" t="str">
         <f>Main!AM46</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="45" spans="1:37">
@@ -18174,15 +18171,15 @@
       </c>
       <c r="AB45" s="173">
         <f>Main!AD47</f>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="AC45" s="174">
         <f>Main!AE47</f>
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="AD45" s="175">
         <f>Main!AF47</f>
-        <v>1.57</v>
+        <v>1.44</v>
       </c>
       <c r="AE45" s="183">
         <f>Main!AG47</f>
@@ -18210,7 +18207,7 @@
       </c>
       <c r="AK45" s="188" t="str">
         <f>Main!AM47</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="46" spans="1:37">
@@ -18324,15 +18321,15 @@
       </c>
       <c r="AB46" s="173">
         <f>Main!AD48</f>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="AC46" s="174">
         <f>Main!AE48</f>
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="AD46" s="175">
         <f>Main!AF48</f>
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="AE46" s="183">
         <f>Main!AG48</f>
@@ -18360,7 +18357,7 @@
       </c>
       <c r="AK46" s="188" t="str">
         <f>Main!AM48</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="47" spans="1:37">
@@ -18474,15 +18471,15 @@
       </c>
       <c r="AB47" s="173">
         <f>Main!AD49</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="AC47" s="174">
         <f>Main!AE49</f>
-        <v>4.4000000000000004</v>
+        <v>2.5</v>
       </c>
       <c r="AD47" s="175">
         <f>Main!AF49</f>
-        <v>1.4</v>
+        <v>1.72</v>
       </c>
       <c r="AE47" s="183">
         <f>Main!AG49</f>
@@ -18510,7 +18507,7 @@
       </c>
       <c r="AK47" s="188" t="str">
         <f>Main!AM49</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="48" spans="1:37">
@@ -18624,15 +18621,15 @@
       </c>
       <c r="AB48" s="173">
         <f>Main!AD50</f>
-        <v>6</v>
+        <v>3.8</v>
       </c>
       <c r="AC48" s="174">
         <f>Main!AE50</f>
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="AD48" s="175">
         <f>Main!AF50</f>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="AE48" s="183">
         <f>Main!AG50</f>
@@ -18660,7 +18657,7 @@
       </c>
       <c r="AK48" s="188" t="str">
         <f>Main!AM50</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
     <row r="49" spans="1:37" ht="15.75" thickBot="1">
@@ -18774,15 +18771,15 @@
       </c>
       <c r="AB49" s="176">
         <f>Main!AD51</f>
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="AC49" s="177">
         <f>Main!AE51</f>
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="AD49" s="178">
         <f>Main!AF51</f>
-        <v>1.61</v>
+        <v>1.8</v>
       </c>
       <c r="AE49" s="185">
         <f>Main!AG51</f>
@@ -18810,7 +18807,7 @@
       </c>
       <c r="AK49" s="189" t="str">
         <f>Main!AM51</f>
-        <v>future</v>
+        <v>predict</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temporary predictions for 29/6
</commit_message>
<xml_diff>
--- a/data/data_wc2014.xlsx
+++ b/data/data_wc2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="474" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="474" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="538" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="99">
   <si>
     <t>Team</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>future</t>
   </si>
 </sst>
 </file>
@@ -4441,11 +4444,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMP67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F46" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="AC46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
+      <selection pane="bottomRight" activeCell="AG59" sqref="AG59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5039,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="AI5" s="150">
-        <f t="shared" ref="AI5:AI51" si="2">AG5-AH5</f>
+        <f t="shared" ref="AI5:AI67" si="2">AG5-AH5</f>
         <v>1</v>
       </c>
       <c r="AJ5" s="156">
@@ -11803,19 +11806,26 @@
         <v>6</v>
       </c>
       <c r="AG52" s="206">
+        <v>1</v>
+      </c>
+      <c r="AH52" s="207">
+        <v>1</v>
+      </c>
+      <c r="AI52" s="208">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AH52" s="207">
-        <v>0</v>
-      </c>
-      <c r="AI52" s="208">
-        <v>0</v>
-      </c>
-      <c r="AJ52" s="209"/>
-      <c r="AK52" s="210"/>
-      <c r="AL52" s="211"/>
+      <c r="AJ52" s="209">
+        <v>1.54</v>
+      </c>
+      <c r="AK52" s="210">
+        <v>1.54</v>
+      </c>
+      <c r="AL52" s="211">
+        <v>0.02</v>
+      </c>
       <c r="AM52" s="212" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO52" s="2">
         <f t="shared" ref="AO52:AO54" si="5">SUM(F52:H52)</f>
@@ -11942,19 +11952,26 @@
         <v>4</v>
       </c>
       <c r="AG53" s="183">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH53" s="184">
         <v>0</v>
       </c>
       <c r="AI53" s="151">
-        <v>0</v>
-      </c>
-      <c r="AJ53" s="156"/>
-      <c r="AK53" s="157"/>
-      <c r="AL53" s="158"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AJ53" s="156">
+        <v>1.08</v>
+      </c>
+      <c r="AK53" s="157">
+        <v>1.29</v>
+      </c>
+      <c r="AL53" s="158">
+        <v>-0.24</v>
+      </c>
       <c r="AM53" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO53" s="2">
         <f t="shared" si="5"/>
@@ -12072,13 +12089,13 @@
         <v>8</v>
       </c>
       <c r="AD54" s="173">
-        <v>2.1</v>
+        <v>1.95</v>
       </c>
       <c r="AE54" s="174">
         <v>3.4</v>
       </c>
       <c r="AF54" s="175">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="AG54" s="183">
         <v>0</v>
@@ -12087,6 +12104,7 @@
         <v>0</v>
       </c>
       <c r="AI54" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ54" s="156"/>
@@ -12211,13 +12229,13 @@
         <v>32</v>
       </c>
       <c r="AD55" s="173">
-        <v>2.4500000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="AE55" s="174">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="AF55" s="175">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="AG55" s="183">
         <v>0</v>
@@ -12226,6 +12244,7 @@
         <v>0</v>
       </c>
       <c r="AI55" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ55" s="156"/>
@@ -12357,13 +12376,14 @@
         <v>0</v>
       </c>
       <c r="AI56" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ56" s="156"/>
       <c r="AK56" s="157"/>
       <c r="AL56" s="158"/>
       <c r="AM56" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="2:42">
@@ -12488,13 +12508,14 @@
         <v>0</v>
       </c>
       <c r="AI57" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ57" s="156"/>
       <c r="AK57" s="157"/>
       <c r="AL57" s="158"/>
       <c r="AM57" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="2:42">
@@ -12619,13 +12640,14 @@
         <v>0</v>
       </c>
       <c r="AI58" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ58" s="156"/>
       <c r="AK58" s="157"/>
       <c r="AL58" s="158"/>
       <c r="AM58" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="2:42">
@@ -12735,13 +12757,13 @@
         <v>3</v>
       </c>
       <c r="AD59" s="173">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="AE59" s="174">
         <v>3.5</v>
       </c>
       <c r="AF59" s="175">
-        <v>4.2</v>
+        <v>3.8</v>
       </c>
       <c r="AG59" s="183">
         <v>0</v>
@@ -12750,13 +12772,14 @@
         <v>0</v>
       </c>
       <c r="AI59" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ59" s="156"/>
       <c r="AK59" s="157"/>
       <c r="AL59" s="158"/>
       <c r="AM59" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="2:42">
@@ -12864,13 +12887,14 @@
         <v>0</v>
       </c>
       <c r="AI60" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ60" s="156"/>
       <c r="AK60" s="157"/>
       <c r="AL60" s="158"/>
       <c r="AM60" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="2:42">
@@ -12978,13 +13002,14 @@
         <v>0</v>
       </c>
       <c r="AI61" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ61" s="156"/>
       <c r="AK61" s="157"/>
       <c r="AL61" s="158"/>
       <c r="AM61" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="2:42">
@@ -13092,13 +13117,14 @@
         <v>0</v>
       </c>
       <c r="AI62" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ62" s="156"/>
       <c r="AK62" s="157"/>
       <c r="AL62" s="158"/>
       <c r="AM62" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="2:42">
@@ -13206,13 +13232,14 @@
         <v>0</v>
       </c>
       <c r="AI63" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ63" s="156"/>
       <c r="AK63" s="157"/>
       <c r="AL63" s="158"/>
       <c r="AM63" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="2:42">
@@ -13320,13 +13347,14 @@
         <v>0</v>
       </c>
       <c r="AI64" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ64" s="156"/>
       <c r="AK64" s="157"/>
       <c r="AL64" s="158"/>
       <c r="AM64" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="2:39">
@@ -13434,13 +13462,14 @@
         <v>0</v>
       </c>
       <c r="AI65" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ65" s="156"/>
       <c r="AK65" s="157"/>
       <c r="AL65" s="158"/>
       <c r="AM65" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="2:39">
@@ -13548,13 +13577,14 @@
         <v>0</v>
       </c>
       <c r="AI66" s="151">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ66" s="156"/>
       <c r="AK66" s="157"/>
       <c r="AL66" s="158"/>
       <c r="AM66" s="67" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="2:39" ht="15.75" thickBot="1">
@@ -13662,13 +13692,14 @@
         <v>0</v>
       </c>
       <c r="AI67" s="152">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ67" s="159"/>
       <c r="AK67" s="160"/>
       <c r="AL67" s="161"/>
       <c r="AM67" s="68" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -13692,8 +13723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="M43" workbookViewId="0">
+      <selection activeCell="AI50" sqref="AI50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20778,11 +20809,11 @@
       </c>
       <c r="AC50" s="183">
         <f>Main!AG52</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD50" s="184">
         <f>Main!AH52</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE50" s="151">
         <f>Main!AI52</f>
@@ -20790,19 +20821,19 @@
       </c>
       <c r="AF50" s="156">
         <f>Main!AJ52</f>
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="AG50" s="157">
         <f>Main!AK52</f>
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="AH50" s="158">
         <f>Main!AL52</f>
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AI50" s="188" t="str">
         <f>Main!AM52</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="51" spans="1:35">
@@ -20920,7 +20951,7 @@
       </c>
       <c r="AC51" s="183">
         <f>Main!AG53</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD51" s="184">
         <f>Main!AH53</f>
@@ -20928,23 +20959,23 @@
       </c>
       <c r="AE51" s="151">
         <f>Main!AI53</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF51" s="156">
         <f>Main!AJ53</f>
-        <v>0</v>
+        <v>1.08</v>
       </c>
       <c r="AG51" s="157">
         <f>Main!AK53</f>
-        <v>0</v>
+        <v>1.29</v>
       </c>
       <c r="AH51" s="158">
         <f>Main!AL53</f>
-        <v>0</v>
+        <v>-0.24</v>
       </c>
       <c r="AI51" s="188" t="str">
         <f>Main!AM53</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="52" spans="1:35">
@@ -21050,7 +21081,7 @@
       </c>
       <c r="Z52" s="173">
         <f>Main!AD54</f>
-        <v>2.1</v>
+        <v>1.95</v>
       </c>
       <c r="AA52" s="174">
         <f>Main!AE54</f>
@@ -21058,7 +21089,7 @@
       </c>
       <c r="AB52" s="175">
         <f>Main!AF54</f>
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="AC52" s="183">
         <f>Main!AG54</f>
@@ -21192,15 +21223,15 @@
       </c>
       <c r="Z53" s="173">
         <f>Main!AD55</f>
-        <v>2.4500000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="AA53" s="174">
         <f>Main!AE55</f>
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="AB53" s="175">
         <f>Main!AF55</f>
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="AC53" s="183">
         <f>Main!AG55</f>
@@ -21370,7 +21401,7 @@
       </c>
       <c r="AI54" s="188" t="str">
         <f>Main!AM56</f>
-        <v>predict</v>
+        <v>future</v>
       </c>
     </row>
     <row r="55" spans="1:35">
@@ -21512,7 +21543,7 @@
       </c>
       <c r="AI55" s="188" t="str">
         <f>Main!AM57</f>
-        <v>predict</v>
+        <v>future</v>
       </c>
     </row>
     <row r="56" spans="1:35">
@@ -21654,7 +21685,7 @@
       </c>
       <c r="AI56" s="188" t="str">
         <f>Main!AM58</f>
-        <v>predict</v>
+        <v>future</v>
       </c>
     </row>
     <row r="57" spans="1:35">
@@ -21760,7 +21791,7 @@
       </c>
       <c r="Z57" s="173">
         <f>Main!AD59</f>
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="AA57" s="174">
         <f>Main!AE59</f>
@@ -21768,7 +21799,7 @@
       </c>
       <c r="AB57" s="175">
         <f>Main!AF59</f>
-        <v>4.2</v>
+        <v>3.8</v>
       </c>
       <c r="AC57" s="183">
         <f>Main!AG59</f>
@@ -21796,7 +21827,7 @@
       </c>
       <c r="AI57" s="188" t="str">
         <f>Main!AM59</f>
-        <v>predict</v>
+        <v>future</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Predictions for 4 July
</commit_message>
<xml_diff>
--- a/data/data_wc2014.xlsx
+++ b/data/data_wc2014.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="99">
   <si>
     <t>Team</t>
   </si>
@@ -1664,42 +1664,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="13" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1764,6 +1728,42 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4445,10 +4445,10 @@
   <dimension ref="A1:AMP67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="AE46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AG55" sqref="AG55"/>
+      <selection pane="bottomRight" activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11551,102 +11551,102 @@
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="C51" s="213">
+      <c r="C51" s="201">
         <v>41816</v>
       </c>
-      <c r="D51" s="214" t="s">
+      <c r="D51" s="202" t="s">
         <v>38</v>
       </c>
-      <c r="E51" s="215" t="s">
+      <c r="E51" s="203" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="216">
+      <c r="F51" s="204">
         <v>19</v>
       </c>
-      <c r="G51" s="217">
+      <c r="G51" s="205">
         <v>54</v>
       </c>
-      <c r="H51" s="218">
+      <c r="H51" s="206">
         <v>27</v>
       </c>
-      <c r="I51" s="219">
+      <c r="I51" s="207">
         <v>11.6</v>
       </c>
-      <c r="J51" s="220">
+      <c r="J51" s="208">
         <v>23.6</v>
       </c>
-      <c r="K51" s="221">
+      <c r="K51" s="209">
         <v>64.8</v>
       </c>
-      <c r="L51" s="219">
+      <c r="L51" s="207">
         <f>VLOOKUP($D51,'538'!$B$4:$F$35,3,0)</f>
         <v>72.400000000000006</v>
       </c>
-      <c r="M51" s="220">
+      <c r="M51" s="208">
         <f>VLOOKUP($D51,'538'!$B$4:$F$35,4,0)</f>
         <v>1.7</v>
       </c>
-      <c r="N51" s="221">
+      <c r="N51" s="209">
         <f>VLOOKUP($D51,'538'!$B$4:$F$35,5,0)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O51" s="222">
+      <c r="O51" s="210">
         <f>VLOOKUP($E51,'538'!$B$4:$F$35,3,0)</f>
         <v>82</v>
       </c>
-      <c r="P51" s="220">
+      <c r="P51" s="208">
         <f>VLOOKUP($E51,'538'!$B$4:$F$35,4,0)</f>
         <v>2.1</v>
       </c>
-      <c r="Q51" s="223">
+      <c r="Q51" s="211">
         <f>VLOOKUP($E51,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="R51" s="216">
+      <c r="R51" s="204">
         <f>VLOOKUP($D51,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>1.9</v>
       </c>
-      <c r="S51" s="217">
+      <c r="S51" s="205">
         <f>VLOOKUP($D51,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>1.4</v>
       </c>
-      <c r="T51" s="217">
+      <c r="T51" s="205">
         <f>VLOOKUP($D51,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>1.5</v>
       </c>
-      <c r="U51" s="216">
+      <c r="U51" s="204">
         <f>VLOOKUP($E51,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.6</v>
       </c>
-      <c r="V51" s="217">
+      <c r="V51" s="205">
         <f>VLOOKUP($E51,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="W51" s="217">
+      <c r="W51" s="205">
         <f>VLOOKUP($E51,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.3</v>
       </c>
-      <c r="X51" s="216">
+      <c r="X51" s="204">
         <f>VLOOKUP($D51,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>57</v>
       </c>
-      <c r="Y51" s="224">
+      <c r="Y51" s="212">
         <f>VLOOKUP($D51,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="Z51" s="218">
+      <c r="Z51" s="206">
         <f>VLOOKUP($D51,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="AA51" s="216">
+      <c r="AA51" s="204">
         <f>VLOOKUP($E51,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="AB51" s="224">
+      <c r="AB51" s="212">
         <f>VLOOKUP($E51,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="AC51" s="218">
+      <c r="AC51" s="206">
         <f>VLOOKUP($E51,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>4</v>
       </c>
@@ -11695,136 +11695,136 @@
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="C52" s="191">
+      <c r="C52" s="213">
         <v>41818</v>
       </c>
-      <c r="D52" s="192" t="s">
+      <c r="D52" s="214" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="193" t="s">
+      <c r="E52" s="215" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="194">
+      <c r="F52" s="216">
         <v>78</v>
       </c>
-      <c r="G52" s="195">
+      <c r="G52" s="217">
         <f>100-F52</f>
         <v>22</v>
       </c>
-      <c r="H52" s="196" t="s">
+      <c r="H52" s="218" t="s">
         <v>97</v>
       </c>
-      <c r="I52" s="197">
+      <c r="I52" s="219">
         <v>81.099999999999994</v>
       </c>
-      <c r="J52" s="198" t="s">
+      <c r="J52" s="220" t="s">
         <v>97</v>
       </c>
-      <c r="K52" s="199">
-        <f t="shared" ref="K52:K59" si="4">100-I52</f>
+      <c r="K52" s="221">
+        <f t="shared" ref="K52:K63" si="4">100-I52</f>
         <v>18.900000000000006</v>
       </c>
-      <c r="L52" s="197">
+      <c r="L52" s="219">
         <f>VLOOKUP($D52,'538'!$B$4:$F$35,3,0)</f>
         <v>91.8</v>
       </c>
-      <c r="M52" s="198">
+      <c r="M52" s="220">
         <f>VLOOKUP($D52,'538'!$B$4:$F$35,4,0)</f>
         <v>3.4</v>
       </c>
-      <c r="N52" s="199">
+      <c r="N52" s="221">
         <f>VLOOKUP($D52,'538'!$B$4:$F$35,5,0)</f>
         <v>0.5</v>
       </c>
-      <c r="O52" s="200">
+      <c r="O52" s="222">
         <f>VLOOKUP($E52,'538'!$B$4:$F$35,3,0)</f>
         <v>86.7</v>
       </c>
-      <c r="P52" s="198">
+      <c r="P52" s="220">
         <f>VLOOKUP($E52,'538'!$B$4:$F$35,4,0)</f>
         <v>2.7</v>
       </c>
-      <c r="Q52" s="201">
+      <c r="Q52" s="223">
         <f>VLOOKUP($E52,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="R52" s="194">
+      <c r="R52" s="216">
         <f>VLOOKUP($D52,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="S52" s="195">
+      <c r="S52" s="217">
         <f>VLOOKUP($D52,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="T52" s="195">
+      <c r="T52" s="217">
         <f>VLOOKUP($D52,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="U52" s="194">
+      <c r="U52" s="216">
         <f>VLOOKUP($E52,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.2</v>
       </c>
-      <c r="V52" s="195">
+      <c r="V52" s="217">
         <f>VLOOKUP($E52,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>2.6</v>
       </c>
-      <c r="W52" s="195">
+      <c r="W52" s="217">
         <f>VLOOKUP($E52,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>3.6</v>
       </c>
-      <c r="X52" s="194">
+      <c r="X52" s="216">
         <f>VLOOKUP($D52,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="Y52" s="202">
+      <c r="Y52" s="224">
         <f>VLOOKUP($D52,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="Z52" s="196">
+      <c r="Z52" s="218">
         <f>VLOOKUP($D52,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AA52" s="194">
+      <c r="AA52" s="216">
         <f>VLOOKUP($E52,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>14</v>
       </c>
-      <c r="AB52" s="202">
+      <c r="AB52" s="224">
         <f>VLOOKUP($E52,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="AC52" s="196">
+      <c r="AC52" s="218">
         <f>VLOOKUP($E52,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="AD52" s="203">
+      <c r="AD52" s="191">
         <v>1.53</v>
       </c>
-      <c r="AE52" s="204">
+      <c r="AE52" s="192">
         <v>4.2</v>
       </c>
-      <c r="AF52" s="205">
+      <c r="AF52" s="193">
         <v>6</v>
       </c>
-      <c r="AG52" s="206">
+      <c r="AG52" s="194">
         <v>1</v>
       </c>
-      <c r="AH52" s="207">
+      <c r="AH52" s="195">
         <v>1</v>
       </c>
-      <c r="AI52" s="208">
+      <c r="AI52" s="196">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ52" s="209">
+      <c r="AJ52" s="197">
         <v>1.54</v>
       </c>
-      <c r="AK52" s="210">
+      <c r="AK52" s="198">
         <v>1.54</v>
       </c>
-      <c r="AL52" s="211">
+      <c r="AL52" s="199">
         <v>0.02</v>
       </c>
-      <c r="AM52" s="212" t="s">
+      <c r="AM52" s="200" t="s">
         <v>61</v>
       </c>
       <c r="AO52" s="2">
@@ -11841,104 +11841,104 @@
         <f t="shared" ref="B53" si="7">B52+1</f>
         <v>50</v>
       </c>
-      <c r="C53" s="48">
+      <c r="C53" s="47">
         <v>41818</v>
       </c>
-      <c r="D53" s="53" t="s">
+      <c r="D53" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="58" t="s">
+      <c r="E53" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="26">
+      <c r="F53" s="24">
         <v>63</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="12">
         <f t="shared" ref="G53:G67" si="8">100-F53</f>
         <v>37</v>
       </c>
-      <c r="H53" s="27" t="s">
+      <c r="H53" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I53" s="37">
+      <c r="I53" s="35">
         <v>54</v>
       </c>
-      <c r="J53" s="9" t="s">
+      <c r="J53" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K53" s="38">
+      <c r="K53" s="36">
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="L53" s="37">
+      <c r="L53" s="35">
         <f>VLOOKUP($D53,'538'!$B$4:$F$35,3,0)</f>
         <v>85.8</v>
       </c>
-      <c r="M53" s="9">
+      <c r="M53" s="13">
         <f>VLOOKUP($D53,'538'!$B$4:$F$35,4,0)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="N53" s="38">
+      <c r="N53" s="36">
         <f>VLOOKUP($D53,'538'!$B$4:$F$35,5,0)</f>
         <v>0.5</v>
       </c>
-      <c r="O53" s="19">
+      <c r="O53" s="18">
         <f>VLOOKUP($E53,'538'!$B$4:$F$35,3,0)</f>
         <v>83.3</v>
       </c>
-      <c r="P53" s="9">
+      <c r="P53" s="13">
         <f>VLOOKUP($E53,'538'!$B$4:$F$35,4,0)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q53" s="64">
+      <c r="Q53" s="63">
         <f>VLOOKUP($E53,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="R53" s="26">
+      <c r="R53" s="24">
         <f>VLOOKUP($D53,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.9</v>
       </c>
-      <c r="S53" s="8">
+      <c r="S53" s="12">
         <f>VLOOKUP($D53,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="T53" s="8">
+      <c r="T53" s="12">
         <f>VLOOKUP($D53,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="U53" s="26">
+      <c r="U53" s="24">
         <f>VLOOKUP($E53,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.3</v>
       </c>
-      <c r="V53" s="8">
+      <c r="V53" s="12">
         <f>VLOOKUP($E53,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>3.1</v>
       </c>
-      <c r="W53" s="8">
+      <c r="W53" s="12">
         <f>VLOOKUP($E53,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>3.8</v>
       </c>
-      <c r="X53" s="26">
+      <c r="X53" s="24">
         <f>VLOOKUP($D53,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="Y53" s="102">
+      <c r="Y53" s="101">
         <f>VLOOKUP($D53,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="Z53" s="27">
+      <c r="Z53" s="25">
         <f>VLOOKUP($D53,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="AA53" s="26">
+      <c r="AA53" s="24">
         <f>VLOOKUP($E53,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="AB53" s="102">
+      <c r="AB53" s="101">
         <f>VLOOKUP($E53,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="AC53" s="27">
+      <c r="AC53" s="25">
         <f>VLOOKUP($E53,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
@@ -11987,104 +11987,104 @@
         <f t="shared" ref="B54:B67" si="9">B53+1</f>
         <v>51</v>
       </c>
-      <c r="C54" s="48">
+      <c r="C54" s="47">
         <v>41819</v>
       </c>
-      <c r="D54" s="53" t="s">
+      <c r="D54" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E54" s="58" t="s">
+      <c r="E54" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="F54" s="26">
+      <c r="F54" s="24">
         <v>69</v>
       </c>
-      <c r="G54" s="8">
+      <c r="G54" s="12">
         <f t="shared" si="8"/>
         <v>31</v>
       </c>
-      <c r="H54" s="27" t="s">
+      <c r="H54" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I54" s="37">
+      <c r="I54" s="35">
         <v>65.599999999999994</v>
       </c>
-      <c r="J54" s="9" t="s">
+      <c r="J54" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K54" s="38">
+      <c r="K54" s="36">
         <f t="shared" si="4"/>
         <v>34.400000000000006</v>
       </c>
-      <c r="L54" s="37">
+      <c r="L54" s="35">
         <f>VLOOKUP($D54,'538'!$B$4:$F$35,3,0)</f>
         <v>82.5</v>
       </c>
-      <c r="M54" s="9">
+      <c r="M54" s="13">
         <f>VLOOKUP($D54,'538'!$B$4:$F$35,4,0)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="N54" s="38">
+      <c r="N54" s="36">
         <f>VLOOKUP($D54,'538'!$B$4:$F$35,5,0)</f>
         <v>0.8</v>
       </c>
-      <c r="O54" s="19">
+      <c r="O54" s="18">
         <f>VLOOKUP($E54,'538'!$B$4:$F$35,3,0)</f>
         <v>77</v>
       </c>
-      <c r="P54" s="9">
+      <c r="P54" s="13">
         <f>VLOOKUP($E54,'538'!$B$4:$F$35,4,0)</f>
         <v>1.6</v>
       </c>
-      <c r="Q54" s="64">
+      <c r="Q54" s="63">
         <f>VLOOKUP($E54,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="R54" s="26">
+      <c r="R54" s="24">
         <f>VLOOKUP($D54,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.9</v>
       </c>
-      <c r="S54" s="8">
+      <c r="S54" s="12">
         <f>VLOOKUP($D54,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="T54" s="8">
+      <c r="T54" s="12">
         <f>VLOOKUP($D54,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.2</v>
       </c>
-      <c r="U54" s="26">
+      <c r="U54" s="24">
         <f>VLOOKUP($E54,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="V54" s="8">
+      <c r="V54" s="12">
         <f>VLOOKUP($E54,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>3.1</v>
       </c>
-      <c r="W54" s="8">
+      <c r="W54" s="12">
         <f>VLOOKUP($E54,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>2.7</v>
       </c>
-      <c r="X54" s="26">
+      <c r="X54" s="24">
         <f>VLOOKUP($D54,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="Y54" s="102">
+      <c r="Y54" s="101">
         <f>VLOOKUP($D54,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="Z54" s="27">
+      <c r="Z54" s="25">
         <f>VLOOKUP($D54,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="AA54" s="26">
+      <c r="AA54" s="24">
         <f>VLOOKUP($E54,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>20</v>
       </c>
-      <c r="AB54" s="102">
+      <c r="AB54" s="101">
         <f>VLOOKUP($E54,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>14</v>
       </c>
-      <c r="AC54" s="27">
+      <c r="AC54" s="25">
         <f>VLOOKUP($E54,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>8</v>
       </c>
@@ -12133,104 +12133,104 @@
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
-      <c r="C55" s="48">
+      <c r="C55" s="47">
         <v>41819</v>
       </c>
-      <c r="D55" s="53" t="s">
+      <c r="D55" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="E55" s="58" t="s">
+      <c r="E55" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="26">
+      <c r="F55" s="24">
         <v>56</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="12">
         <f t="shared" si="8"/>
         <v>44</v>
       </c>
-      <c r="H55" s="27" t="s">
+      <c r="H55" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I55" s="37">
+      <c r="I55" s="35">
         <v>32.299999999999997</v>
       </c>
-      <c r="J55" s="9" t="s">
+      <c r="J55" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K55" s="38">
+      <c r="K55" s="36">
         <f t="shared" si="4"/>
         <v>67.7</v>
       </c>
-      <c r="L55" s="37">
+      <c r="L55" s="35">
         <f>VLOOKUP($D55,'538'!$B$4:$F$35,3,0)</f>
         <v>74.099999999999994</v>
       </c>
-      <c r="M55" s="9">
+      <c r="M55" s="13">
         <f>VLOOKUP($D55,'538'!$B$4:$F$35,4,0)</f>
         <v>1.3</v>
       </c>
-      <c r="N55" s="38">
+      <c r="N55" s="36">
         <f>VLOOKUP($D55,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="O55" s="19">
+      <c r="O55" s="18">
         <f>VLOOKUP($E55,'538'!$B$4:$F$35,3,0)</f>
         <v>76.8</v>
       </c>
-      <c r="P55" s="9">
+      <c r="P55" s="13">
         <f>VLOOKUP($E55,'538'!$B$4:$F$35,4,0)</f>
         <v>1.3</v>
       </c>
-      <c r="Q55" s="64">
+      <c r="Q55" s="63">
         <f>VLOOKUP($E55,'538'!$B$4:$F$35,5,0)</f>
         <v>0.5</v>
       </c>
-      <c r="R55" s="26">
+      <c r="R55" s="24">
         <f>VLOOKUP($D55,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>1.6</v>
       </c>
-      <c r="S55" s="8">
+      <c r="S55" s="12">
         <f>VLOOKUP($D55,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>1.2</v>
       </c>
-      <c r="T55" s="8">
+      <c r="T55" s="12">
         <f>VLOOKUP($D55,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>1.3</v>
       </c>
-      <c r="U55" s="26">
+      <c r="U55" s="24">
         <f>VLOOKUP($E55,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="V55" s="8">
+      <c r="V55" s="12">
         <f>VLOOKUP($E55,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>3.8</v>
       </c>
-      <c r="W55" s="8">
+      <c r="W55" s="12">
         <f>VLOOKUP($E55,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="X55" s="26">
+      <c r="X55" s="24">
         <f>VLOOKUP($D55,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="Y55" s="102">
+      <c r="Y55" s="101">
         <f>VLOOKUP($D55,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="Z55" s="27">
+      <c r="Z55" s="25">
         <f>VLOOKUP($D55,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="AA55" s="26">
+      <c r="AA55" s="24">
         <f>VLOOKUP($E55,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>12</v>
       </c>
-      <c r="AB55" s="102">
+      <c r="AB55" s="101">
         <f>VLOOKUP($E55,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="AC55" s="27">
+      <c r="AC55" s="25">
         <f>VLOOKUP($E55,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>32</v>
       </c>
@@ -12264,6 +12264,14 @@
       </c>
       <c r="AM55" s="67" t="s">
         <v>61</v>
+      </c>
+      <c r="AO55" s="2">
+        <f t="shared" ref="AO55:AO63" si="10">SUM(F55:H55)</f>
+        <v>100</v>
+      </c>
+      <c r="AP55" s="2">
+        <f t="shared" ref="AP55:AP60" si="11">SUM(I55:K55)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="2:42">
@@ -12271,104 +12279,104 @@
         <f t="shared" si="9"/>
         <v>53</v>
       </c>
-      <c r="C56" s="48">
+      <c r="C56" s="47">
         <v>41820</v>
       </c>
-      <c r="D56" s="53" t="s">
+      <c r="D56" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="58" t="s">
+      <c r="E56" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="F56" s="26">
+      <c r="F56" s="24">
         <v>72</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="12">
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="H56" s="27" t="s">
+      <c r="H56" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I56" s="37">
+      <c r="I56" s="35">
         <v>66.8</v>
       </c>
-      <c r="J56" s="9" t="s">
+      <c r="J56" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K56" s="38">
+      <c r="K56" s="36">
         <f t="shared" si="4"/>
         <v>33.200000000000003</v>
       </c>
-      <c r="L56" s="37">
+      <c r="L56" s="35">
         <f>VLOOKUP($D56,'538'!$B$4:$F$35,3,0)</f>
         <v>86.1</v>
       </c>
-      <c r="M56" s="9">
+      <c r="M56" s="13">
         <f>VLOOKUP($D56,'538'!$B$4:$F$35,4,0)</f>
         <v>2.5</v>
       </c>
-      <c r="N56" s="38">
+      <c r="N56" s="36">
         <f>VLOOKUP($D56,'538'!$B$4:$F$35,5,0)</f>
         <v>0.6</v>
       </c>
-      <c r="O56" s="19">
+      <c r="O56" s="18">
         <f>VLOOKUP($E56,'538'!$B$4:$F$35,3,0)</f>
         <v>75.2</v>
       </c>
-      <c r="P56" s="9">
+      <c r="P56" s="13">
         <f>VLOOKUP($E56,'538'!$B$4:$F$35,4,0)</f>
         <v>1.7</v>
       </c>
-      <c r="Q56" s="64">
+      <c r="Q56" s="63">
         <f>VLOOKUP($E56,'538'!$B$4:$F$35,5,0)</f>
         <v>0.9</v>
       </c>
-      <c r="R56" s="26">
+      <c r="R56" s="24">
         <f>VLOOKUP($D56,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.3</v>
       </c>
-      <c r="S56" s="8">
+      <c r="S56" s="12">
         <f>VLOOKUP($D56,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="T56" s="8">
+      <c r="T56" s="12">
         <f>VLOOKUP($D56,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>3.7</v>
       </c>
-      <c r="U56" s="26">
+      <c r="U56" s="24">
         <f>VLOOKUP($E56,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>1.3</v>
       </c>
-      <c r="V56" s="8">
+      <c r="V56" s="12">
         <f>VLOOKUP($E56,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="W56" s="8">
+      <c r="W56" s="12">
         <f>VLOOKUP($E56,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>1.9</v>
       </c>
-      <c r="X56" s="26">
+      <c r="X56" s="24">
         <f>VLOOKUP($D56,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>17</v>
       </c>
-      <c r="Y56" s="102">
+      <c r="Y56" s="101">
         <f>VLOOKUP($D56,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>13</v>
       </c>
-      <c r="Z56" s="27">
+      <c r="Z56" s="25">
         <f>VLOOKUP($D56,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AA56" s="26">
+      <c r="AA56" s="24">
         <f>VLOOKUP($E56,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>44</v>
       </c>
-      <c r="AB56" s="102">
+      <c r="AB56" s="101">
         <f>VLOOKUP($E56,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="AC56" s="27">
+      <c r="AC56" s="25">
         <f>VLOOKUP($E56,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>16</v>
       </c>
@@ -12382,20 +12390,34 @@
         <v>8</v>
       </c>
       <c r="AG56" s="183">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH56" s="184">
         <v>0</v>
       </c>
       <c r="AI56" s="151">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AJ56" s="156"/>
-      <c r="AK56" s="157"/>
-      <c r="AL56" s="158"/>
+        <v>2</v>
+      </c>
+      <c r="AJ56" s="156">
+        <v>1.99</v>
+      </c>
+      <c r="AK56" s="157">
+        <v>1.05</v>
+      </c>
+      <c r="AL56" s="158">
+        <v>0.81</v>
+      </c>
       <c r="AM56" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="AO56" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="AP56" s="2">
+        <f t="shared" si="11"/>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="2:42">
@@ -12403,104 +12425,104 @@
         <f t="shared" si="9"/>
         <v>54</v>
       </c>
-      <c r="C57" s="48">
+      <c r="C57" s="47">
         <v>41820</v>
       </c>
-      <c r="D57" s="53" t="s">
+      <c r="D57" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="E57" s="58" t="s">
+      <c r="E57" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="F57" s="26">
+      <c r="F57" s="24">
         <v>82</v>
       </c>
-      <c r="G57" s="8">
+      <c r="G57" s="12">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="H57" s="27" t="s">
+      <c r="H57" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I57" s="37">
+      <c r="I57" s="35">
         <v>87.1</v>
       </c>
-      <c r="J57" s="9" t="s">
+      <c r="J57" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K57" s="38">
+      <c r="K57" s="36">
         <f t="shared" si="4"/>
         <v>12.900000000000006</v>
       </c>
-      <c r="L57" s="37">
+      <c r="L57" s="35">
         <f>VLOOKUP($D57,'538'!$B$4:$F$35,3,0)</f>
         <v>88.9</v>
       </c>
-      <c r="M57" s="9">
+      <c r="M57" s="13">
         <f>VLOOKUP($D57,'538'!$B$4:$F$35,4,0)</f>
         <v>3.2</v>
       </c>
-      <c r="N57" s="38">
+      <c r="N57" s="36">
         <f>VLOOKUP($D57,'538'!$B$4:$F$35,5,0)</f>
         <v>0.8</v>
       </c>
-      <c r="O57" s="19">
+      <c r="O57" s="18">
         <f>VLOOKUP($E57,'538'!$B$4:$F$35,3,0)</f>
         <v>63.4</v>
       </c>
-      <c r="P57" s="9">
+      <c r="P57" s="13">
         <f>VLOOKUP($E57,'538'!$B$4:$F$35,4,0)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q57" s="64">
+      <c r="Q57" s="63">
         <f>VLOOKUP($E57,'538'!$B$4:$F$35,5,0)</f>
         <v>1.2</v>
       </c>
-      <c r="R57" s="26">
+      <c r="R57" s="24">
         <f>VLOOKUP($D57,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="S57" s="8">
+      <c r="S57" s="12">
         <f>VLOOKUP($D57,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5</v>
       </c>
-      <c r="T57" s="8">
+      <c r="T57" s="12">
         <f>VLOOKUP($D57,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="U57" s="26">
+      <c r="U57" s="24">
         <f>VLOOKUP($E57,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>1.4</v>
       </c>
-      <c r="V57" s="8">
+      <c r="V57" s="12">
         <f>VLOOKUP($E57,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>1.3</v>
       </c>
-      <c r="W57" s="8">
+      <c r="W57" s="12">
         <f>VLOOKUP($E57,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>1.3</v>
       </c>
-      <c r="X57" s="26">
+      <c r="X57" s="24">
         <f>VLOOKUP($D57,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="Y57" s="102">
+      <c r="Y57" s="101">
         <f>VLOOKUP($D57,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>17</v>
       </c>
-      <c r="Z57" s="27">
+      <c r="Z57" s="25">
         <f>VLOOKUP($D57,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AA57" s="26">
+      <c r="AA57" s="24">
         <f>VLOOKUP($E57,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>22</v>
       </c>
-      <c r="AB57" s="102">
+      <c r="AB57" s="101">
         <f>VLOOKUP($E57,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="AC57" s="27">
+      <c r="AC57" s="25">
         <f>VLOOKUP($E57,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>32</v>
       </c>
@@ -12523,11 +12545,25 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ57" s="156"/>
-      <c r="AK57" s="157"/>
-      <c r="AL57" s="158"/>
+      <c r="AJ57" s="156">
+        <v>2.19</v>
+      </c>
+      <c r="AK57" s="157">
+        <v>0.89</v>
+      </c>
+      <c r="AL57" s="158">
+        <v>1.48</v>
+      </c>
       <c r="AM57" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="AO57" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="AP57" s="2">
+        <f t="shared" si="11"/>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="2:42">
@@ -12535,115 +12571,115 @@
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="C58" s="48">
+      <c r="C58" s="47">
         <v>41821</v>
       </c>
-      <c r="D58" s="53" t="s">
+      <c r="D58" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="58" t="s">
+      <c r="E58" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="F58" s="26">
+      <c r="F58" s="24">
         <v>75</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G58" s="12">
         <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="H58" s="27" t="s">
+      <c r="H58" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I58" s="37">
+      <c r="I58" s="35">
         <v>77.7</v>
       </c>
-      <c r="J58" s="9" t="s">
+      <c r="J58" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K58" s="38">
+      <c r="K58" s="36">
         <f t="shared" si="4"/>
         <v>22.299999999999997</v>
       </c>
-      <c r="L58" s="37">
+      <c r="L58" s="35">
         <f>VLOOKUP($D58,'538'!$B$4:$F$35,3,0)</f>
         <v>90</v>
       </c>
-      <c r="M58" s="9">
+      <c r="M58" s="13">
         <f>VLOOKUP($D58,'538'!$B$4:$F$35,4,0)</f>
         <v>2.9</v>
       </c>
-      <c r="N58" s="38">
+      <c r="N58" s="36">
         <f>VLOOKUP($D58,'538'!$B$4:$F$35,5,0)</f>
         <v>0.4</v>
       </c>
-      <c r="O58" s="19">
+      <c r="O58" s="18">
         <f>VLOOKUP($E58,'538'!$B$4:$F$35,3,0)</f>
         <v>78</v>
       </c>
-      <c r="P58" s="9">
+      <c r="P58" s="13">
         <f>VLOOKUP($E58,'538'!$B$4:$F$35,4,0)</f>
         <v>2</v>
       </c>
-      <c r="Q58" s="64">
+      <c r="Q58" s="63">
         <f>VLOOKUP($E58,'538'!$B$4:$F$35,5,0)</f>
         <v>0.9</v>
       </c>
-      <c r="R58" s="26">
+      <c r="R58" s="24">
         <f>VLOOKUP($D58,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="S58" s="8">
+      <c r="S58" s="12">
         <f>VLOOKUP($D58,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5</v>
       </c>
-      <c r="T58" s="8">
+      <c r="T58" s="12">
         <f>VLOOKUP($D58,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.7</v>
       </c>
-      <c r="U58" s="26">
+      <c r="U58" s="24">
         <f>VLOOKUP($E58,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>1.9</v>
       </c>
-      <c r="V58" s="8">
+      <c r="V58" s="12">
         <f>VLOOKUP($E58,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>2.6</v>
       </c>
-      <c r="W58" s="8">
+      <c r="W58" s="12">
         <f>VLOOKUP($E58,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="X58" s="26">
+      <c r="X58" s="24">
         <f>VLOOKUP($D58,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="Y58" s="102">
+      <c r="Y58" s="101">
         <f>VLOOKUP($D58,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="Z58" s="27">
+      <c r="Z58" s="25">
         <f>VLOOKUP($D58,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AA58" s="26">
+      <c r="AA58" s="24">
         <f>VLOOKUP($E58,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="AB58" s="102">
+      <c r="AB58" s="101">
         <f>VLOOKUP($E58,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="AC58" s="27">
+      <c r="AC58" s="25">
         <f>VLOOKUP($E58,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>8</v>
       </c>
       <c r="AD58" s="173">
-        <v>1.5</v>
+        <v>1.57</v>
       </c>
       <c r="AE58" s="174">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="AF58" s="175">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AG58" s="183">
         <v>0</v>
@@ -12655,11 +12691,25 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ58" s="156"/>
-      <c r="AK58" s="157"/>
-      <c r="AL58" s="158"/>
+      <c r="AJ58" s="156">
+        <v>2.6</v>
+      </c>
+      <c r="AK58" s="157">
+        <v>1.35</v>
+      </c>
+      <c r="AL58" s="158">
+        <v>1.19</v>
+      </c>
       <c r="AM58" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="AO58" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="AP58" s="2">
+        <f t="shared" si="11"/>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="2:42">
@@ -12667,104 +12717,104 @@
         <f t="shared" si="9"/>
         <v>56</v>
       </c>
-      <c r="C59" s="48">
+      <c r="C59" s="47">
         <v>41821</v>
       </c>
-      <c r="D59" s="53" t="s">
+      <c r="D59" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="58" t="s">
+      <c r="E59" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="F59" s="26">
+      <c r="F59" s="24">
         <v>59</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G59" s="12">
         <f t="shared" si="8"/>
         <v>41</v>
       </c>
-      <c r="H59" s="27" t="s">
+      <c r="H59" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I59" s="37">
+      <c r="I59" s="35">
         <v>69.2</v>
       </c>
-      <c r="J59" s="9" t="s">
+      <c r="J59" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K59" s="38">
+      <c r="K59" s="36">
         <f t="shared" si="4"/>
         <v>30.799999999999997</v>
       </c>
-      <c r="L59" s="37">
+      <c r="L59" s="35">
         <f>VLOOKUP($D59,'538'!$B$4:$F$35,3,0)</f>
         <v>82</v>
       </c>
-      <c r="M59" s="9">
+      <c r="M59" s="13">
         <f>VLOOKUP($D59,'538'!$B$4:$F$35,4,0)</f>
         <v>2.1</v>
       </c>
-      <c r="N59" s="38">
+      <c r="N59" s="36">
         <f>VLOOKUP($D59,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="O59" s="19">
+      <c r="O59" s="18">
         <f>VLOOKUP($E59,'538'!$B$4:$F$35,3,0)</f>
         <v>77.400000000000006</v>
       </c>
-      <c r="P59" s="9">
+      <c r="P59" s="13">
         <f>VLOOKUP($E59,'538'!$B$4:$F$35,4,0)</f>
         <v>2</v>
       </c>
-      <c r="Q59" s="64">
+      <c r="Q59" s="63">
         <f>VLOOKUP($E59,'538'!$B$4:$F$35,5,0)</f>
         <v>1</v>
       </c>
-      <c r="R59" s="26">
+      <c r="R59" s="24">
         <f>VLOOKUP($D59,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.6</v>
       </c>
-      <c r="S59" s="8">
+      <c r="S59" s="12">
         <f>VLOOKUP($D59,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="T59" s="8">
+      <c r="T59" s="12">
         <f>VLOOKUP($D59,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.3</v>
       </c>
-      <c r="U59" s="26">
+      <c r="U59" s="24">
         <f>VLOOKUP($E59,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.6</v>
       </c>
-      <c r="V59" s="8">
+      <c r="V59" s="12">
         <f>VLOOKUP($E59,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>1.7</v>
       </c>
-      <c r="W59" s="8">
+      <c r="W59" s="12">
         <f>VLOOKUP($E59,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>2.6</v>
       </c>
-      <c r="X59" s="26">
+      <c r="X59" s="24">
         <f>VLOOKUP($D59,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="Y59" s="102">
+      <c r="Y59" s="101">
         <f>VLOOKUP($D59,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="Z59" s="27">
+      <c r="Z59" s="25">
         <f>VLOOKUP($D59,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="AA59" s="26">
+      <c r="AA59" s="24">
         <f>VLOOKUP($E59,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>13</v>
       </c>
-      <c r="AB59" s="102">
+      <c r="AB59" s="101">
         <f>VLOOKUP($E59,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="AC59" s="27">
+      <c r="AC59" s="25">
         <f>VLOOKUP($E59,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>3</v>
       </c>
@@ -12787,11 +12837,25 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ59" s="156"/>
-      <c r="AK59" s="157"/>
-      <c r="AL59" s="158"/>
+      <c r="AJ59" s="156">
+        <v>1.75</v>
+      </c>
+      <c r="AK59" s="157">
+        <v>0.97</v>
+      </c>
+      <c r="AL59" s="158">
+        <v>0.85</v>
+      </c>
       <c r="AM59" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="AO59" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="AP59" s="2">
+        <f t="shared" si="11"/>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="2:42">
@@ -12799,99 +12863,116 @@
         <f t="shared" si="9"/>
         <v>57</v>
       </c>
-      <c r="C60" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="D60" s="53"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="26"/>
+      <c r="C60" s="48">
+        <v>41824</v>
+      </c>
+      <c r="D60" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="26">
+        <v>47</v>
+      </c>
       <c r="G60" s="8">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="H60" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I60" s="37"/>
+      <c r="I60" s="37">
+        <v>30.8</v>
+      </c>
       <c r="J60" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K60" s="38"/>
-      <c r="L60" s="37" t="e">
+      <c r="K60" s="38">
+        <f t="shared" si="4"/>
+        <v>69.2</v>
+      </c>
+      <c r="L60" s="37">
         <f>VLOOKUP($D60,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M60" s="9" t="e">
+        <v>86.1</v>
+      </c>
+      <c r="M60" s="9">
         <f>VLOOKUP($D60,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N60" s="38" t="e">
+        <v>2.5</v>
+      </c>
+      <c r="N60" s="38">
         <f>VLOOKUP($D60,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O60" s="19" t="e">
+        <v>0.6</v>
+      </c>
+      <c r="O60" s="19">
         <f>VLOOKUP($E60,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P60" s="9" t="e">
+        <v>88.9</v>
+      </c>
+      <c r="P60" s="9">
         <f>VLOOKUP($E60,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q60" s="64" t="e">
+        <v>3.2</v>
+      </c>
+      <c r="Q60" s="64">
         <f>VLOOKUP($E60,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R60" s="26" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="R60" s="26">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S60" s="8" t="e">
+        <v>3.3</v>
+      </c>
+      <c r="S60" s="8">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T60" s="8" t="e">
+        <v>4</v>
+      </c>
+      <c r="T60" s="8">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U60" s="26" t="e">
+        <v>3.7</v>
+      </c>
+      <c r="U60" s="26">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V60" s="8" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="V60" s="8">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W60" s="8" t="e">
+        <v>4.5</v>
+      </c>
+      <c r="W60" s="8">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X60" s="26" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="X60" s="26">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y60" s="102" t="e">
+        <v>17</v>
+      </c>
+      <c r="Y60" s="102">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z60" s="27" t="e">
+        <v>13</v>
+      </c>
+      <c r="Z60" s="27">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA60" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="AA60" s="26">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB60" s="102" t="e">
+        <v>2</v>
+      </c>
+      <c r="AB60" s="102">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC60" s="27" t="e">
+        <v>17</v>
+      </c>
+      <c r="AC60" s="27">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD60" s="173"/>
-      <c r="AE60" s="174"/>
-      <c r="AF60" s="175"/>
+        <v>1</v>
+      </c>
+      <c r="AD60" s="173">
+        <v>3</v>
+      </c>
+      <c r="AE60" s="174">
+        <v>3</v>
+      </c>
+      <c r="AF60" s="175">
+        <v>2.5</v>
+      </c>
       <c r="AG60" s="183">
         <v>0</v>
       </c>
@@ -12906,7 +12987,15 @@
       <c r="AK60" s="157"/>
       <c r="AL60" s="158"/>
       <c r="AM60" s="67" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="AO60" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="AP60" s="2">
+        <f t="shared" si="11"/>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="2:42">
@@ -12914,99 +13003,116 @@
         <f t="shared" si="9"/>
         <v>58</v>
       </c>
-      <c r="C61" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="D61" s="53"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="26"/>
+      <c r="C61" s="48">
+        <v>41824</v>
+      </c>
+      <c r="D61" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="26">
+        <v>72</v>
+      </c>
       <c r="G61" s="8">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="H61" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I61" s="37"/>
+      <c r="I61" s="37">
+        <v>71.400000000000006</v>
+      </c>
       <c r="J61" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K61" s="38"/>
-      <c r="L61" s="37" t="e">
+      <c r="K61" s="38">
+        <f t="shared" si="4"/>
+        <v>28.599999999999994</v>
+      </c>
+      <c r="L61" s="37">
         <f>VLOOKUP($D61,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M61" s="9" t="e">
+        <v>91.8</v>
+      </c>
+      <c r="M61" s="9">
         <f>VLOOKUP($D61,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N61" s="38" t="e">
+        <v>3.4</v>
+      </c>
+      <c r="N61" s="38">
         <f>VLOOKUP($D61,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O61" s="19" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="O61" s="19">
         <f>VLOOKUP($E61,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P61" s="9" t="e">
+        <v>85.8</v>
+      </c>
+      <c r="P61" s="9">
         <f>VLOOKUP($E61,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q61" s="64" t="e">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q61" s="64">
         <f>VLOOKUP($E61,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R61" s="26" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="R61" s="26">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S61" s="8" t="e">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="S61" s="8">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T61" s="8" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="T61" s="8">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U61" s="26" t="e">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="U61" s="26">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V61" s="8" t="e">
+        <v>3.9</v>
+      </c>
+      <c r="V61" s="8">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W61" s="8" t="e">
+        <v>4</v>
+      </c>
+      <c r="W61" s="8">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X61" s="26" t="e">
+        <v>4</v>
+      </c>
+      <c r="X61" s="26">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y61" s="102" t="e">
+        <v>3</v>
+      </c>
+      <c r="Y61" s="102">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z61" s="27" t="e">
+        <v>19</v>
+      </c>
+      <c r="Z61" s="27">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA61" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="26">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB61" s="102" t="e">
+        <v>8</v>
+      </c>
+      <c r="AB61" s="102">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC61" s="27" t="e">
+        <v>4</v>
+      </c>
+      <c r="AC61" s="27">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD61" s="173"/>
-      <c r="AE61" s="174"/>
-      <c r="AF61" s="175"/>
+        <v>16</v>
+      </c>
+      <c r="AD61" s="173">
+        <v>1.83</v>
+      </c>
+      <c r="AE61" s="174">
+        <v>3.6</v>
+      </c>
+      <c r="AF61" s="175">
+        <v>4.2</v>
+      </c>
       <c r="AG61" s="183">
         <v>0</v>
       </c>
@@ -13021,7 +13127,11 @@
       <c r="AK61" s="157"/>
       <c r="AL61" s="158"/>
       <c r="AM61" s="67" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="AO61" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="2:42">
@@ -13029,99 +13139,116 @@
         <f t="shared" si="9"/>
         <v>59</v>
       </c>
-      <c r="C62" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="D62" s="53"/>
-      <c r="E62" s="58"/>
-      <c r="F62" s="26"/>
+      <c r="C62" s="48">
+        <v>41825</v>
+      </c>
+      <c r="D62" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" s="26">
+        <v>72</v>
+      </c>
       <c r="G62" s="8">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="H62" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I62" s="37"/>
+      <c r="I62" s="37">
+        <v>58.2</v>
+      </c>
       <c r="J62" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K62" s="38"/>
-      <c r="L62" s="37" t="e">
+      <c r="K62" s="38">
+        <f t="shared" si="4"/>
+        <v>41.8</v>
+      </c>
+      <c r="L62" s="37">
         <f>VLOOKUP($D62,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M62" s="9" t="e">
+        <v>90</v>
+      </c>
+      <c r="M62" s="9">
         <f>VLOOKUP($D62,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N62" s="38" t="e">
+        <v>2.9</v>
+      </c>
+      <c r="N62" s="38">
         <f>VLOOKUP($D62,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O62" s="19" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="O62" s="19">
         <f>VLOOKUP($E62,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P62" s="9" t="e">
+        <v>82</v>
+      </c>
+      <c r="P62" s="9">
         <f>VLOOKUP($E62,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q62" s="64" t="e">
+        <v>2.1</v>
+      </c>
+      <c r="Q62" s="64">
         <f>VLOOKUP($E62,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R62" s="26" t="e">
+        <v>0.7</v>
+      </c>
+      <c r="R62" s="26">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S62" s="8" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="S62" s="8">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T62" s="8" t="e">
+        <v>4.5</v>
+      </c>
+      <c r="T62" s="8">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U62" s="26" t="e">
+        <v>4.7</v>
+      </c>
+      <c r="U62" s="26">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V62" s="8" t="e">
+        <v>3.6</v>
+      </c>
+      <c r="V62" s="8">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W62" s="8" t="e">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="W62" s="8">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X62" s="26" t="e">
+        <v>4.3</v>
+      </c>
+      <c r="X62" s="26">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y62" s="102" t="e">
+        <v>5</v>
+      </c>
+      <c r="Y62" s="102">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z62" s="27" t="e">
+        <v>15</v>
+      </c>
+      <c r="Z62" s="27">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA62" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="AA62" s="26">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB62" s="102" t="e">
+        <v>11</v>
+      </c>
+      <c r="AB62" s="102">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC62" s="27" t="e">
+        <v>11</v>
+      </c>
+      <c r="AC62" s="27">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD62" s="173"/>
-      <c r="AE62" s="174"/>
-      <c r="AF62" s="175"/>
+        <v>4</v>
+      </c>
+      <c r="AD62" s="173">
+        <v>2.1</v>
+      </c>
+      <c r="AE62" s="174">
+        <v>3.2</v>
+      </c>
+      <c r="AF62" s="175">
+        <v>3.6</v>
+      </c>
       <c r="AG62" s="183">
         <v>0</v>
       </c>
@@ -13136,7 +13263,11 @@
       <c r="AK62" s="157"/>
       <c r="AL62" s="158"/>
       <c r="AM62" s="67" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="AO62" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="2:42">
@@ -13144,99 +13275,116 @@
         <f t="shared" si="9"/>
         <v>60</v>
       </c>
-      <c r="C63" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="D63" s="53"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="26"/>
+      <c r="C63" s="48">
+        <v>41825</v>
+      </c>
+      <c r="D63" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="F63" s="26">
+        <v>76</v>
+      </c>
       <c r="G63" s="8">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="H63" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I63" s="37"/>
+      <c r="I63" s="37">
+        <v>85.3</v>
+      </c>
       <c r="J63" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="38"/>
-      <c r="L63" s="37" t="e">
+      <c r="K63" s="38">
+        <f t="shared" si="4"/>
+        <v>14.700000000000003</v>
+      </c>
+      <c r="L63" s="37">
         <f>VLOOKUP($D63,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M63" s="9" t="e">
+        <v>82.5</v>
+      </c>
+      <c r="M63" s="9">
         <f>VLOOKUP($D63,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N63" s="38" t="e">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N63" s="38">
         <f>VLOOKUP($D63,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O63" s="19" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="O63" s="19">
         <f>VLOOKUP($E63,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P63" s="9" t="e">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="P63" s="9">
         <f>VLOOKUP($E63,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q63" s="64" t="e">
+        <v>1.3</v>
+      </c>
+      <c r="Q63" s="64">
         <f>VLOOKUP($E63,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R63" s="26" t="e">
+        <v>0.7</v>
+      </c>
+      <c r="R63" s="26">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S63" s="8" t="e">
+        <v>3.9</v>
+      </c>
+      <c r="S63" s="8">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T63" s="8" t="e">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="T63" s="8">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U63" s="26" t="e">
+        <v>4.2</v>
+      </c>
+      <c r="U63" s="26">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V63" s="8" t="e">
+        <v>1.6</v>
+      </c>
+      <c r="V63" s="8">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W63" s="8" t="e">
+        <v>1.2</v>
+      </c>
+      <c r="W63" s="8">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X63" s="26" t="e">
+        <v>1.3</v>
+      </c>
+      <c r="X63" s="26">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y63" s="102" t="e">
+        <v>15</v>
+      </c>
+      <c r="Y63" s="102">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z63" s="27" t="e">
+        <v>9</v>
+      </c>
+      <c r="Z63" s="27">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA63" s="26" t="e">
+        <v>2</v>
+      </c>
+      <c r="AA63" s="26">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB63" s="102" t="e">
+        <v>28</v>
+      </c>
+      <c r="AB63" s="102">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC63" s="27" t="e">
+        <v>3</v>
+      </c>
+      <c r="AC63" s="27">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD63" s="173"/>
-      <c r="AE63" s="174"/>
-      <c r="AF63" s="175"/>
+        <v>16</v>
+      </c>
+      <c r="AD63" s="173">
+        <v>1.5</v>
+      </c>
+      <c r="AE63" s="174">
+        <v>3.8</v>
+      </c>
+      <c r="AF63" s="175">
+        <v>7.5</v>
+      </c>
       <c r="AG63" s="183">
         <v>0</v>
       </c>
@@ -13251,7 +13399,11 @@
       <c r="AK63" s="157"/>
       <c r="AL63" s="158"/>
       <c r="AM63" s="67" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="AO63" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="2:42">
@@ -13733,10 +13885,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI57"/>
+  <dimension ref="A1:AI61"/>
   <sheetViews>
-    <sheetView topLeftCell="M43" workbookViewId="0">
-      <selection activeCell="AI50" sqref="AI50"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20568,103 +20720,103 @@
       </c>
     </row>
     <row r="49" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A49" s="213">
+      <c r="A49" s="201">
         <f>Main!C51</f>
         <v>41816</v>
       </c>
-      <c r="B49" s="214" t="str">
+      <c r="B49" s="202" t="str">
         <f>Main!D51</f>
         <v>S Korea</v>
       </c>
-      <c r="C49" s="215" t="str">
+      <c r="C49" s="203" t="str">
         <f>Main!E51</f>
         <v>Belgium</v>
       </c>
-      <c r="D49" s="219">
+      <c r="D49" s="207">
         <f>Main!F51/(Main!$F51+Main!$G51)*100</f>
         <v>26.027397260273972</v>
       </c>
-      <c r="E49" s="220">
+      <c r="E49" s="208">
         <f>Main!G51/(Main!$F51+Main!$G51)*100</f>
         <v>73.972602739726028</v>
       </c>
-      <c r="F49" s="219">
+      <c r="F49" s="207">
         <f>Main!I51/(Main!$I51+Main!$K51)*100</f>
         <v>15.183246073298431</v>
       </c>
-      <c r="G49" s="221">
+      <c r="G49" s="209">
         <f>Main!K51/(Main!$I51+Main!$K51)*100</f>
         <v>84.816753926701566</v>
       </c>
-      <c r="H49" s="219">
+      <c r="H49" s="207">
         <f>Main!L51</f>
         <v>72.400000000000006</v>
       </c>
-      <c r="I49" s="220">
+      <c r="I49" s="208">
         <f>Main!M51</f>
         <v>1.7</v>
       </c>
-      <c r="J49" s="221">
+      <c r="J49" s="209">
         <f>Main!N51</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="K49" s="222">
+      <c r="K49" s="210">
         <f>Main!O51</f>
         <v>82</v>
       </c>
-      <c r="L49" s="220">
+      <c r="L49" s="208">
         <f>Main!P51</f>
         <v>2.1</v>
       </c>
-      <c r="M49" s="223">
+      <c r="M49" s="211">
         <f>Main!Q51</f>
         <v>0.7</v>
       </c>
-      <c r="N49" s="216">
+      <c r="N49" s="204">
         <f>Main!R51</f>
         <v>1.9</v>
       </c>
-      <c r="O49" s="217">
+      <c r="O49" s="205">
         <f>Main!S51</f>
         <v>1.4</v>
       </c>
-      <c r="P49" s="217">
+      <c r="P49" s="205">
         <f>Main!T51</f>
         <v>1.5</v>
       </c>
-      <c r="Q49" s="216">
+      <c r="Q49" s="204">
         <f>Main!U51</f>
         <v>3.6</v>
       </c>
-      <c r="R49" s="217">
+      <c r="R49" s="205">
         <f>Main!V51</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="S49" s="217">
+      <c r="S49" s="205">
         <f>Main!W51</f>
         <v>4.3</v>
       </c>
-      <c r="T49" s="216">
+      <c r="T49" s="204">
         <f>Main!X51</f>
         <v>57</v>
       </c>
-      <c r="U49" s="224">
+      <c r="U49" s="212">
         <f>Main!Y51</f>
         <v>8</v>
       </c>
-      <c r="V49" s="218">
+      <c r="V49" s="206">
         <f>Main!Z51</f>
         <v>4</v>
       </c>
-      <c r="W49" s="216">
+      <c r="W49" s="204">
         <f>Main!AA51</f>
         <v>11</v>
       </c>
-      <c r="X49" s="224">
+      <c r="X49" s="212">
         <f>Main!AB51</f>
         <v>11</v>
       </c>
-      <c r="Y49" s="218">
+      <c r="Y49" s="206">
         <f>Main!AC51</f>
         <v>4</v>
       </c>
@@ -21389,7 +21541,7 @@
       </c>
       <c r="AC54" s="183">
         <f>Main!AG56</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD54" s="184">
         <f>Main!AH56</f>
@@ -21397,23 +21549,23 @@
       </c>
       <c r="AE54" s="151">
         <f>Main!AI56</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF54" s="156">
         <f>Main!AJ56</f>
-        <v>0</v>
+        <v>1.99</v>
       </c>
       <c r="AG54" s="157">
         <f>Main!AK56</f>
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="AH54" s="158">
         <f>Main!AL56</f>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="AI54" s="188" t="str">
         <f>Main!AM56</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="55" spans="1:35">
@@ -21543,19 +21695,19 @@
       </c>
       <c r="AF55" s="156">
         <f>Main!AJ57</f>
-        <v>0</v>
+        <v>2.19</v>
       </c>
       <c r="AG55" s="157">
         <f>Main!AK57</f>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="AH55" s="158">
         <f>Main!AL57</f>
-        <v>0</v>
+        <v>1.48</v>
       </c>
       <c r="AI55" s="188" t="str">
         <f>Main!AM57</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="56" spans="1:35">
@@ -21661,15 +21813,15 @@
       </c>
       <c r="Z56" s="173">
         <f>Main!AD58</f>
-        <v>1.5</v>
+        <v>1.57</v>
       </c>
       <c r="AA56" s="174">
         <f>Main!AE58</f>
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="AB56" s="175">
         <f>Main!AF58</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AC56" s="183">
         <f>Main!AG58</f>
@@ -21685,19 +21837,19 @@
       </c>
       <c r="AF56" s="156">
         <f>Main!AJ58</f>
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="AG56" s="157">
         <f>Main!AK58</f>
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="AH56" s="158">
         <f>Main!AL58</f>
-        <v>0</v>
+        <v>1.19</v>
       </c>
       <c r="AI56" s="188" t="str">
         <f>Main!AM58</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="57" spans="1:35">
@@ -21827,18 +21979,586 @@
       </c>
       <c r="AF57" s="156">
         <f>Main!AJ59</f>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="AG57" s="157">
         <f>Main!AK59</f>
-        <v>0</v>
+        <v>0.97</v>
       </c>
       <c r="AH57" s="158">
         <f>Main!AL59</f>
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="AI57" s="188" t="str">
         <f>Main!AM59</f>
+        <v>train</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35">
+      <c r="A58" s="48">
+        <f>Main!C60</f>
+        <v>41824</v>
+      </c>
+      <c r="B58" s="53" t="str">
+        <f>Main!D60</f>
+        <v>France</v>
+      </c>
+      <c r="C58" s="58" t="str">
+        <f>Main!E60</f>
+        <v>Germany</v>
+      </c>
+      <c r="D58" s="37">
+        <f>Main!F60/(Main!$F60+Main!$G60)*100</f>
+        <v>47</v>
+      </c>
+      <c r="E58" s="9">
+        <f>Main!G60/(Main!$F60+Main!$G60)*100</f>
+        <v>53</v>
+      </c>
+      <c r="F58" s="37">
+        <f>Main!I60/(Main!$I60+Main!$K60)*100</f>
+        <v>30.8</v>
+      </c>
+      <c r="G58" s="38">
+        <f>Main!K60/(Main!$I60+Main!$K60)*100</f>
+        <v>69.2</v>
+      </c>
+      <c r="H58" s="37">
+        <f>Main!L60</f>
+        <v>86.1</v>
+      </c>
+      <c r="I58" s="9">
+        <f>Main!M60</f>
+        <v>2.5</v>
+      </c>
+      <c r="J58" s="38">
+        <f>Main!N60</f>
+        <v>0.6</v>
+      </c>
+      <c r="K58" s="19">
+        <f>Main!O60</f>
+        <v>88.9</v>
+      </c>
+      <c r="L58" s="9">
+        <f>Main!P60</f>
+        <v>3.2</v>
+      </c>
+      <c r="M58" s="64">
+        <f>Main!Q60</f>
+        <v>0.8</v>
+      </c>
+      <c r="N58" s="26">
+        <f>Main!R60</f>
+        <v>3.3</v>
+      </c>
+      <c r="O58" s="8">
+        <f>Main!S60</f>
+        <v>4</v>
+      </c>
+      <c r="P58" s="8">
+        <f>Main!T60</f>
+        <v>3.7</v>
+      </c>
+      <c r="Q58" s="26">
+        <f>Main!U60</f>
+        <v>4.8</v>
+      </c>
+      <c r="R58" s="8">
+        <f>Main!V60</f>
+        <v>4.5</v>
+      </c>
+      <c r="S58" s="8">
+        <f>Main!W60</f>
+        <v>4.8</v>
+      </c>
+      <c r="T58" s="26">
+        <f>Main!X60</f>
+        <v>17</v>
+      </c>
+      <c r="U58" s="102">
+        <f>Main!Y60</f>
+        <v>13</v>
+      </c>
+      <c r="V58" s="27">
+        <f>Main!Z60</f>
+        <v>1</v>
+      </c>
+      <c r="W58" s="26">
+        <f>Main!AA60</f>
+        <v>2</v>
+      </c>
+      <c r="X58" s="102">
+        <f>Main!AB60</f>
+        <v>17</v>
+      </c>
+      <c r="Y58" s="27">
+        <f>Main!AC60</f>
+        <v>1</v>
+      </c>
+      <c r="Z58" s="173">
+        <f>Main!AD60</f>
+        <v>3</v>
+      </c>
+      <c r="AA58" s="174">
+        <f>Main!AE60</f>
+        <v>3</v>
+      </c>
+      <c r="AB58" s="175">
+        <f>Main!AF60</f>
+        <v>2.5</v>
+      </c>
+      <c r="AC58" s="183">
+        <f>Main!AG60</f>
+        <v>0</v>
+      </c>
+      <c r="AD58" s="184">
+        <f>Main!AH60</f>
+        <v>0</v>
+      </c>
+      <c r="AE58" s="151">
+        <f>Main!AI60</f>
+        <v>0</v>
+      </c>
+      <c r="AF58" s="156">
+        <f>Main!AJ60</f>
+        <v>0</v>
+      </c>
+      <c r="AG58" s="157">
+        <f>Main!AK60</f>
+        <v>0</v>
+      </c>
+      <c r="AH58" s="158">
+        <f>Main!AL60</f>
+        <v>0</v>
+      </c>
+      <c r="AI58" s="188" t="str">
+        <f>Main!AM60</f>
+        <v>predict</v>
+      </c>
+    </row>
+    <row r="59" spans="1:35">
+      <c r="A59" s="48">
+        <f>Main!C61</f>
+        <v>41824</v>
+      </c>
+      <c r="B59" s="53" t="str">
+        <f>Main!D61</f>
+        <v>Brazil</v>
+      </c>
+      <c r="C59" s="58" t="str">
+        <f>Main!E61</f>
+        <v>Colombia</v>
+      </c>
+      <c r="D59" s="37">
+        <f>Main!F61/(Main!$F61+Main!$G61)*100</f>
+        <v>72</v>
+      </c>
+      <c r="E59" s="9">
+        <f>Main!G61/(Main!$F61+Main!$G61)*100</f>
+        <v>28.000000000000004</v>
+      </c>
+      <c r="F59" s="37">
+        <f>Main!I61/(Main!$I61+Main!$K61)*100</f>
+        <v>71.400000000000006</v>
+      </c>
+      <c r="G59" s="38">
+        <f>Main!K61/(Main!$I61+Main!$K61)*100</f>
+        <v>28.599999999999991</v>
+      </c>
+      <c r="H59" s="37">
+        <f>Main!L61</f>
+        <v>91.8</v>
+      </c>
+      <c r="I59" s="9">
+        <f>Main!M61</f>
+        <v>3.4</v>
+      </c>
+      <c r="J59" s="38">
+        <f>Main!N61</f>
+        <v>0.5</v>
+      </c>
+      <c r="K59" s="19">
+        <f>Main!O61</f>
+        <v>85.8</v>
+      </c>
+      <c r="L59" s="9">
+        <f>Main!P61</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M59" s="64">
+        <f>Main!Q61</f>
+        <v>0.5</v>
+      </c>
+      <c r="N59" s="26">
+        <f>Main!R61</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="O59" s="8">
+        <f>Main!S61</f>
+        <v>4.8</v>
+      </c>
+      <c r="P59" s="8">
+        <f>Main!T61</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q59" s="26">
+        <f>Main!U61</f>
+        <v>3.9</v>
+      </c>
+      <c r="R59" s="8">
+        <f>Main!V61</f>
+        <v>4</v>
+      </c>
+      <c r="S59" s="8">
+        <f>Main!W61</f>
+        <v>4</v>
+      </c>
+      <c r="T59" s="26">
+        <f>Main!X61</f>
+        <v>3</v>
+      </c>
+      <c r="U59" s="102">
+        <f>Main!Y61</f>
+        <v>19</v>
+      </c>
+      <c r="V59" s="27">
+        <f>Main!Z61</f>
+        <v>1</v>
+      </c>
+      <c r="W59" s="26">
+        <f>Main!AA61</f>
+        <v>8</v>
+      </c>
+      <c r="X59" s="102">
+        <f>Main!AB61</f>
+        <v>4</v>
+      </c>
+      <c r="Y59" s="27">
+        <f>Main!AC61</f>
+        <v>16</v>
+      </c>
+      <c r="Z59" s="173">
+        <f>Main!AD61</f>
+        <v>1.83</v>
+      </c>
+      <c r="AA59" s="174">
+        <f>Main!AE61</f>
+        <v>3.6</v>
+      </c>
+      <c r="AB59" s="175">
+        <f>Main!AF61</f>
+        <v>4.2</v>
+      </c>
+      <c r="AC59" s="183">
+        <f>Main!AG61</f>
+        <v>0</v>
+      </c>
+      <c r="AD59" s="184">
+        <f>Main!AH61</f>
+        <v>0</v>
+      </c>
+      <c r="AE59" s="151">
+        <f>Main!AI61</f>
+        <v>0</v>
+      </c>
+      <c r="AF59" s="156">
+        <f>Main!AJ61</f>
+        <v>0</v>
+      </c>
+      <c r="AG59" s="157">
+        <f>Main!AK61</f>
+        <v>0</v>
+      </c>
+      <c r="AH59" s="158">
+        <f>Main!AL61</f>
+        <v>0</v>
+      </c>
+      <c r="AI59" s="188" t="str">
+        <f>Main!AM61</f>
+        <v>predict</v>
+      </c>
+    </row>
+    <row r="60" spans="1:35">
+      <c r="A60" s="48">
+        <f>Main!C62</f>
+        <v>41825</v>
+      </c>
+      <c r="B60" s="53" t="str">
+        <f>Main!D62</f>
+        <v>Argentina</v>
+      </c>
+      <c r="C60" s="58" t="str">
+        <f>Main!E62</f>
+        <v>Belgium</v>
+      </c>
+      <c r="D60" s="37">
+        <f>Main!F62/(Main!$F62+Main!$G62)*100</f>
+        <v>72</v>
+      </c>
+      <c r="E60" s="9">
+        <f>Main!G62/(Main!$F62+Main!$G62)*100</f>
+        <v>28.000000000000004</v>
+      </c>
+      <c r="F60" s="37">
+        <f>Main!I62/(Main!$I62+Main!$K62)*100</f>
+        <v>58.20000000000001</v>
+      </c>
+      <c r="G60" s="38">
+        <f>Main!K62/(Main!$I62+Main!$K62)*100</f>
+        <v>41.8</v>
+      </c>
+      <c r="H60" s="37">
+        <f>Main!L62</f>
+        <v>90</v>
+      </c>
+      <c r="I60" s="9">
+        <f>Main!M62</f>
+        <v>2.9</v>
+      </c>
+      <c r="J60" s="38">
+        <f>Main!N62</f>
+        <v>0.4</v>
+      </c>
+      <c r="K60" s="19">
+        <f>Main!O62</f>
+        <v>82</v>
+      </c>
+      <c r="L60" s="9">
+        <f>Main!P62</f>
+        <v>2.1</v>
+      </c>
+      <c r="M60" s="64">
+        <f>Main!Q62</f>
+        <v>0.7</v>
+      </c>
+      <c r="N60" s="26">
+        <f>Main!R62</f>
+        <v>4.8</v>
+      </c>
+      <c r="O60" s="8">
+        <f>Main!S62</f>
+        <v>4.5</v>
+      </c>
+      <c r="P60" s="8">
+        <f>Main!T62</f>
+        <v>4.7</v>
+      </c>
+      <c r="Q60" s="26">
+        <f>Main!U62</f>
+        <v>3.6</v>
+      </c>
+      <c r="R60" s="8">
+        <f>Main!V62</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="S60" s="8">
+        <f>Main!W62</f>
+        <v>4.3</v>
+      </c>
+      <c r="T60" s="26">
+        <f>Main!X62</f>
+        <v>5</v>
+      </c>
+      <c r="U60" s="102">
+        <f>Main!Y62</f>
+        <v>15</v>
+      </c>
+      <c r="V60" s="27">
+        <f>Main!Z62</f>
+        <v>1</v>
+      </c>
+      <c r="W60" s="26">
+        <f>Main!AA62</f>
+        <v>11</v>
+      </c>
+      <c r="X60" s="102">
+        <f>Main!AB62</f>
+        <v>11</v>
+      </c>
+      <c r="Y60" s="27">
+        <f>Main!AC62</f>
+        <v>4</v>
+      </c>
+      <c r="Z60" s="173">
+        <f>Main!AD62</f>
+        <v>2.1</v>
+      </c>
+      <c r="AA60" s="174">
+        <f>Main!AE62</f>
+        <v>3.2</v>
+      </c>
+      <c r="AB60" s="175">
+        <f>Main!AF62</f>
+        <v>3.6</v>
+      </c>
+      <c r="AC60" s="183">
+        <f>Main!AG62</f>
+        <v>0</v>
+      </c>
+      <c r="AD60" s="184">
+        <f>Main!AH62</f>
+        <v>0</v>
+      </c>
+      <c r="AE60" s="151">
+        <f>Main!AI62</f>
+        <v>0</v>
+      </c>
+      <c r="AF60" s="156">
+        <f>Main!AJ62</f>
+        <v>0</v>
+      </c>
+      <c r="AG60" s="157">
+        <f>Main!AK62</f>
+        <v>0</v>
+      </c>
+      <c r="AH60" s="158">
+        <f>Main!AL62</f>
+        <v>0</v>
+      </c>
+      <c r="AI60" s="188" t="str">
+        <f>Main!AM62</f>
+        <v>predict</v>
+      </c>
+    </row>
+    <row r="61" spans="1:35">
+      <c r="A61" s="48">
+        <f>Main!C63</f>
+        <v>41825</v>
+      </c>
+      <c r="B61" s="53" t="str">
+        <f>Main!D63</f>
+        <v>Netherlands</v>
+      </c>
+      <c r="C61" s="58" t="str">
+        <f>Main!E63</f>
+        <v>Costa Rica</v>
+      </c>
+      <c r="D61" s="37">
+        <f>Main!F63/(Main!$F63+Main!$G63)*100</f>
+        <v>76</v>
+      </c>
+      <c r="E61" s="9">
+        <f>Main!G63/(Main!$F63+Main!$G63)*100</f>
+        <v>24</v>
+      </c>
+      <c r="F61" s="37">
+        <f>Main!I63/(Main!$I63+Main!$K63)*100</f>
+        <v>85.3</v>
+      </c>
+      <c r="G61" s="38">
+        <f>Main!K63/(Main!$I63+Main!$K63)*100</f>
+        <v>14.700000000000003</v>
+      </c>
+      <c r="H61" s="37">
+        <f>Main!L63</f>
+        <v>82.5</v>
+      </c>
+      <c r="I61" s="9">
+        <f>Main!M63</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J61" s="38">
+        <f>Main!N63</f>
+        <v>0.8</v>
+      </c>
+      <c r="K61" s="19">
+        <f>Main!O63</f>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="L61" s="9">
+        <f>Main!P63</f>
+        <v>1.3</v>
+      </c>
+      <c r="M61" s="64">
+        <f>Main!Q63</f>
+        <v>0.7</v>
+      </c>
+      <c r="N61" s="26">
+        <f>Main!R63</f>
+        <v>3.9</v>
+      </c>
+      <c r="O61" s="8">
+        <f>Main!S63</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P61" s="8">
+        <f>Main!T63</f>
+        <v>4.2</v>
+      </c>
+      <c r="Q61" s="26">
+        <f>Main!U63</f>
+        <v>1.6</v>
+      </c>
+      <c r="R61" s="8">
+        <f>Main!V63</f>
+        <v>1.2</v>
+      </c>
+      <c r="S61" s="8">
+        <f>Main!W63</f>
+        <v>1.3</v>
+      </c>
+      <c r="T61" s="26">
+        <f>Main!X63</f>
+        <v>15</v>
+      </c>
+      <c r="U61" s="102">
+        <f>Main!Y63</f>
+        <v>9</v>
+      </c>
+      <c r="V61" s="27">
+        <f>Main!Z63</f>
+        <v>2</v>
+      </c>
+      <c r="W61" s="26">
+        <f>Main!AA63</f>
+        <v>28</v>
+      </c>
+      <c r="X61" s="102">
+        <f>Main!AB63</f>
+        <v>3</v>
+      </c>
+      <c r="Y61" s="27">
+        <f>Main!AC63</f>
+        <v>16</v>
+      </c>
+      <c r="Z61" s="173">
+        <f>Main!AD63</f>
+        <v>1.5</v>
+      </c>
+      <c r="AA61" s="174">
+        <f>Main!AE63</f>
+        <v>3.8</v>
+      </c>
+      <c r="AB61" s="175">
+        <f>Main!AF63</f>
+        <v>7.5</v>
+      </c>
+      <c r="AC61" s="183">
+        <f>Main!AG63</f>
+        <v>0</v>
+      </c>
+      <c r="AD61" s="184">
+        <f>Main!AH63</f>
+        <v>0</v>
+      </c>
+      <c r="AE61" s="151">
+        <f>Main!AI63</f>
+        <v>0</v>
+      </c>
+      <c r="AF61" s="156">
+        <f>Main!AJ63</f>
+        <v>0</v>
+      </c>
+      <c r="AG61" s="157">
+        <f>Main!AK63</f>
+        <v>0</v>
+      </c>
+      <c r="AH61" s="158">
+        <f>Main!AL63</f>
+        <v>0</v>
+      </c>
+      <c r="AI61" s="188" t="str">
+        <f>Main!AM63</f>
         <v>predict</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added predictions for 5 July
</commit_message>
<xml_diff>
--- a/data/data_wc2014.xlsx
+++ b/data/data_wc2014.xlsx
@@ -4445,10 +4445,10 @@
   <dimension ref="A1:AMP67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J63" sqref="J63"/>
+      <selection pane="bottomRight" activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12977,17 +12977,23 @@
         <v>0</v>
       </c>
       <c r="AH60" s="184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI60" s="151">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AJ60" s="156"/>
-      <c r="AK60" s="157"/>
-      <c r="AL60" s="158"/>
+        <v>-1</v>
+      </c>
+      <c r="AJ60" s="156">
+        <v>0.88</v>
+      </c>
+      <c r="AK60" s="157">
+        <v>1.71</v>
+      </c>
+      <c r="AL60" s="158">
+        <v>-0.72</v>
+      </c>
       <c r="AM60" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO60" s="2">
         <f t="shared" si="10"/>
@@ -13114,20 +13120,26 @@
         <v>4.2</v>
       </c>
       <c r="AG61" s="183">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH61" s="184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI61" s="151">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AJ61" s="156"/>
-      <c r="AK61" s="157"/>
-      <c r="AL61" s="158"/>
+        <v>1</v>
+      </c>
+      <c r="AJ61" s="156">
+        <v>1.44</v>
+      </c>
+      <c r="AK61" s="157">
+        <v>0.91</v>
+      </c>
+      <c r="AL61" s="158">
+        <v>0.61</v>
+      </c>
       <c r="AM61" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO61" s="2">
         <f t="shared" si="10"/>
@@ -13244,10 +13256,10 @@
         <v>2.1</v>
       </c>
       <c r="AE62" s="174">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="AF62" s="175">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="AG62" s="183">
         <v>0</v>
@@ -13259,9 +13271,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ62" s="156"/>
-      <c r="AK62" s="157"/>
-      <c r="AL62" s="158"/>
+      <c r="AJ62" s="156">
+        <v>1.78</v>
+      </c>
+      <c r="AK62" s="157">
+        <v>1.07</v>
+      </c>
+      <c r="AL62" s="158">
+        <v>0.24</v>
+      </c>
       <c r="AM62" s="67" t="s">
         <v>62</v>
       </c>
@@ -13377,13 +13395,13 @@
         <v>16</v>
       </c>
       <c r="AD63" s="173">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
       <c r="AE63" s="174">
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="AF63" s="175">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="AG63" s="183">
         <v>0</v>
@@ -13395,9 +13413,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ63" s="156"/>
-      <c r="AK63" s="157"/>
-      <c r="AL63" s="158"/>
+      <c r="AJ63" s="156">
+        <v>1.29</v>
+      </c>
+      <c r="AK63" s="157">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AL63" s="158">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="AM63" s="67" t="s">
         <v>62</v>
       </c>
@@ -22113,27 +22137,27 @@
       </c>
       <c r="AD58" s="184">
         <f>Main!AH60</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE58" s="151">
         <f>Main!AI60</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AF58" s="156">
         <f>Main!AJ60</f>
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="AG58" s="157">
         <f>Main!AK60</f>
-        <v>0</v>
+        <v>1.71</v>
       </c>
       <c r="AH58" s="158">
         <f>Main!AL60</f>
-        <v>0</v>
+        <v>-0.72</v>
       </c>
       <c r="AI58" s="188" t="str">
         <f>Main!AM60</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="59" spans="1:35">
@@ -22251,31 +22275,31 @@
       </c>
       <c r="AC59" s="183">
         <f>Main!AG61</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD59" s="184">
         <f>Main!AH61</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE59" s="151">
         <f>Main!AI61</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF59" s="156">
         <f>Main!AJ61</f>
-        <v>0</v>
+        <v>1.44</v>
       </c>
       <c r="AG59" s="157">
         <f>Main!AK61</f>
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="AH59" s="158">
         <f>Main!AL61</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="AI59" s="188" t="str">
         <f>Main!AM61</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="60" spans="1:35">
@@ -22385,11 +22409,11 @@
       </c>
       <c r="AA60" s="174">
         <f>Main!AE62</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="AB60" s="175">
         <f>Main!AF62</f>
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="AC60" s="183">
         <f>Main!AG62</f>
@@ -22405,15 +22429,15 @@
       </c>
       <c r="AF60" s="156">
         <f>Main!AJ62</f>
-        <v>0</v>
+        <v>1.78</v>
       </c>
       <c r="AG60" s="157">
         <f>Main!AK62</f>
-        <v>0</v>
+        <v>1.07</v>
       </c>
       <c r="AH60" s="158">
         <f>Main!AL62</f>
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="AI60" s="188" t="str">
         <f>Main!AM62</f>
@@ -22523,15 +22547,15 @@
       </c>
       <c r="Z61" s="173">
         <f>Main!AD63</f>
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
       <c r="AA61" s="174">
         <f>Main!AE63</f>
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="AB61" s="175">
         <f>Main!AF63</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="AC61" s="183">
         <f>Main!AG63</f>
@@ -22547,15 +22571,15 @@
       </c>
       <c r="AF61" s="156">
         <f>Main!AJ63</f>
-        <v>0</v>
+        <v>1.29</v>
       </c>
       <c r="AG61" s="157">
         <f>Main!AK63</f>
-        <v>0</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="AH61" s="158">
         <f>Main!AL63</f>
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI61" s="188" t="str">
         <f>Main!AM63</f>

</xml_diff>

<commit_message>
Predictions for 8 July
</commit_message>
<xml_diff>
--- a/data/data_wc2014.xlsx
+++ b/data/data_wc2014.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="99">
   <si>
     <t>Team</t>
   </si>
@@ -4445,10 +4445,10 @@
   <dimension ref="A1:AMP67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="AB40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G63" sqref="G63"/>
+      <selection pane="bottomRight" activeCell="AF66" sqref="AF66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11721,7 +11721,7 @@
         <v>97</v>
       </c>
       <c r="K52" s="221">
-        <f t="shared" ref="K52:K63" si="4">100-I52</f>
+        <f t="shared" ref="K52:K65" si="4">100-I52</f>
         <v>18.900000000000006</v>
       </c>
       <c r="L52" s="219">
@@ -12266,7 +12266,7 @@
         <v>61</v>
       </c>
       <c r="AO55" s="2">
-        <f t="shared" ref="AO55:AO63" si="10">SUM(F55:H55)</f>
+        <f t="shared" ref="AO55:AO65" si="10">SUM(F55:H55)</f>
         <v>100</v>
       </c>
       <c r="AP55" s="2">
@@ -12863,104 +12863,104 @@
         <f t="shared" si="9"/>
         <v>57</v>
       </c>
-      <c r="C60" s="48">
+      <c r="C60" s="47">
         <v>41824</v>
       </c>
-      <c r="D60" s="53" t="s">
+      <c r="D60" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E60" s="58" t="s">
+      <c r="E60" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="26">
+      <c r="F60" s="24">
         <v>47</v>
       </c>
-      <c r="G60" s="8">
+      <c r="G60" s="12">
         <f t="shared" si="8"/>
         <v>53</v>
       </c>
-      <c r="H60" s="27" t="s">
+      <c r="H60" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I60" s="37">
+      <c r="I60" s="35">
         <v>30.8</v>
       </c>
-      <c r="J60" s="9" t="s">
+      <c r="J60" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K60" s="38">
+      <c r="K60" s="36">
         <f t="shared" si="4"/>
         <v>69.2</v>
       </c>
-      <c r="L60" s="37">
+      <c r="L60" s="35">
         <f>VLOOKUP($D60,'538'!$B$4:$F$35,3,0)</f>
         <v>86.1</v>
       </c>
-      <c r="M60" s="9">
+      <c r="M60" s="13">
         <f>VLOOKUP($D60,'538'!$B$4:$F$35,4,0)</f>
         <v>2.5</v>
       </c>
-      <c r="N60" s="38">
+      <c r="N60" s="36">
         <f>VLOOKUP($D60,'538'!$B$4:$F$35,5,0)</f>
         <v>0.6</v>
       </c>
-      <c r="O60" s="19">
+      <c r="O60" s="18">
         <f>VLOOKUP($E60,'538'!$B$4:$F$35,3,0)</f>
         <v>88.9</v>
       </c>
-      <c r="P60" s="9">
+      <c r="P60" s="13">
         <f>VLOOKUP($E60,'538'!$B$4:$F$35,4,0)</f>
         <v>3.2</v>
       </c>
-      <c r="Q60" s="64">
+      <c r="Q60" s="63">
         <f>VLOOKUP($E60,'538'!$B$4:$F$35,5,0)</f>
         <v>0.8</v>
       </c>
-      <c r="R60" s="26">
+      <c r="R60" s="24">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.3</v>
       </c>
-      <c r="S60" s="8">
+      <c r="S60" s="12">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="T60" s="8">
+      <c r="T60" s="12">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>3.7</v>
       </c>
-      <c r="U60" s="26">
+      <c r="U60" s="24">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="V60" s="8">
+      <c r="V60" s="12">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5</v>
       </c>
-      <c r="W60" s="8">
+      <c r="W60" s="12">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="X60" s="26">
+      <c r="X60" s="24">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>17</v>
       </c>
-      <c r="Y60" s="102">
+      <c r="Y60" s="101">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>13</v>
       </c>
-      <c r="Z60" s="27">
+      <c r="Z60" s="25">
         <f>VLOOKUP($D60,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AA60" s="26">
+      <c r="AA60" s="24">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="AB60" s="102">
+      <c r="AB60" s="101">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>17</v>
       </c>
-      <c r="AC60" s="27">
+      <c r="AC60" s="25">
         <f>VLOOKUP($E60,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
@@ -13009,104 +13009,104 @@
         <f t="shared" si="9"/>
         <v>58</v>
       </c>
-      <c r="C61" s="48">
+      <c r="C61" s="47">
         <v>41824</v>
       </c>
-      <c r="D61" s="53" t="s">
+      <c r="D61" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E61" s="58" t="s">
+      <c r="E61" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="26">
+      <c r="F61" s="24">
         <v>72</v>
       </c>
-      <c r="G61" s="8">
+      <c r="G61" s="12">
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="H61" s="27" t="s">
+      <c r="H61" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I61" s="37">
+      <c r="I61" s="35">
         <v>71.400000000000006</v>
       </c>
-      <c r="J61" s="9" t="s">
+      <c r="J61" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K61" s="38">
+      <c r="K61" s="36">
         <f t="shared" si="4"/>
         <v>28.599999999999994</v>
       </c>
-      <c r="L61" s="37">
+      <c r="L61" s="35">
         <f>VLOOKUP($D61,'538'!$B$4:$F$35,3,0)</f>
         <v>91.8</v>
       </c>
-      <c r="M61" s="9">
+      <c r="M61" s="13">
         <f>VLOOKUP($D61,'538'!$B$4:$F$35,4,0)</f>
         <v>3.4</v>
       </c>
-      <c r="N61" s="38">
+      <c r="N61" s="36">
         <f>VLOOKUP($D61,'538'!$B$4:$F$35,5,0)</f>
         <v>0.5</v>
       </c>
-      <c r="O61" s="19">
+      <c r="O61" s="18">
         <f>VLOOKUP($E61,'538'!$B$4:$F$35,3,0)</f>
         <v>85.8</v>
       </c>
-      <c r="P61" s="9">
+      <c r="P61" s="13">
         <f>VLOOKUP($E61,'538'!$B$4:$F$35,4,0)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q61" s="64">
+      <c r="Q61" s="63">
         <f>VLOOKUP($E61,'538'!$B$4:$F$35,5,0)</f>
         <v>0.5</v>
       </c>
-      <c r="R61" s="26">
+      <c r="R61" s="24">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="S61" s="8">
+      <c r="S61" s="12">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="T61" s="8">
+      <c r="T61" s="12">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="U61" s="26">
+      <c r="U61" s="24">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.9</v>
       </c>
-      <c r="V61" s="8">
+      <c r="V61" s="12">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="W61" s="8">
+      <c r="W61" s="12">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="X61" s="26">
+      <c r="X61" s="24">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="Y61" s="102">
+      <c r="Y61" s="101">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="Z61" s="27">
+      <c r="Z61" s="25">
         <f>VLOOKUP($D61,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AA61" s="26">
+      <c r="AA61" s="24">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="AB61" s="102">
+      <c r="AB61" s="101">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="AC61" s="27">
+      <c r="AC61" s="25">
         <f>VLOOKUP($E61,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>16</v>
       </c>
@@ -13151,104 +13151,104 @@
         <f t="shared" si="9"/>
         <v>59</v>
       </c>
-      <c r="C62" s="48">
+      <c r="C62" s="47">
         <v>41825</v>
       </c>
-      <c r="D62" s="53" t="s">
+      <c r="D62" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="58" t="s">
+      <c r="E62" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="F62" s="26">
+      <c r="F62" s="24">
         <v>72</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="12">
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="H62" s="27" t="s">
+      <c r="H62" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I62" s="37">
+      <c r="I62" s="35">
         <v>58.2</v>
       </c>
-      <c r="J62" s="9" t="s">
+      <c r="J62" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K62" s="38">
+      <c r="K62" s="36">
         <f t="shared" si="4"/>
         <v>41.8</v>
       </c>
-      <c r="L62" s="37">
+      <c r="L62" s="35">
         <f>VLOOKUP($D62,'538'!$B$4:$F$35,3,0)</f>
         <v>90</v>
       </c>
-      <c r="M62" s="9">
+      <c r="M62" s="13">
         <f>VLOOKUP($D62,'538'!$B$4:$F$35,4,0)</f>
         <v>2.9</v>
       </c>
-      <c r="N62" s="38">
+      <c r="N62" s="36">
         <f>VLOOKUP($D62,'538'!$B$4:$F$35,5,0)</f>
         <v>0.4</v>
       </c>
-      <c r="O62" s="19">
+      <c r="O62" s="18">
         <f>VLOOKUP($E62,'538'!$B$4:$F$35,3,0)</f>
         <v>82</v>
       </c>
-      <c r="P62" s="9">
+      <c r="P62" s="13">
         <f>VLOOKUP($E62,'538'!$B$4:$F$35,4,0)</f>
         <v>2.1</v>
       </c>
-      <c r="Q62" s="64">
+      <c r="Q62" s="63">
         <f>VLOOKUP($E62,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="R62" s="26">
+      <c r="R62" s="24">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="S62" s="8">
+      <c r="S62" s="12">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5</v>
       </c>
-      <c r="T62" s="8">
+      <c r="T62" s="12">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.7</v>
       </c>
-      <c r="U62" s="26">
+      <c r="U62" s="24">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.6</v>
       </c>
-      <c r="V62" s="8">
+      <c r="V62" s="12">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="W62" s="8">
+      <c r="W62" s="12">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.3</v>
       </c>
-      <c r="X62" s="26">
+      <c r="X62" s="24">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="Y62" s="102">
+      <c r="Y62" s="101">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="Z62" s="27">
+      <c r="Z62" s="25">
         <f>VLOOKUP($D62,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AA62" s="26">
+      <c r="AA62" s="24">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="AB62" s="102">
+      <c r="AB62" s="101">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="AC62" s="27">
+      <c r="AC62" s="25">
         <f>VLOOKUP($E62,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>4</v>
       </c>
@@ -13262,14 +13262,14 @@
         <v>4</v>
       </c>
       <c r="AG62" s="183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH62" s="184">
         <v>0</v>
       </c>
       <c r="AI62" s="151">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ62" s="156">
         <v>1.78</v>
@@ -13281,7 +13281,7 @@
         <v>0.24</v>
       </c>
       <c r="AM62" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO62" s="2">
         <f t="shared" si="10"/>
@@ -13293,104 +13293,104 @@
         <f t="shared" si="9"/>
         <v>60</v>
       </c>
-      <c r="C63" s="48">
+      <c r="C63" s="47">
         <v>41825</v>
       </c>
-      <c r="D63" s="53" t="s">
+      <c r="D63" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="58" t="s">
+      <c r="E63" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="F63" s="26">
+      <c r="F63" s="24">
         <v>76</v>
       </c>
-      <c r="G63" s="8">
+      <c r="G63" s="12">
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="H63" s="27" t="s">
+      <c r="H63" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I63" s="37">
+      <c r="I63" s="35">
         <v>85.3</v>
       </c>
-      <c r="J63" s="9" t="s">
+      <c r="J63" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="38">
+      <c r="K63" s="36">
         <f t="shared" si="4"/>
         <v>14.700000000000003</v>
       </c>
-      <c r="L63" s="37">
+      <c r="L63" s="35">
         <f>VLOOKUP($D63,'538'!$B$4:$F$35,3,0)</f>
         <v>82.5</v>
       </c>
-      <c r="M63" s="9">
+      <c r="M63" s="13">
         <f>VLOOKUP($D63,'538'!$B$4:$F$35,4,0)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="N63" s="38">
+      <c r="N63" s="36">
         <f>VLOOKUP($D63,'538'!$B$4:$F$35,5,0)</f>
         <v>0.8</v>
       </c>
-      <c r="O63" s="19">
+      <c r="O63" s="18">
         <f>VLOOKUP($E63,'538'!$B$4:$F$35,3,0)</f>
         <v>74.099999999999994</v>
       </c>
-      <c r="P63" s="9">
+      <c r="P63" s="13">
         <f>VLOOKUP($E63,'538'!$B$4:$F$35,4,0)</f>
         <v>1.3</v>
       </c>
-      <c r="Q63" s="64">
+      <c r="Q63" s="63">
         <f>VLOOKUP($E63,'538'!$B$4:$F$35,5,0)</f>
         <v>0.7</v>
       </c>
-      <c r="R63" s="26">
+      <c r="R63" s="24">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.9</v>
       </c>
-      <c r="S63" s="8">
+      <c r="S63" s="12">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="T63" s="8">
+      <c r="T63" s="12">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.2</v>
       </c>
-      <c r="U63" s="26">
+      <c r="U63" s="24">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>1.6</v>
       </c>
-      <c r="V63" s="8">
+      <c r="V63" s="12">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>1.2</v>
       </c>
-      <c r="W63" s="8">
+      <c r="W63" s="12">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>1.3</v>
       </c>
-      <c r="X63" s="26">
+      <c r="X63" s="24">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="Y63" s="102">
+      <c r="Y63" s="101">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="Z63" s="27">
+      <c r="Z63" s="25">
         <f>VLOOKUP($D63,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="AA63" s="26">
+      <c r="AA63" s="24">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="AB63" s="102">
+      <c r="AB63" s="101">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="AC63" s="27">
+      <c r="AC63" s="25">
         <f>VLOOKUP($E63,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>16</v>
       </c>
@@ -13423,7 +13423,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AM63" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO63" s="2">
         <f t="shared" si="10"/>
@@ -13435,99 +13435,116 @@
         <f t="shared" si="9"/>
         <v>61</v>
       </c>
-      <c r="C64" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="D64" s="53"/>
-      <c r="E64" s="58"/>
-      <c r="F64" s="26"/>
+      <c r="C64" s="48">
+        <v>41828</v>
+      </c>
+      <c r="D64" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="26">
+        <v>73</v>
+      </c>
       <c r="G64" s="8">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="H64" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I64" s="37"/>
+      <c r="I64" s="37">
+        <v>49.2</v>
+      </c>
       <c r="J64" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K64" s="38"/>
-      <c r="L64" s="37" t="e">
+      <c r="K64" s="38">
+        <f t="shared" si="4"/>
+        <v>50.8</v>
+      </c>
+      <c r="L64" s="37">
         <f>VLOOKUP($D64,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M64" s="9" t="e">
+        <v>91.8</v>
+      </c>
+      <c r="M64" s="9">
         <f>VLOOKUP($D64,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N64" s="38" t="e">
+        <v>3.4</v>
+      </c>
+      <c r="N64" s="38">
         <f>VLOOKUP($D64,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O64" s="19" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="O64" s="19">
         <f>VLOOKUP($E64,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P64" s="9" t="e">
+        <v>88.9</v>
+      </c>
+      <c r="P64" s="9">
         <f>VLOOKUP($E64,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q64" s="64" t="e">
+        <v>3.2</v>
+      </c>
+      <c r="Q64" s="64">
         <f>VLOOKUP($E64,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R64" s="26" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="R64" s="26">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S64" s="8" t="e">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="S64" s="8">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T64" s="8" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="T64" s="8">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U64" s="26" t="e">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="U64" s="26">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V64" s="8" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="V64" s="8">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W64" s="8" t="e">
+        <v>4.5</v>
+      </c>
+      <c r="W64" s="8">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X64" s="26" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="X64" s="26">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y64" s="102" t="e">
+        <v>3</v>
+      </c>
+      <c r="Y64" s="102">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z64" s="27" t="e">
+        <v>19</v>
+      </c>
+      <c r="Z64" s="27">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA64" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="AA64" s="26">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB64" s="102" t="e">
+        <v>2</v>
+      </c>
+      <c r="AB64" s="102">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC64" s="27" t="e">
+        <v>17</v>
+      </c>
+      <c r="AC64" s="27">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD64" s="173"/>
-      <c r="AE64" s="174"/>
-      <c r="AF64" s="175"/>
+        <v>1</v>
+      </c>
+      <c r="AD64" s="173">
+        <v>2.75</v>
+      </c>
+      <c r="AE64" s="174">
+        <v>3.1</v>
+      </c>
+      <c r="AF64" s="175">
+        <v>2.87</v>
+      </c>
       <c r="AG64" s="183">
         <v>0</v>
       </c>
@@ -13538,111 +13555,138 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ64" s="156"/>
-      <c r="AK64" s="157"/>
-      <c r="AL64" s="158"/>
+      <c r="AJ64" s="156">
+        <v>0</v>
+      </c>
+      <c r="AK64" s="157">
+        <v>0</v>
+      </c>
+      <c r="AL64" s="158">
+        <v>0</v>
+      </c>
       <c r="AM64" s="67" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="AO64" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
       </c>
     </row>
-    <row r="65" spans="2:39">
+    <row r="65" spans="2:41">
       <c r="B65" s="43">
         <f t="shared" si="9"/>
         <v>62</v>
       </c>
-      <c r="C65" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="D65" s="53"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="26"/>
+      <c r="C65" s="48">
+        <v>41829</v>
+      </c>
+      <c r="D65" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="26">
+        <v>43</v>
+      </c>
       <c r="G65" s="8">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="H65" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I65" s="37"/>
+      <c r="I65" s="37">
+        <v>39.299999999999997</v>
+      </c>
       <c r="J65" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K65" s="38"/>
-      <c r="L65" s="37" t="e">
+      <c r="K65" s="38">
+        <f t="shared" si="4"/>
+        <v>60.7</v>
+      </c>
+      <c r="L65" s="37">
         <f>VLOOKUP($D65,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M65" s="9" t="e">
+        <v>82.5</v>
+      </c>
+      <c r="M65" s="9">
         <f>VLOOKUP($D65,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N65" s="38" t="e">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N65" s="38">
         <f>VLOOKUP($D65,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O65" s="19" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="O65" s="19">
         <f>VLOOKUP($E65,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P65" s="9" t="e">
+        <v>90</v>
+      </c>
+      <c r="P65" s="9">
         <f>VLOOKUP($E65,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q65" s="64" t="e">
+        <v>2.9</v>
+      </c>
+      <c r="Q65" s="64">
         <f>VLOOKUP($E65,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R65" s="26" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="R65" s="26">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S65" s="8" t="e">
+        <v>3.9</v>
+      </c>
+      <c r="S65" s="8">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T65" s="8" t="e">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="T65" s="8">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U65" s="26" t="e">
+        <v>4.2</v>
+      </c>
+      <c r="U65" s="26">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V65" s="8" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="V65" s="8">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W65" s="8" t="e">
+        <v>4.5</v>
+      </c>
+      <c r="W65" s="8">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X65" s="26" t="e">
+        <v>4.7</v>
+      </c>
+      <c r="X65" s="26">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y65" s="102" t="e">
+        <v>15</v>
+      </c>
+      <c r="Y65" s="102">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z65" s="27" t="e">
+        <v>9</v>
+      </c>
+      <c r="Z65" s="27">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA65" s="26" t="e">
+        <v>2</v>
+      </c>
+      <c r="AA65" s="26">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB65" s="102" t="e">
+        <v>5</v>
+      </c>
+      <c r="AB65" s="102">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC65" s="27" t="e">
+        <v>15</v>
+      </c>
+      <c r="AC65" s="27">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD65" s="173"/>
-      <c r="AE65" s="174"/>
-      <c r="AF65" s="175"/>
+        <v>1</v>
+      </c>
+      <c r="AD65" s="173">
+        <v>3.2</v>
+      </c>
+      <c r="AE65" s="174">
+        <v>3.1</v>
+      </c>
+      <c r="AF65" s="175">
+        <v>2.37</v>
+      </c>
       <c r="AG65" s="183">
         <v>0</v>
       </c>
@@ -13653,14 +13697,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ65" s="156"/>
-      <c r="AK65" s="157"/>
-      <c r="AL65" s="158"/>
+      <c r="AJ65" s="156">
+        <v>0</v>
+      </c>
+      <c r="AK65" s="157">
+        <v>0</v>
+      </c>
+      <c r="AL65" s="158">
+        <v>0</v>
+      </c>
       <c r="AM65" s="67" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="AO65" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
       </c>
     </row>
-    <row r="66" spans="2:39">
+    <row r="66" spans="2:41">
       <c r="B66" s="43">
         <f t="shared" si="9"/>
         <v>63</v>
@@ -13775,7 +13829,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="2:39" ht="15.75" thickBot="1">
+    <row r="67" spans="2:41" ht="15.75" thickBot="1">
       <c r="B67" s="44">
         <f t="shared" si="9"/>
         <v>64</v>
@@ -13909,10 +13963,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI61"/>
+  <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22417,7 +22471,7 @@
       </c>
       <c r="AC60" s="183">
         <f>Main!AG62</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD60" s="184">
         <f>Main!AH62</f>
@@ -22425,7 +22479,7 @@
       </c>
       <c r="AE60" s="151">
         <f>Main!AI62</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF60" s="156">
         <f>Main!AJ62</f>
@@ -22441,7 +22495,7 @@
       </c>
       <c r="AI60" s="188" t="str">
         <f>Main!AM62</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="61" spans="1:35">
@@ -22583,6 +22637,290 @@
       </c>
       <c r="AI61" s="188" t="str">
         <f>Main!AM63</f>
+        <v>train</v>
+      </c>
+    </row>
+    <row r="62" spans="1:35">
+      <c r="A62" s="48">
+        <f>Main!C64</f>
+        <v>41828</v>
+      </c>
+      <c r="B62" s="53" t="str">
+        <f>Main!D64</f>
+        <v>Brazil</v>
+      </c>
+      <c r="C62" s="58" t="str">
+        <f>Main!E64</f>
+        <v>Germany</v>
+      </c>
+      <c r="D62" s="37">
+        <f>Main!F64/(Main!$F64+Main!$G64)*100</f>
+        <v>73</v>
+      </c>
+      <c r="E62" s="9">
+        <f>Main!G64/(Main!$F64+Main!$G64)*100</f>
+        <v>27</v>
+      </c>
+      <c r="F62" s="37">
+        <f>Main!I64/(Main!$I64+Main!$K64)*100</f>
+        <v>49.2</v>
+      </c>
+      <c r="G62" s="38">
+        <f>Main!K64/(Main!$I64+Main!$K64)*100</f>
+        <v>50.8</v>
+      </c>
+      <c r="H62" s="37">
+        <f>Main!L64</f>
+        <v>91.8</v>
+      </c>
+      <c r="I62" s="9">
+        <f>Main!M64</f>
+        <v>3.4</v>
+      </c>
+      <c r="J62" s="38">
+        <f>Main!N64</f>
+        <v>0.5</v>
+      </c>
+      <c r="K62" s="19">
+        <f>Main!O64</f>
+        <v>88.9</v>
+      </c>
+      <c r="L62" s="9">
+        <f>Main!P64</f>
+        <v>3.2</v>
+      </c>
+      <c r="M62" s="64">
+        <f>Main!Q64</f>
+        <v>0.8</v>
+      </c>
+      <c r="N62" s="26">
+        <f>Main!R64</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="O62" s="8">
+        <f>Main!S64</f>
+        <v>4.8</v>
+      </c>
+      <c r="P62" s="8">
+        <f>Main!T64</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q62" s="26">
+        <f>Main!U64</f>
+        <v>4.8</v>
+      </c>
+      <c r="R62" s="8">
+        <f>Main!V64</f>
+        <v>4.5</v>
+      </c>
+      <c r="S62" s="8">
+        <f>Main!W64</f>
+        <v>4.8</v>
+      </c>
+      <c r="T62" s="26">
+        <f>Main!X64</f>
+        <v>3</v>
+      </c>
+      <c r="U62" s="102">
+        <f>Main!Y64</f>
+        <v>19</v>
+      </c>
+      <c r="V62" s="27">
+        <f>Main!Z64</f>
+        <v>1</v>
+      </c>
+      <c r="W62" s="26">
+        <f>Main!AA64</f>
+        <v>2</v>
+      </c>
+      <c r="X62" s="102">
+        <f>Main!AB64</f>
+        <v>17</v>
+      </c>
+      <c r="Y62" s="27">
+        <f>Main!AC64</f>
+        <v>1</v>
+      </c>
+      <c r="Z62" s="173">
+        <f>Main!AD64</f>
+        <v>2.75</v>
+      </c>
+      <c r="AA62" s="174">
+        <f>Main!AE64</f>
+        <v>3.1</v>
+      </c>
+      <c r="AB62" s="175">
+        <f>Main!AF64</f>
+        <v>2.87</v>
+      </c>
+      <c r="AC62" s="183">
+        <f>Main!AG64</f>
+        <v>0</v>
+      </c>
+      <c r="AD62" s="184">
+        <f>Main!AH64</f>
+        <v>0</v>
+      </c>
+      <c r="AE62" s="151">
+        <f>Main!AI64</f>
+        <v>0</v>
+      </c>
+      <c r="AF62" s="156">
+        <f>Main!AJ64</f>
+        <v>0</v>
+      </c>
+      <c r="AG62" s="157">
+        <f>Main!AK64</f>
+        <v>0</v>
+      </c>
+      <c r="AH62" s="158">
+        <f>Main!AL64</f>
+        <v>0</v>
+      </c>
+      <c r="AI62" s="188" t="str">
+        <f>Main!AM64</f>
+        <v>predict</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35">
+      <c r="A63" s="48">
+        <f>Main!C65</f>
+        <v>41829</v>
+      </c>
+      <c r="B63" s="53" t="str">
+        <f>Main!D65</f>
+        <v>Netherlands</v>
+      </c>
+      <c r="C63" s="58" t="str">
+        <f>Main!E65</f>
+        <v>Argentina</v>
+      </c>
+      <c r="D63" s="37">
+        <f>Main!F65/(Main!$F65+Main!$G65)*100</f>
+        <v>43</v>
+      </c>
+      <c r="E63" s="9">
+        <f>Main!G65/(Main!$F65+Main!$G65)*100</f>
+        <v>56.999999999999993</v>
+      </c>
+      <c r="F63" s="37">
+        <f>Main!I65/(Main!$I65+Main!$K65)*100</f>
+        <v>39.299999999999997</v>
+      </c>
+      <c r="G63" s="38">
+        <f>Main!K65/(Main!$I65+Main!$K65)*100</f>
+        <v>60.699999999999996</v>
+      </c>
+      <c r="H63" s="37">
+        <f>Main!L65</f>
+        <v>82.5</v>
+      </c>
+      <c r="I63" s="9">
+        <f>Main!M65</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J63" s="38">
+        <f>Main!N65</f>
+        <v>0.8</v>
+      </c>
+      <c r="K63" s="19">
+        <f>Main!O65</f>
+        <v>90</v>
+      </c>
+      <c r="L63" s="9">
+        <f>Main!P65</f>
+        <v>2.9</v>
+      </c>
+      <c r="M63" s="64">
+        <f>Main!Q65</f>
+        <v>0.4</v>
+      </c>
+      <c r="N63" s="26">
+        <f>Main!R65</f>
+        <v>3.9</v>
+      </c>
+      <c r="O63" s="8">
+        <f>Main!S65</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P63" s="8">
+        <f>Main!T65</f>
+        <v>4.2</v>
+      </c>
+      <c r="Q63" s="26">
+        <f>Main!U65</f>
+        <v>4.8</v>
+      </c>
+      <c r="R63" s="8">
+        <f>Main!V65</f>
+        <v>4.5</v>
+      </c>
+      <c r="S63" s="8">
+        <f>Main!W65</f>
+        <v>4.7</v>
+      </c>
+      <c r="T63" s="26">
+        <f>Main!X65</f>
+        <v>15</v>
+      </c>
+      <c r="U63" s="102">
+        <f>Main!Y65</f>
+        <v>9</v>
+      </c>
+      <c r="V63" s="27">
+        <f>Main!Z65</f>
+        <v>2</v>
+      </c>
+      <c r="W63" s="26">
+        <f>Main!AA65</f>
+        <v>5</v>
+      </c>
+      <c r="X63" s="102">
+        <f>Main!AB65</f>
+        <v>15</v>
+      </c>
+      <c r="Y63" s="27">
+        <f>Main!AC65</f>
+        <v>1</v>
+      </c>
+      <c r="Z63" s="173">
+        <f>Main!AD65</f>
+        <v>3.2</v>
+      </c>
+      <c r="AA63" s="174">
+        <f>Main!AE65</f>
+        <v>3.1</v>
+      </c>
+      <c r="AB63" s="175">
+        <f>Main!AF65</f>
+        <v>2.37</v>
+      </c>
+      <c r="AC63" s="183">
+        <f>Main!AG65</f>
+        <v>0</v>
+      </c>
+      <c r="AD63" s="184">
+        <f>Main!AH65</f>
+        <v>0</v>
+      </c>
+      <c r="AE63" s="151">
+        <f>Main!AI65</f>
+        <v>0</v>
+      </c>
+      <c r="AF63" s="156">
+        <f>Main!AJ65</f>
+        <v>0</v>
+      </c>
+      <c r="AG63" s="157">
+        <f>Main!AK65</f>
+        <v>0</v>
+      </c>
+      <c r="AH63" s="158">
+        <f>Main!AL65</f>
+        <v>0</v>
+      </c>
+      <c r="AI63" s="188" t="str">
+        <f>Main!AM65</f>
         <v>predict</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Predictions for 9 July
</commit_message>
<xml_diff>
--- a/data/data_wc2014.xlsx
+++ b/data/data_wc2014.xlsx
@@ -4445,10 +4445,10 @@
   <dimension ref="A1:AMP67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="AB40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="AE40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AF66" sqref="AF66"/>
+      <selection pane="bottomRight" activeCell="AM65" sqref="AM65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13435,104 +13435,104 @@
         <f t="shared" si="9"/>
         <v>61</v>
       </c>
-      <c r="C64" s="48">
+      <c r="C64" s="47">
         <v>41828</v>
       </c>
-      <c r="D64" s="53" t="s">
+      <c r="D64" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="58" t="s">
+      <c r="E64" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="F64" s="26">
+      <c r="F64" s="24">
         <v>73</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G64" s="12">
         <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="H64" s="27" t="s">
+      <c r="H64" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I64" s="37">
+      <c r="I64" s="35">
         <v>49.2</v>
       </c>
-      <c r="J64" s="9" t="s">
+      <c r="J64" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K64" s="38">
+      <c r="K64" s="36">
         <f t="shared" si="4"/>
         <v>50.8</v>
       </c>
-      <c r="L64" s="37">
+      <c r="L64" s="35">
         <f>VLOOKUP($D64,'538'!$B$4:$F$35,3,0)</f>
         <v>91.8</v>
       </c>
-      <c r="M64" s="9">
+      <c r="M64" s="13">
         <f>VLOOKUP($D64,'538'!$B$4:$F$35,4,0)</f>
         <v>3.4</v>
       </c>
-      <c r="N64" s="38">
+      <c r="N64" s="36">
         <f>VLOOKUP($D64,'538'!$B$4:$F$35,5,0)</f>
         <v>0.5</v>
       </c>
-      <c r="O64" s="19">
+      <c r="O64" s="18">
         <f>VLOOKUP($E64,'538'!$B$4:$F$35,3,0)</f>
         <v>88.9</v>
       </c>
-      <c r="P64" s="9">
+      <c r="P64" s="13">
         <f>VLOOKUP($E64,'538'!$B$4:$F$35,4,0)</f>
         <v>3.2</v>
       </c>
-      <c r="Q64" s="64">
+      <c r="Q64" s="63">
         <f>VLOOKUP($E64,'538'!$B$4:$F$35,5,0)</f>
         <v>0.8</v>
       </c>
-      <c r="R64" s="26">
+      <c r="R64" s="24">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="S64" s="8">
+      <c r="S64" s="12">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="T64" s="8">
+      <c r="T64" s="12">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="U64" s="26">
+      <c r="U64" s="24">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="V64" s="8">
+      <c r="V64" s="12">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5</v>
       </c>
-      <c r="W64" s="8">
+      <c r="W64" s="12">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="X64" s="26">
+      <c r="X64" s="24">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="Y64" s="102">
+      <c r="Y64" s="101">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>19</v>
       </c>
-      <c r="Z64" s="27">
+      <c r="Z64" s="25">
         <f>VLOOKUP($D64,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="AA64" s="26">
+      <c r="AA64" s="24">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="AB64" s="102">
+      <c r="AB64" s="101">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>17</v>
       </c>
-      <c r="AC64" s="27">
+      <c r="AC64" s="25">
         <f>VLOOKUP($E64,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
@@ -13546,26 +13546,26 @@
         <v>2.87</v>
       </c>
       <c r="AG64" s="183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH64" s="184">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AI64" s="151">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="AJ64" s="156">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="AK64" s="157">
-        <v>0</v>
+        <v>0.87</v>
       </c>
       <c r="AL64" s="158">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AM64" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO64" s="2">
         <f t="shared" si="10"/>
@@ -13679,10 +13679,10 @@
         <v>1</v>
       </c>
       <c r="AD65" s="173">
+        <v>3.1</v>
+      </c>
+      <c r="AE65" s="174">
         <v>3.2</v>
-      </c>
-      <c r="AE65" s="174">
-        <v>3.1</v>
       </c>
       <c r="AF65" s="175">
         <v>2.37</v>
@@ -13698,13 +13698,13 @@
         <v>0</v>
       </c>
       <c r="AJ65" s="156">
-        <v>0</v>
+        <v>1.01</v>
       </c>
       <c r="AK65" s="157">
-        <v>0</v>
+        <v>1.37</v>
       </c>
       <c r="AL65" s="158">
-        <v>0</v>
+        <v>-0.11</v>
       </c>
       <c r="AM65" s="67" t="s">
         <v>62</v>
@@ -22755,31 +22755,31 @@
       </c>
       <c r="AC62" s="183">
         <f>Main!AG64</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD62" s="184">
         <f>Main!AH64</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AE62" s="151">
         <f>Main!AI64</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="AF62" s="156">
         <f>Main!AJ64</f>
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="AG62" s="157">
         <f>Main!AK64</f>
-        <v>0</v>
+        <v>0.87</v>
       </c>
       <c r="AH62" s="158">
         <f>Main!AL64</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AI62" s="188" t="str">
         <f>Main!AM64</f>
-        <v>predict</v>
+        <v>train</v>
       </c>
     </row>
     <row r="63" spans="1:35">
@@ -22885,11 +22885,11 @@
       </c>
       <c r="Z63" s="173">
         <f>Main!AD65</f>
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="AA63" s="174">
         <f>Main!AE65</f>
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="AB63" s="175">
         <f>Main!AF65</f>
@@ -22909,15 +22909,15 @@
       </c>
       <c r="AF63" s="156">
         <f>Main!AJ65</f>
-        <v>0</v>
+        <v>1.01</v>
       </c>
       <c r="AG63" s="157">
         <f>Main!AK65</f>
-        <v>0</v>
+        <v>1.37</v>
       </c>
       <c r="AH63" s="158">
         <f>Main!AL65</f>
-        <v>0</v>
+        <v>-0.11</v>
       </c>
       <c r="AI63" s="188" t="str">
         <f>Main!AM65</f>

</xml_diff>

<commit_message>
predictions for 12 July
</commit_message>
<xml_diff>
--- a/data/data_wc2014.xlsx
+++ b/data/data_wc2014.xlsx
@@ -28,8 +28,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jo-fai Chow</author>
+  </authors>
+  <commentList>
+    <comment ref="F66" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jo-fai Chow:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not available
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="97">
   <si>
     <t>Team</t>
   </si>
@@ -319,13 +354,7 @@
     <t>RES_DIFF</t>
   </si>
   <si>
-    <t>xx/xx/xxxx</t>
-  </si>
-  <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>future</t>
   </si>
 </sst>
 </file>
@@ -335,7 +364,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -365,6 +394,26 @@
       <name val="Sans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1094,7 +1143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1801,6 +1850,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4441,14 +4496,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMP67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="AE40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="AD40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AM65" sqref="AM65"/>
+      <selection pane="bottomRight" activeCell="AH67" sqref="AH67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11712,16 +11767,16 @@
         <v>22</v>
       </c>
       <c r="H52" s="218" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I52" s="219">
         <v>81.099999999999994</v>
       </c>
       <c r="J52" s="220" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K52" s="221">
-        <f t="shared" ref="K52:K65" si="4">100-I52</f>
+        <f t="shared" ref="K52:K67" si="4">100-I52</f>
         <v>18.900000000000006</v>
       </c>
       <c r="L52" s="219">
@@ -11858,13 +11913,13 @@
         <v>37</v>
       </c>
       <c r="H53" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I53" s="35">
         <v>54</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K53" s="36">
         <f t="shared" si="4"/>
@@ -12004,13 +12059,13 @@
         <v>31</v>
       </c>
       <c r="H54" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I54" s="35">
         <v>65.599999999999994</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K54" s="36">
         <f t="shared" si="4"/>
@@ -12150,13 +12205,13 @@
         <v>44</v>
       </c>
       <c r="H55" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I55" s="35">
         <v>32.299999999999997</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K55" s="36">
         <f t="shared" si="4"/>
@@ -12266,7 +12321,7 @@
         <v>61</v>
       </c>
       <c r="AO55" s="2">
-        <f t="shared" ref="AO55:AO65" si="10">SUM(F55:H55)</f>
+        <f t="shared" ref="AO55:AO66" si="10">SUM(F55:H55)</f>
         <v>100</v>
       </c>
       <c r="AP55" s="2">
@@ -12296,13 +12351,13 @@
         <v>28</v>
       </c>
       <c r="H56" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I56" s="35">
         <v>66.8</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K56" s="36">
         <f t="shared" si="4"/>
@@ -12442,13 +12497,13 @@
         <v>18</v>
       </c>
       <c r="H57" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I57" s="35">
         <v>87.1</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K57" s="36">
         <f t="shared" si="4"/>
@@ -12588,13 +12643,13 @@
         <v>25</v>
       </c>
       <c r="H58" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I58" s="35">
         <v>77.7</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K58" s="36">
         <f t="shared" si="4"/>
@@ -12734,13 +12789,13 @@
         <v>41</v>
       </c>
       <c r="H59" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I59" s="35">
         <v>69.2</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K59" s="36">
         <f t="shared" si="4"/>
@@ -12880,13 +12935,13 @@
         <v>53</v>
       </c>
       <c r="H60" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I60" s="35">
         <v>30.8</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K60" s="36">
         <f t="shared" si="4"/>
@@ -13026,13 +13081,13 @@
         <v>28</v>
       </c>
       <c r="H61" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I61" s="35">
         <v>71.400000000000006</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K61" s="36">
         <f t="shared" si="4"/>
@@ -13168,13 +13223,13 @@
         <v>28</v>
       </c>
       <c r="H62" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I62" s="35">
         <v>58.2</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K62" s="36">
         <f t="shared" si="4"/>
@@ -13310,13 +13365,13 @@
         <v>24</v>
       </c>
       <c r="H63" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I63" s="35">
         <v>85.3</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K63" s="36">
         <f t="shared" si="4"/>
@@ -13452,13 +13507,13 @@
         <v>27</v>
       </c>
       <c r="H64" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I64" s="35">
         <v>49.2</v>
       </c>
       <c r="J64" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K64" s="36">
         <f t="shared" si="4"/>
@@ -13577,104 +13632,104 @@
         <f t="shared" si="9"/>
         <v>62</v>
       </c>
-      <c r="C65" s="48">
+      <c r="C65" s="47">
         <v>41829</v>
       </c>
-      <c r="D65" s="53" t="s">
+      <c r="D65" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E65" s="58" t="s">
+      <c r="E65" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="F65" s="26">
+      <c r="F65" s="24">
         <v>43</v>
       </c>
-      <c r="G65" s="8">
+      <c r="G65" s="12">
         <f t="shared" si="8"/>
         <v>57</v>
       </c>
-      <c r="H65" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="I65" s="37">
+      <c r="H65" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="I65" s="35">
         <v>39.299999999999997</v>
       </c>
-      <c r="J65" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="K65" s="38">
+      <c r="J65" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="K65" s="36">
         <f t="shared" si="4"/>
         <v>60.7</v>
       </c>
-      <c r="L65" s="37">
+      <c r="L65" s="35">
         <f>VLOOKUP($D65,'538'!$B$4:$F$35,3,0)</f>
         <v>82.5</v>
       </c>
-      <c r="M65" s="9">
+      <c r="M65" s="13">
         <f>VLOOKUP($D65,'538'!$B$4:$F$35,4,0)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="N65" s="38">
+      <c r="N65" s="36">
         <f>VLOOKUP($D65,'538'!$B$4:$F$35,5,0)</f>
         <v>0.8</v>
       </c>
-      <c r="O65" s="19">
+      <c r="O65" s="18">
         <f>VLOOKUP($E65,'538'!$B$4:$F$35,3,0)</f>
         <v>90</v>
       </c>
-      <c r="P65" s="9">
+      <c r="P65" s="13">
         <f>VLOOKUP($E65,'538'!$B$4:$F$35,4,0)</f>
         <v>2.9</v>
       </c>
-      <c r="Q65" s="64">
+      <c r="Q65" s="63">
         <f>VLOOKUP($E65,'538'!$B$4:$F$35,5,0)</f>
         <v>0.4</v>
       </c>
-      <c r="R65" s="26">
+      <c r="R65" s="24">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>3.9</v>
       </c>
-      <c r="S65" s="8">
+      <c r="S65" s="12">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="T65" s="8">
+      <c r="T65" s="12">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.2</v>
       </c>
-      <c r="U65" s="26">
+      <c r="U65" s="24">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,6,FALSE)</f>
         <v>4.8</v>
       </c>
-      <c r="V65" s="8">
+      <c r="V65" s="12">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,7,FALSE)</f>
         <v>4.5</v>
       </c>
-      <c r="W65" s="8">
+      <c r="W65" s="12">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,8,FALSE)</f>
         <v>4.7</v>
       </c>
-      <c r="X65" s="26">
+      <c r="X65" s="24">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="Y65" s="102">
+      <c r="Y65" s="101">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="Z65" s="27">
+      <c r="Z65" s="25">
         <f>VLOOKUP($D65,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="AA65" s="26">
+      <c r="AA65" s="24">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,9,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="AB65" s="102">
+      <c r="AB65" s="101">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,10,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="AC65" s="27">
+      <c r="AC65" s="25">
         <f>VLOOKUP($E65,'538'!$B$3:$L$35,11,FALSE)</f>
         <v>1</v>
       </c>
@@ -13707,7 +13762,7 @@
         <v>-0.11</v>
       </c>
       <c r="AM65" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AO65" s="2">
         <f t="shared" si="10"/>
@@ -13719,99 +13774,116 @@
         <f t="shared" si="9"/>
         <v>63</v>
       </c>
-      <c r="C66" s="48" t="s">
+      <c r="C66" s="48">
+        <v>41832</v>
+      </c>
+      <c r="D66" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F66" s="237">
+        <v>50</v>
+      </c>
+      <c r="G66" s="238">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="H66" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D66" s="53"/>
-      <c r="E66" s="58"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="8">
-        <f t="shared" si="8"/>
-        <v>100</v>
-      </c>
-      <c r="H66" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="I66" s="37"/>
+      <c r="I66" s="37">
+        <v>60.6</v>
+      </c>
       <c r="J66" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="K66" s="38"/>
-      <c r="L66" s="37" t="e">
+        <v>96</v>
+      </c>
+      <c r="K66" s="38">
+        <f t="shared" si="4"/>
+        <v>39.4</v>
+      </c>
+      <c r="L66" s="37">
         <f>VLOOKUP($D66,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M66" s="9" t="e">
+        <v>91.8</v>
+      </c>
+      <c r="M66" s="9">
         <f>VLOOKUP($D66,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N66" s="38" t="e">
+        <v>3.4</v>
+      </c>
+      <c r="N66" s="38">
         <f>VLOOKUP($D66,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O66" s="19" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="O66" s="19">
         <f>VLOOKUP($E66,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P66" s="9" t="e">
+        <v>82.5</v>
+      </c>
+      <c r="P66" s="9">
         <f>VLOOKUP($E66,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q66" s="64" t="e">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q66" s="64">
         <f>VLOOKUP($E66,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R66" s="26" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="R66" s="26">
         <f>VLOOKUP($D66,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S66" s="8" t="e">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="S66" s="8">
         <f>VLOOKUP($D66,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T66" s="8" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="T66" s="8">
         <f>VLOOKUP($D66,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U66" s="26" t="e">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="U66" s="26">
         <f>VLOOKUP($E66,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V66" s="8" t="e">
+        <v>3.9</v>
+      </c>
+      <c r="V66" s="8">
         <f>VLOOKUP($E66,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W66" s="8" t="e">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="W66" s="8">
         <f>VLOOKUP($E66,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X66" s="26" t="e">
+        <v>4.2</v>
+      </c>
+      <c r="X66" s="26">
         <f>VLOOKUP($D66,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y66" s="102" t="e">
+        <v>3</v>
+      </c>
+      <c r="Y66" s="102">
         <f>VLOOKUP($D66,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z66" s="27" t="e">
+        <v>19</v>
+      </c>
+      <c r="Z66" s="27">
         <f>VLOOKUP($D66,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA66" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="AA66" s="26">
         <f>VLOOKUP($E66,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB66" s="102" t="e">
+        <v>15</v>
+      </c>
+      <c r="AB66" s="102">
         <f>VLOOKUP($E66,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC66" s="27" t="e">
+        <v>9</v>
+      </c>
+      <c r="AC66" s="27">
         <f>VLOOKUP($E66,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD66" s="173"/>
-      <c r="AE66" s="174"/>
-      <c r="AF66" s="175"/>
+        <v>2</v>
+      </c>
+      <c r="AD66" s="173">
+        <v>2.15</v>
+      </c>
+      <c r="AE66" s="174">
+        <v>3.6</v>
+      </c>
+      <c r="AF66" s="175">
+        <v>3.2</v>
+      </c>
       <c r="AG66" s="183">
         <v>0</v>
       </c>
@@ -13826,7 +13898,11 @@
       <c r="AK66" s="157"/>
       <c r="AL66" s="158"/>
       <c r="AM66" s="67" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="AO66" s="2">
+        <f t="shared" si="10"/>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="2:41" ht="15.75" thickBot="1">
@@ -13834,99 +13910,116 @@
         <f t="shared" si="9"/>
         <v>64</v>
       </c>
-      <c r="C67" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D67" s="54"/>
-      <c r="E67" s="59"/>
-      <c r="F67" s="28"/>
+      <c r="C67" s="49">
+        <v>41833</v>
+      </c>
+      <c r="D67" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="28">
+        <v>63</v>
+      </c>
       <c r="G67" s="29">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="H67" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="I67" s="39"/>
+        <v>96</v>
+      </c>
+      <c r="I67" s="39">
+        <v>50.9</v>
+      </c>
       <c r="J67" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="K67" s="41"/>
-      <c r="L67" s="39" t="e">
+        <v>96</v>
+      </c>
+      <c r="K67" s="38">
+        <f t="shared" si="4"/>
+        <v>49.1</v>
+      </c>
+      <c r="L67" s="39">
         <f>VLOOKUP($D67,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M67" s="40" t="e">
+        <v>88.9</v>
+      </c>
+      <c r="M67" s="40">
         <f>VLOOKUP($D67,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N67" s="41" t="e">
+        <v>3.2</v>
+      </c>
+      <c r="N67" s="41">
         <f>VLOOKUP($D67,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O67" s="60" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="O67" s="60">
         <f>VLOOKUP($E67,'538'!$B$4:$F$35,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P67" s="40" t="e">
+        <v>90</v>
+      </c>
+      <c r="P67" s="40">
         <f>VLOOKUP($E67,'538'!$B$4:$F$35,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q67" s="65" t="e">
+        <v>2.9</v>
+      </c>
+      <c r="Q67" s="65">
         <f>VLOOKUP($E67,'538'!$B$4:$F$35,5,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R67" s="28" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="R67" s="28">
         <f>VLOOKUP($D67,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S67" s="29" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="S67" s="29">
         <f>VLOOKUP($D67,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T67" s="29" t="e">
+        <v>4.5</v>
+      </c>
+      <c r="T67" s="29">
         <f>VLOOKUP($D67,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U67" s="28" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="U67" s="28">
         <f>VLOOKUP($E67,'538'!$B$3:$L$35,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V67" s="29" t="e">
+        <v>4.8</v>
+      </c>
+      <c r="V67" s="29">
         <f>VLOOKUP($E67,'538'!$B$3:$L$35,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W67" s="29" t="e">
+        <v>4.5</v>
+      </c>
+      <c r="W67" s="29">
         <f>VLOOKUP($E67,'538'!$B$3:$L$35,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X67" s="28" t="e">
+        <v>4.7</v>
+      </c>
+      <c r="X67" s="28">
         <f>VLOOKUP($D67,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y67" s="103" t="e">
+        <v>2</v>
+      </c>
+      <c r="Y67" s="103">
         <f>VLOOKUP($D67,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z67" s="30" t="e">
+        <v>17</v>
+      </c>
+      <c r="Z67" s="30">
         <f>VLOOKUP($D67,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA67" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="AA67" s="28">
         <f>VLOOKUP($E67,'538'!$B$3:$L$35,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB67" s="103" t="e">
+        <v>5</v>
+      </c>
+      <c r="AB67" s="103">
         <f>VLOOKUP($E67,'538'!$B$3:$L$35,10,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC67" s="30" t="e">
+        <v>15</v>
+      </c>
+      <c r="AC67" s="30">
         <f>VLOOKUP($E67,'538'!$B$3:$L$35,11,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD67" s="176"/>
-      <c r="AE67" s="177"/>
-      <c r="AF67" s="178"/>
+        <v>1</v>
+      </c>
+      <c r="AD67" s="176">
+        <v>2.25</v>
+      </c>
+      <c r="AE67" s="177">
+        <v>3.1</v>
+      </c>
+      <c r="AF67" s="178">
+        <v>3.4</v>
+      </c>
       <c r="AG67" s="185">
         <v>0</v>
       </c>
@@ -13941,7 +14034,7 @@
       <c r="AK67" s="160"/>
       <c r="AL67" s="161"/>
       <c r="AM67" s="68" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -13958,15 +14051,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI63"/>
+  <dimension ref="A1:AI65"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:Y63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20940,103 +21034,103 @@
       </c>
     </row>
     <row r="50" spans="1:35">
-      <c r="A50" s="48">
+      <c r="A50" s="47">
         <f>Main!C52</f>
         <v>41818</v>
       </c>
-      <c r="B50" s="53" t="str">
+      <c r="B50" s="52" t="str">
         <f>Main!D52</f>
         <v>Brazil</v>
       </c>
-      <c r="C50" s="58" t="str">
+      <c r="C50" s="57" t="str">
         <f>Main!E52</f>
         <v>Chile</v>
       </c>
-      <c r="D50" s="37">
+      <c r="D50" s="35">
         <f>Main!F52/(Main!$F52+Main!$G52)*100</f>
         <v>78</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="13">
         <f>Main!G52/(Main!$F52+Main!$G52)*100</f>
         <v>22</v>
       </c>
-      <c r="F50" s="37">
+      <c r="F50" s="35">
         <f>Main!I52/(Main!$I52+Main!$K52)*100</f>
         <v>81.099999999999994</v>
       </c>
-      <c r="G50" s="38">
+      <c r="G50" s="36">
         <f>Main!K52/(Main!$I52+Main!$K52)*100</f>
         <v>18.900000000000006</v>
       </c>
-      <c r="H50" s="37">
+      <c r="H50" s="35">
         <f>Main!L52</f>
         <v>91.8</v>
       </c>
-      <c r="I50" s="9">
+      <c r="I50" s="13">
         <f>Main!M52</f>
         <v>3.4</v>
       </c>
-      <c r="J50" s="38">
+      <c r="J50" s="36">
         <f>Main!N52</f>
         <v>0.5</v>
       </c>
-      <c r="K50" s="19">
+      <c r="K50" s="18">
         <f>Main!O52</f>
         <v>86.7</v>
       </c>
-      <c r="L50" s="9">
+      <c r="L50" s="13">
         <f>Main!P52</f>
         <v>2.7</v>
       </c>
-      <c r="M50" s="64">
+      <c r="M50" s="63">
         <f>Main!Q52</f>
         <v>0.7</v>
       </c>
-      <c r="N50" s="26">
+      <c r="N50" s="24">
         <f>Main!R52</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="O50" s="8">
+      <c r="O50" s="12">
         <f>Main!S52</f>
         <v>4.8</v>
       </c>
-      <c r="P50" s="8">
+      <c r="P50" s="12">
         <f>Main!T52</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="Q50" s="26">
+      <c r="Q50" s="24">
         <f>Main!U52</f>
         <v>4.2</v>
       </c>
-      <c r="R50" s="8">
+      <c r="R50" s="12">
         <f>Main!V52</f>
         <v>2.6</v>
       </c>
-      <c r="S50" s="8">
+      <c r="S50" s="12">
         <f>Main!W52</f>
         <v>3.6</v>
       </c>
-      <c r="T50" s="26">
+      <c r="T50" s="24">
         <f>Main!X52</f>
         <v>3</v>
       </c>
-      <c r="U50" s="102">
+      <c r="U50" s="101">
         <f>Main!Y52</f>
         <v>19</v>
       </c>
-      <c r="V50" s="27">
+      <c r="V50" s="25">
         <f>Main!Z52</f>
         <v>1</v>
       </c>
-      <c r="W50" s="26">
+      <c r="W50" s="24">
         <f>Main!AA52</f>
         <v>14</v>
       </c>
-      <c r="X50" s="102">
+      <c r="X50" s="101">
         <f>Main!AB52</f>
         <v>8</v>
       </c>
-      <c r="Y50" s="27">
+      <c r="Y50" s="25">
         <f>Main!AC52</f>
         <v>3</v>
       </c>
@@ -21079,103 +21173,103 @@
       </c>
     </row>
     <row r="51" spans="1:35">
-      <c r="A51" s="48">
+      <c r="A51" s="47">
         <f>Main!C53</f>
         <v>41818</v>
       </c>
-      <c r="B51" s="53" t="str">
+      <c r="B51" s="52" t="str">
         <f>Main!D53</f>
         <v>Colombia</v>
       </c>
-      <c r="C51" s="58" t="str">
+      <c r="C51" s="57" t="str">
         <f>Main!E53</f>
         <v>Uruguay</v>
       </c>
-      <c r="D51" s="37">
+      <c r="D51" s="35">
         <f>Main!F53/(Main!$F53+Main!$G53)*100</f>
         <v>63</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E51" s="13">
         <f>Main!G53/(Main!$F53+Main!$G53)*100</f>
         <v>37</v>
       </c>
-      <c r="F51" s="37">
+      <c r="F51" s="35">
         <f>Main!I53/(Main!$I53+Main!$K53)*100</f>
         <v>54</v>
       </c>
-      <c r="G51" s="38">
+      <c r="G51" s="36">
         <f>Main!K53/(Main!$I53+Main!$K53)*100</f>
         <v>46</v>
       </c>
-      <c r="H51" s="37">
+      <c r="H51" s="35">
         <f>Main!L53</f>
         <v>85.8</v>
       </c>
-      <c r="I51" s="9">
+      <c r="I51" s="13">
         <f>Main!M53</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="J51" s="38">
+      <c r="J51" s="36">
         <f>Main!N53</f>
         <v>0.5</v>
       </c>
-      <c r="K51" s="19">
+      <c r="K51" s="18">
         <f>Main!O53</f>
         <v>83.3</v>
       </c>
-      <c r="L51" s="9">
+      <c r="L51" s="13">
         <f>Main!P53</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="M51" s="64">
+      <c r="M51" s="63">
         <f>Main!Q53</f>
         <v>0.7</v>
       </c>
-      <c r="N51" s="26">
+      <c r="N51" s="24">
         <f>Main!R53</f>
         <v>3.9</v>
       </c>
-      <c r="O51" s="8">
+      <c r="O51" s="12">
         <f>Main!S53</f>
         <v>4</v>
       </c>
-      <c r="P51" s="8">
+      <c r="P51" s="12">
         <f>Main!T53</f>
         <v>4</v>
       </c>
-      <c r="Q51" s="26">
+      <c r="Q51" s="24">
         <f>Main!U53</f>
         <v>4.3</v>
       </c>
-      <c r="R51" s="8">
+      <c r="R51" s="12">
         <f>Main!V53</f>
         <v>3.1</v>
       </c>
-      <c r="S51" s="8">
+      <c r="S51" s="12">
         <f>Main!W53</f>
         <v>3.8</v>
       </c>
-      <c r="T51" s="26">
+      <c r="T51" s="24">
         <f>Main!X53</f>
         <v>8</v>
       </c>
-      <c r="U51" s="102">
+      <c r="U51" s="101">
         <f>Main!Y53</f>
         <v>4</v>
       </c>
-      <c r="V51" s="27">
+      <c r="V51" s="25">
         <f>Main!Z53</f>
         <v>16</v>
       </c>
-      <c r="W51" s="26">
+      <c r="W51" s="24">
         <f>Main!AA53</f>
         <v>7</v>
       </c>
-      <c r="X51" s="102">
+      <c r="X51" s="101">
         <f>Main!AB53</f>
         <v>11</v>
       </c>
-      <c r="Y51" s="27">
+      <c r="Y51" s="25">
         <f>Main!AC53</f>
         <v>1</v>
       </c>
@@ -21221,103 +21315,103 @@
       </c>
     </row>
     <row r="52" spans="1:35">
-      <c r="A52" s="48">
+      <c r="A52" s="47">
         <f>Main!C54</f>
         <v>41819</v>
       </c>
-      <c r="B52" s="53" t="str">
+      <c r="B52" s="52" t="str">
         <f>Main!D54</f>
         <v>Netherlands</v>
       </c>
-      <c r="C52" s="58" t="str">
+      <c r="C52" s="57" t="str">
         <f>Main!E54</f>
         <v>Mexico</v>
       </c>
-      <c r="D52" s="37">
+      <c r="D52" s="35">
         <f>Main!F54/(Main!$F54+Main!$G54)*100</f>
         <v>69</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="13">
         <f>Main!G54/(Main!$F54+Main!$G54)*100</f>
         <v>31</v>
       </c>
-      <c r="F52" s="37">
+      <c r="F52" s="35">
         <f>Main!I54/(Main!$I54+Main!$K54)*100</f>
         <v>65.599999999999994</v>
       </c>
-      <c r="G52" s="38">
+      <c r="G52" s="36">
         <f>Main!K54/(Main!$I54+Main!$K54)*100</f>
         <v>34.400000000000006</v>
       </c>
-      <c r="H52" s="37">
+      <c r="H52" s="35">
         <f>Main!L54</f>
         <v>82.5</v>
       </c>
-      <c r="I52" s="9">
+      <c r="I52" s="13">
         <f>Main!M54</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="J52" s="38">
+      <c r="J52" s="36">
         <f>Main!N54</f>
         <v>0.8</v>
       </c>
-      <c r="K52" s="19">
+      <c r="K52" s="18">
         <f>Main!O54</f>
         <v>77</v>
       </c>
-      <c r="L52" s="9">
+      <c r="L52" s="13">
         <f>Main!P54</f>
         <v>1.6</v>
       </c>
-      <c r="M52" s="64">
+      <c r="M52" s="63">
         <f>Main!Q54</f>
         <v>0.7</v>
       </c>
-      <c r="N52" s="26">
+      <c r="N52" s="24">
         <f>Main!R54</f>
         <v>3.9</v>
       </c>
-      <c r="O52" s="8">
+      <c r="O52" s="12">
         <f>Main!S54</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="P52" s="8">
+      <c r="P52" s="12">
         <f>Main!T54</f>
         <v>4.2</v>
       </c>
-      <c r="Q52" s="26">
+      <c r="Q52" s="24">
         <f>Main!U54</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="R52" s="8">
+      <c r="R52" s="12">
         <f>Main!V54</f>
         <v>3.1</v>
       </c>
-      <c r="S52" s="8">
+      <c r="S52" s="12">
         <f>Main!W54</f>
         <v>2.7</v>
       </c>
-      <c r="T52" s="26">
+      <c r="T52" s="24">
         <f>Main!X54</f>
         <v>15</v>
       </c>
-      <c r="U52" s="102">
+      <c r="U52" s="101">
         <f>Main!Y54</f>
         <v>9</v>
       </c>
-      <c r="V52" s="27">
+      <c r="V52" s="25">
         <f>Main!Z54</f>
         <v>2</v>
       </c>
-      <c r="W52" s="26">
+      <c r="W52" s="24">
         <f>Main!AA54</f>
         <v>20</v>
       </c>
-      <c r="X52" s="102">
+      <c r="X52" s="101">
         <f>Main!AB54</f>
         <v>14</v>
       </c>
-      <c r="Y52" s="27">
+      <c r="Y52" s="25">
         <f>Main!AC54</f>
         <v>8</v>
       </c>
@@ -21363,103 +21457,103 @@
       </c>
     </row>
     <row r="53" spans="1:35">
-      <c r="A53" s="48">
+      <c r="A53" s="47">
         <f>Main!C55</f>
         <v>41819</v>
       </c>
-      <c r="B53" s="53" t="str">
+      <c r="B53" s="52" t="str">
         <f>Main!D55</f>
         <v>Costa Rica</v>
       </c>
-      <c r="C53" s="58" t="str">
+      <c r="C53" s="57" t="str">
         <f>Main!E55</f>
         <v>Greece</v>
       </c>
-      <c r="D53" s="37">
+      <c r="D53" s="35">
         <f>Main!F55/(Main!$F55+Main!$G55)*100</f>
         <v>56.000000000000007</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E53" s="13">
         <f>Main!G55/(Main!$F55+Main!$G55)*100</f>
         <v>44</v>
       </c>
-      <c r="F53" s="37">
+      <c r="F53" s="35">
         <f>Main!I55/(Main!$I55+Main!$K55)*100</f>
         <v>32.299999999999997</v>
       </c>
-      <c r="G53" s="38">
+      <c r="G53" s="36">
         <f>Main!K55/(Main!$I55+Main!$K55)*100</f>
         <v>67.7</v>
       </c>
-      <c r="H53" s="37">
+      <c r="H53" s="35">
         <f>Main!L55</f>
         <v>74.099999999999994</v>
       </c>
-      <c r="I53" s="9">
+      <c r="I53" s="13">
         <f>Main!M55</f>
         <v>1.3</v>
       </c>
-      <c r="J53" s="38">
+      <c r="J53" s="36">
         <f>Main!N55</f>
         <v>0.7</v>
       </c>
-      <c r="K53" s="19">
+      <c r="K53" s="18">
         <f>Main!O55</f>
         <v>76.8</v>
       </c>
-      <c r="L53" s="9">
+      <c r="L53" s="13">
         <f>Main!P55</f>
         <v>1.3</v>
       </c>
-      <c r="M53" s="64">
+      <c r="M53" s="63">
         <f>Main!Q55</f>
         <v>0.5</v>
       </c>
-      <c r="N53" s="26">
+      <c r="N53" s="24">
         <f>Main!R55</f>
         <v>1.6</v>
       </c>
-      <c r="O53" s="8">
+      <c r="O53" s="12">
         <f>Main!S55</f>
         <v>1.2</v>
       </c>
-      <c r="P53" s="8">
+      <c r="P53" s="12">
         <f>Main!T55</f>
         <v>1.3</v>
       </c>
-      <c r="Q53" s="26">
+      <c r="Q53" s="24">
         <f>Main!U55</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="R53" s="8">
+      <c r="R53" s="12">
         <f>Main!V55</f>
         <v>3.8</v>
       </c>
-      <c r="S53" s="8">
+      <c r="S53" s="12">
         <f>Main!W55</f>
         <v>3</v>
       </c>
-      <c r="T53" s="26">
+      <c r="T53" s="24">
         <f>Main!X55</f>
         <v>28</v>
       </c>
-      <c r="U53" s="102">
+      <c r="U53" s="101">
         <f>Main!Y55</f>
         <v>3</v>
       </c>
-      <c r="V53" s="27">
+      <c r="V53" s="25">
         <f>Main!Z55</f>
         <v>16</v>
       </c>
-      <c r="W53" s="26">
+      <c r="W53" s="24">
         <f>Main!AA55</f>
         <v>12</v>
       </c>
-      <c r="X53" s="102">
+      <c r="X53" s="101">
         <f>Main!AB55</f>
         <v>2</v>
       </c>
-      <c r="Y53" s="27">
+      <c r="Y53" s="25">
         <f>Main!AC55</f>
         <v>32</v>
       </c>
@@ -21505,103 +21599,103 @@
       </c>
     </row>
     <row r="54" spans="1:35">
-      <c r="A54" s="48">
+      <c r="A54" s="47">
         <f>Main!C56</f>
         <v>41820</v>
       </c>
-      <c r="B54" s="53" t="str">
+      <c r="B54" s="52" t="str">
         <f>Main!D56</f>
         <v>France</v>
       </c>
-      <c r="C54" s="58" t="str">
+      <c r="C54" s="57" t="str">
         <f>Main!E56</f>
         <v>Nigeria</v>
       </c>
-      <c r="D54" s="37">
+      <c r="D54" s="35">
         <f>Main!F56/(Main!$F56+Main!$G56)*100</f>
         <v>72</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="13">
         <f>Main!G56/(Main!$F56+Main!$G56)*100</f>
         <v>28.000000000000004</v>
       </c>
-      <c r="F54" s="37">
+      <c r="F54" s="35">
         <f>Main!I56/(Main!$I56+Main!$K56)*100</f>
         <v>66.8</v>
       </c>
-      <c r="G54" s="38">
+      <c r="G54" s="36">
         <f>Main!K56/(Main!$I56+Main!$K56)*100</f>
         <v>33.200000000000003</v>
       </c>
-      <c r="H54" s="37">
+      <c r="H54" s="35">
         <f>Main!L56</f>
         <v>86.1</v>
       </c>
-      <c r="I54" s="9">
+      <c r="I54" s="13">
         <f>Main!M56</f>
         <v>2.5</v>
       </c>
-      <c r="J54" s="38">
+      <c r="J54" s="36">
         <f>Main!N56</f>
         <v>0.6</v>
       </c>
-      <c r="K54" s="19">
+      <c r="K54" s="18">
         <f>Main!O56</f>
         <v>75.2</v>
       </c>
-      <c r="L54" s="9">
+      <c r="L54" s="13">
         <f>Main!P56</f>
         <v>1.7</v>
       </c>
-      <c r="M54" s="64">
+      <c r="M54" s="63">
         <f>Main!Q56</f>
         <v>0.9</v>
       </c>
-      <c r="N54" s="26">
+      <c r="N54" s="24">
         <f>Main!R56</f>
         <v>3.3</v>
       </c>
-      <c r="O54" s="8">
+      <c r="O54" s="12">
         <f>Main!S56</f>
         <v>4</v>
       </c>
-      <c r="P54" s="8">
+      <c r="P54" s="12">
         <f>Main!T56</f>
         <v>3.7</v>
       </c>
-      <c r="Q54" s="26">
+      <c r="Q54" s="24">
         <f>Main!U56</f>
         <v>1.3</v>
       </c>
-      <c r="R54" s="8">
+      <c r="R54" s="12">
         <f>Main!V56</f>
         <v>3</v>
       </c>
-      <c r="S54" s="8">
+      <c r="S54" s="12">
         <f>Main!W56</f>
         <v>1.9</v>
       </c>
-      <c r="T54" s="26">
+      <c r="T54" s="24">
         <f>Main!X56</f>
         <v>17</v>
       </c>
-      <c r="U54" s="102">
+      <c r="U54" s="101">
         <f>Main!Y56</f>
         <v>13</v>
       </c>
-      <c r="V54" s="27">
+      <c r="V54" s="25">
         <f>Main!Z56</f>
         <v>1</v>
       </c>
-      <c r="W54" s="26">
+      <c r="W54" s="24">
         <f>Main!AA56</f>
         <v>44</v>
       </c>
-      <c r="X54" s="102">
+      <c r="X54" s="101">
         <f>Main!AB56</f>
         <v>4</v>
       </c>
-      <c r="Y54" s="27">
+      <c r="Y54" s="25">
         <f>Main!AC56</f>
         <v>16</v>
       </c>
@@ -21647,103 +21741,103 @@
       </c>
     </row>
     <row r="55" spans="1:35">
-      <c r="A55" s="48">
+      <c r="A55" s="47">
         <f>Main!C57</f>
         <v>41820</v>
       </c>
-      <c r="B55" s="53" t="str">
+      <c r="B55" s="52" t="str">
         <f>Main!D57</f>
         <v>Germany</v>
       </c>
-      <c r="C55" s="58" t="str">
+      <c r="C55" s="57" t="str">
         <f>Main!E57</f>
         <v>Algeria</v>
       </c>
-      <c r="D55" s="37">
+      <c r="D55" s="35">
         <f>Main!F57/(Main!$F57+Main!$G57)*100</f>
         <v>82</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="13">
         <f>Main!G57/(Main!$F57+Main!$G57)*100</f>
         <v>18</v>
       </c>
-      <c r="F55" s="37">
+      <c r="F55" s="35">
         <f>Main!I57/(Main!$I57+Main!$K57)*100</f>
         <v>87.1</v>
       </c>
-      <c r="G55" s="38">
+      <c r="G55" s="36">
         <f>Main!K57/(Main!$I57+Main!$K57)*100</f>
         <v>12.900000000000006</v>
       </c>
-      <c r="H55" s="37">
+      <c r="H55" s="35">
         <f>Main!L57</f>
         <v>88.9</v>
       </c>
-      <c r="I55" s="9">
+      <c r="I55" s="13">
         <f>Main!M57</f>
         <v>3.2</v>
       </c>
-      <c r="J55" s="38">
+      <c r="J55" s="36">
         <f>Main!N57</f>
         <v>0.8</v>
       </c>
-      <c r="K55" s="19">
+      <c r="K55" s="18">
         <f>Main!O57</f>
         <v>63.4</v>
       </c>
-      <c r="L55" s="9">
+      <c r="L55" s="13">
         <f>Main!P57</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="M55" s="64">
+      <c r="M55" s="63">
         <f>Main!Q57</f>
         <v>1.2</v>
       </c>
-      <c r="N55" s="26">
+      <c r="N55" s="24">
         <f>Main!R57</f>
         <v>4.8</v>
       </c>
-      <c r="O55" s="8">
+      <c r="O55" s="12">
         <f>Main!S57</f>
         <v>4.5</v>
       </c>
-      <c r="P55" s="8">
+      <c r="P55" s="12">
         <f>Main!T57</f>
         <v>4.8</v>
       </c>
-      <c r="Q55" s="26">
+      <c r="Q55" s="24">
         <f>Main!U57</f>
         <v>1.4</v>
       </c>
-      <c r="R55" s="8">
+      <c r="R55" s="12">
         <f>Main!V57</f>
         <v>1.3</v>
       </c>
-      <c r="S55" s="8">
+      <c r="S55" s="12">
         <f>Main!W57</f>
         <v>1.3</v>
       </c>
-      <c r="T55" s="26">
+      <c r="T55" s="24">
         <f>Main!X57</f>
         <v>2</v>
       </c>
-      <c r="U55" s="102">
+      <c r="U55" s="101">
         <f>Main!Y57</f>
         <v>17</v>
       </c>
-      <c r="V55" s="27">
+      <c r="V55" s="25">
         <f>Main!Z57</f>
         <v>1</v>
       </c>
-      <c r="W55" s="26">
+      <c r="W55" s="24">
         <f>Main!AA57</f>
         <v>22</v>
       </c>
-      <c r="X55" s="102">
+      <c r="X55" s="101">
         <f>Main!AB57</f>
         <v>3</v>
       </c>
-      <c r="Y55" s="27">
+      <c r="Y55" s="25">
         <f>Main!AC57</f>
         <v>32</v>
       </c>
@@ -21789,103 +21883,103 @@
       </c>
     </row>
     <row r="56" spans="1:35">
-      <c r="A56" s="48">
+      <c r="A56" s="47">
         <f>Main!C58</f>
         <v>41821</v>
       </c>
-      <c r="B56" s="53" t="str">
+      <c r="B56" s="52" t="str">
         <f>Main!D58</f>
         <v>Argentina</v>
       </c>
-      <c r="C56" s="58" t="str">
+      <c r="C56" s="57" t="str">
         <f>Main!E58</f>
         <v>Switzerland</v>
       </c>
-      <c r="D56" s="37">
+      <c r="D56" s="35">
         <f>Main!F58/(Main!$F58+Main!$G58)*100</f>
         <v>75</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E56" s="13">
         <f>Main!G58/(Main!$F58+Main!$G58)*100</f>
         <v>25</v>
       </c>
-      <c r="F56" s="37">
+      <c r="F56" s="35">
         <f>Main!I58/(Main!$I58+Main!$K58)*100</f>
         <v>77.7</v>
       </c>
-      <c r="G56" s="38">
+      <c r="G56" s="36">
         <f>Main!K58/(Main!$I58+Main!$K58)*100</f>
         <v>22.299999999999997</v>
       </c>
-      <c r="H56" s="37">
+      <c r="H56" s="35">
         <f>Main!L58</f>
         <v>90</v>
       </c>
-      <c r="I56" s="9">
+      <c r="I56" s="13">
         <f>Main!M58</f>
         <v>2.9</v>
       </c>
-      <c r="J56" s="38">
+      <c r="J56" s="36">
         <f>Main!N58</f>
         <v>0.4</v>
       </c>
-      <c r="K56" s="19">
+      <c r="K56" s="18">
         <f>Main!O58</f>
         <v>78</v>
       </c>
-      <c r="L56" s="9">
+      <c r="L56" s="13">
         <f>Main!P58</f>
         <v>2</v>
       </c>
-      <c r="M56" s="64">
+      <c r="M56" s="63">
         <f>Main!Q58</f>
         <v>0.9</v>
       </c>
-      <c r="N56" s="26">
+      <c r="N56" s="24">
         <f>Main!R58</f>
         <v>4.8</v>
       </c>
-      <c r="O56" s="8">
+      <c r="O56" s="12">
         <f>Main!S58</f>
         <v>4.5</v>
       </c>
-      <c r="P56" s="8">
+      <c r="P56" s="12">
         <f>Main!T58</f>
         <v>4.7</v>
       </c>
-      <c r="Q56" s="26">
+      <c r="Q56" s="24">
         <f>Main!U58</f>
         <v>1.9</v>
       </c>
-      <c r="R56" s="8">
+      <c r="R56" s="12">
         <f>Main!V58</f>
         <v>2.6</v>
       </c>
-      <c r="S56" s="8">
+      <c r="S56" s="12">
         <f>Main!W58</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="T56" s="26">
+      <c r="T56" s="24">
         <f>Main!X58</f>
         <v>5</v>
       </c>
-      <c r="U56" s="102">
+      <c r="U56" s="101">
         <f>Main!Y58</f>
         <v>15</v>
       </c>
-      <c r="V56" s="27">
+      <c r="V56" s="25">
         <f>Main!Z58</f>
         <v>1</v>
       </c>
-      <c r="W56" s="26">
+      <c r="W56" s="24">
         <f>Main!AA58</f>
         <v>6</v>
       </c>
-      <c r="X56" s="102">
+      <c r="X56" s="101">
         <f>Main!AB58</f>
         <v>9</v>
       </c>
-      <c r="Y56" s="27">
+      <c r="Y56" s="25">
         <f>Main!AC58</f>
         <v>8</v>
       </c>
@@ -21931,103 +22025,103 @@
       </c>
     </row>
     <row r="57" spans="1:35">
-      <c r="A57" s="48">
+      <c r="A57" s="47">
         <f>Main!C59</f>
         <v>41821</v>
       </c>
-      <c r="B57" s="53" t="str">
+      <c r="B57" s="52" t="str">
         <f>Main!D59</f>
         <v>Belgium</v>
       </c>
-      <c r="C57" s="58" t="str">
+      <c r="C57" s="57" t="str">
         <f>Main!E59</f>
         <v>USA</v>
       </c>
-      <c r="D57" s="37">
+      <c r="D57" s="35">
         <f>Main!F59/(Main!$F59+Main!$G59)*100</f>
         <v>59</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="13">
         <f>Main!G59/(Main!$F59+Main!$G59)*100</f>
         <v>41</v>
       </c>
-      <c r="F57" s="37">
+      <c r="F57" s="35">
         <f>Main!I59/(Main!$I59+Main!$K59)*100</f>
         <v>69.2</v>
       </c>
-      <c r="G57" s="38">
+      <c r="G57" s="36">
         <f>Main!K59/(Main!$I59+Main!$K59)*100</f>
         <v>30.8</v>
       </c>
-      <c r="H57" s="37">
+      <c r="H57" s="35">
         <f>Main!L59</f>
         <v>82</v>
       </c>
-      <c r="I57" s="9">
+      <c r="I57" s="13">
         <f>Main!M59</f>
         <v>2.1</v>
       </c>
-      <c r="J57" s="38">
+      <c r="J57" s="36">
         <f>Main!N59</f>
         <v>0.7</v>
       </c>
-      <c r="K57" s="19">
+      <c r="K57" s="18">
         <f>Main!O59</f>
         <v>77.400000000000006</v>
       </c>
-      <c r="L57" s="9">
+      <c r="L57" s="13">
         <f>Main!P59</f>
         <v>2</v>
       </c>
-      <c r="M57" s="64">
+      <c r="M57" s="63">
         <f>Main!Q59</f>
         <v>1</v>
       </c>
-      <c r="N57" s="26">
+      <c r="N57" s="24">
         <f>Main!R59</f>
         <v>3.6</v>
       </c>
-      <c r="O57" s="8">
+      <c r="O57" s="12">
         <f>Main!S59</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="P57" s="8">
+      <c r="P57" s="12">
         <f>Main!T59</f>
         <v>4.3</v>
       </c>
-      <c r="Q57" s="26">
+      <c r="Q57" s="24">
         <f>Main!U59</f>
         <v>3.6</v>
       </c>
-      <c r="R57" s="8">
+      <c r="R57" s="12">
         <f>Main!V59</f>
         <v>1.7</v>
       </c>
-      <c r="S57" s="8">
+      <c r="S57" s="12">
         <f>Main!W59</f>
         <v>2.6</v>
       </c>
-      <c r="T57" s="26">
+      <c r="T57" s="24">
         <f>Main!X59</f>
         <v>11</v>
       </c>
-      <c r="U57" s="102">
+      <c r="U57" s="101">
         <f>Main!Y59</f>
         <v>11</v>
       </c>
-      <c r="V57" s="27">
+      <c r="V57" s="25">
         <f>Main!Z59</f>
         <v>4</v>
       </c>
-      <c r="W57" s="26">
+      <c r="W57" s="24">
         <f>Main!AA59</f>
         <v>13</v>
       </c>
-      <c r="X57" s="102">
+      <c r="X57" s="101">
         <f>Main!AB59</f>
         <v>9</v>
       </c>
-      <c r="Y57" s="27">
+      <c r="Y57" s="25">
         <f>Main!AC59</f>
         <v>3</v>
       </c>
@@ -22073,103 +22167,103 @@
       </c>
     </row>
     <row r="58" spans="1:35">
-      <c r="A58" s="48">
+      <c r="A58" s="47">
         <f>Main!C60</f>
         <v>41824</v>
       </c>
-      <c r="B58" s="53" t="str">
+      <c r="B58" s="52" t="str">
         <f>Main!D60</f>
         <v>France</v>
       </c>
-      <c r="C58" s="58" t="str">
+      <c r="C58" s="57" t="str">
         <f>Main!E60</f>
         <v>Germany</v>
       </c>
-      <c r="D58" s="37">
+      <c r="D58" s="35">
         <f>Main!F60/(Main!$F60+Main!$G60)*100</f>
         <v>47</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="13">
         <f>Main!G60/(Main!$F60+Main!$G60)*100</f>
         <v>53</v>
       </c>
-      <c r="F58" s="37">
+      <c r="F58" s="35">
         <f>Main!I60/(Main!$I60+Main!$K60)*100</f>
         <v>30.8</v>
       </c>
-      <c r="G58" s="38">
+      <c r="G58" s="36">
         <f>Main!K60/(Main!$I60+Main!$K60)*100</f>
         <v>69.2</v>
       </c>
-      <c r="H58" s="37">
+      <c r="H58" s="35">
         <f>Main!L60</f>
         <v>86.1</v>
       </c>
-      <c r="I58" s="9">
+      <c r="I58" s="13">
         <f>Main!M60</f>
         <v>2.5</v>
       </c>
-      <c r="J58" s="38">
+      <c r="J58" s="36">
         <f>Main!N60</f>
         <v>0.6</v>
       </c>
-      <c r="K58" s="19">
+      <c r="K58" s="18">
         <f>Main!O60</f>
         <v>88.9</v>
       </c>
-      <c r="L58" s="9">
+      <c r="L58" s="13">
         <f>Main!P60</f>
         <v>3.2</v>
       </c>
-      <c r="M58" s="64">
+      <c r="M58" s="63">
         <f>Main!Q60</f>
         <v>0.8</v>
       </c>
-      <c r="N58" s="26">
+      <c r="N58" s="24">
         <f>Main!R60</f>
         <v>3.3</v>
       </c>
-      <c r="O58" s="8">
+      <c r="O58" s="12">
         <f>Main!S60</f>
         <v>4</v>
       </c>
-      <c r="P58" s="8">
+      <c r="P58" s="12">
         <f>Main!T60</f>
         <v>3.7</v>
       </c>
-      <c r="Q58" s="26">
+      <c r="Q58" s="24">
         <f>Main!U60</f>
         <v>4.8</v>
       </c>
-      <c r="R58" s="8">
+      <c r="R58" s="12">
         <f>Main!V60</f>
         <v>4.5</v>
       </c>
-      <c r="S58" s="8">
+      <c r="S58" s="12">
         <f>Main!W60</f>
         <v>4.8</v>
       </c>
-      <c r="T58" s="26">
+      <c r="T58" s="24">
         <f>Main!X60</f>
         <v>17</v>
       </c>
-      <c r="U58" s="102">
+      <c r="U58" s="101">
         <f>Main!Y60</f>
         <v>13</v>
       </c>
-      <c r="V58" s="27">
+      <c r="V58" s="25">
         <f>Main!Z60</f>
         <v>1</v>
       </c>
-      <c r="W58" s="26">
+      <c r="W58" s="24">
         <f>Main!AA60</f>
         <v>2</v>
       </c>
-      <c r="X58" s="102">
+      <c r="X58" s="101">
         <f>Main!AB60</f>
         <v>17</v>
       </c>
-      <c r="Y58" s="27">
+      <c r="Y58" s="25">
         <f>Main!AC60</f>
         <v>1</v>
       </c>
@@ -22215,103 +22309,103 @@
       </c>
     </row>
     <row r="59" spans="1:35">
-      <c r="A59" s="48">
+      <c r="A59" s="47">
         <f>Main!C61</f>
         <v>41824</v>
       </c>
-      <c r="B59" s="53" t="str">
+      <c r="B59" s="52" t="str">
         <f>Main!D61</f>
         <v>Brazil</v>
       </c>
-      <c r="C59" s="58" t="str">
+      <c r="C59" s="57" t="str">
         <f>Main!E61</f>
         <v>Colombia</v>
       </c>
-      <c r="D59" s="37">
+      <c r="D59" s="35">
         <f>Main!F61/(Main!$F61+Main!$G61)*100</f>
         <v>72</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="13">
         <f>Main!G61/(Main!$F61+Main!$G61)*100</f>
         <v>28.000000000000004</v>
       </c>
-      <c r="F59" s="37">
+      <c r="F59" s="35">
         <f>Main!I61/(Main!$I61+Main!$K61)*100</f>
         <v>71.400000000000006</v>
       </c>
-      <c r="G59" s="38">
+      <c r="G59" s="36">
         <f>Main!K61/(Main!$I61+Main!$K61)*100</f>
         <v>28.599999999999991</v>
       </c>
-      <c r="H59" s="37">
+      <c r="H59" s="35">
         <f>Main!L61</f>
         <v>91.8</v>
       </c>
-      <c r="I59" s="9">
+      <c r="I59" s="13">
         <f>Main!M61</f>
         <v>3.4</v>
       </c>
-      <c r="J59" s="38">
+      <c r="J59" s="36">
         <f>Main!N61</f>
         <v>0.5</v>
       </c>
-      <c r="K59" s="19">
+      <c r="K59" s="18">
         <f>Main!O61</f>
         <v>85.8</v>
       </c>
-      <c r="L59" s="9">
+      <c r="L59" s="13">
         <f>Main!P61</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="M59" s="64">
+      <c r="M59" s="63">
         <f>Main!Q61</f>
         <v>0.5</v>
       </c>
-      <c r="N59" s="26">
+      <c r="N59" s="24">
         <f>Main!R61</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="O59" s="8">
+      <c r="O59" s="12">
         <f>Main!S61</f>
         <v>4.8</v>
       </c>
-      <c r="P59" s="8">
+      <c r="P59" s="12">
         <f>Main!T61</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="Q59" s="26">
+      <c r="Q59" s="24">
         <f>Main!U61</f>
         <v>3.9</v>
       </c>
-      <c r="R59" s="8">
+      <c r="R59" s="12">
         <f>Main!V61</f>
         <v>4</v>
       </c>
-      <c r="S59" s="8">
+      <c r="S59" s="12">
         <f>Main!W61</f>
         <v>4</v>
       </c>
-      <c r="T59" s="26">
+      <c r="T59" s="24">
         <f>Main!X61</f>
         <v>3</v>
       </c>
-      <c r="U59" s="102">
+      <c r="U59" s="101">
         <f>Main!Y61</f>
         <v>19</v>
       </c>
-      <c r="V59" s="27">
+      <c r="V59" s="25">
         <f>Main!Z61</f>
         <v>1</v>
       </c>
-      <c r="W59" s="26">
+      <c r="W59" s="24">
         <f>Main!AA61</f>
         <v>8</v>
       </c>
-      <c r="X59" s="102">
+      <c r="X59" s="101">
         <f>Main!AB61</f>
         <v>4</v>
       </c>
-      <c r="Y59" s="27">
+      <c r="Y59" s="25">
         <f>Main!AC61</f>
         <v>16</v>
       </c>
@@ -22357,103 +22451,103 @@
       </c>
     </row>
     <row r="60" spans="1:35">
-      <c r="A60" s="48">
+      <c r="A60" s="47">
         <f>Main!C62</f>
         <v>41825</v>
       </c>
-      <c r="B60" s="53" t="str">
+      <c r="B60" s="52" t="str">
         <f>Main!D62</f>
         <v>Argentina</v>
       </c>
-      <c r="C60" s="58" t="str">
+      <c r="C60" s="57" t="str">
         <f>Main!E62</f>
         <v>Belgium</v>
       </c>
-      <c r="D60" s="37">
+      <c r="D60" s="35">
         <f>Main!F62/(Main!$F62+Main!$G62)*100</f>
         <v>72</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="13">
         <f>Main!G62/(Main!$F62+Main!$G62)*100</f>
         <v>28.000000000000004</v>
       </c>
-      <c r="F60" s="37">
+      <c r="F60" s="35">
         <f>Main!I62/(Main!$I62+Main!$K62)*100</f>
         <v>58.20000000000001</v>
       </c>
-      <c r="G60" s="38">
+      <c r="G60" s="36">
         <f>Main!K62/(Main!$I62+Main!$K62)*100</f>
         <v>41.8</v>
       </c>
-      <c r="H60" s="37">
+      <c r="H60" s="35">
         <f>Main!L62</f>
         <v>90</v>
       </c>
-      <c r="I60" s="9">
+      <c r="I60" s="13">
         <f>Main!M62</f>
         <v>2.9</v>
       </c>
-      <c r="J60" s="38">
+      <c r="J60" s="36">
         <f>Main!N62</f>
         <v>0.4</v>
       </c>
-      <c r="K60" s="19">
+      <c r="K60" s="18">
         <f>Main!O62</f>
         <v>82</v>
       </c>
-      <c r="L60" s="9">
+      <c r="L60" s="13">
         <f>Main!P62</f>
         <v>2.1</v>
       </c>
-      <c r="M60" s="64">
+      <c r="M60" s="63">
         <f>Main!Q62</f>
         <v>0.7</v>
       </c>
-      <c r="N60" s="26">
+      <c r="N60" s="24">
         <f>Main!R62</f>
         <v>4.8</v>
       </c>
-      <c r="O60" s="8">
+      <c r="O60" s="12">
         <f>Main!S62</f>
         <v>4.5</v>
       </c>
-      <c r="P60" s="8">
+      <c r="P60" s="12">
         <f>Main!T62</f>
         <v>4.7</v>
       </c>
-      <c r="Q60" s="26">
+      <c r="Q60" s="24">
         <f>Main!U62</f>
         <v>3.6</v>
       </c>
-      <c r="R60" s="8">
+      <c r="R60" s="12">
         <f>Main!V62</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="S60" s="8">
+      <c r="S60" s="12">
         <f>Main!W62</f>
         <v>4.3</v>
       </c>
-      <c r="T60" s="26">
+      <c r="T60" s="24">
         <f>Main!X62</f>
         <v>5</v>
       </c>
-      <c r="U60" s="102">
+      <c r="U60" s="101">
         <f>Main!Y62</f>
         <v>15</v>
       </c>
-      <c r="V60" s="27">
+      <c r="V60" s="25">
         <f>Main!Z62</f>
         <v>1</v>
       </c>
-      <c r="W60" s="26">
+      <c r="W60" s="24">
         <f>Main!AA62</f>
         <v>11</v>
       </c>
-      <c r="X60" s="102">
+      <c r="X60" s="101">
         <f>Main!AB62</f>
         <v>11</v>
       </c>
-      <c r="Y60" s="27">
+      <c r="Y60" s="25">
         <f>Main!AC62</f>
         <v>4</v>
       </c>
@@ -22499,103 +22593,103 @@
       </c>
     </row>
     <row r="61" spans="1:35">
-      <c r="A61" s="48">
+      <c r="A61" s="47">
         <f>Main!C63</f>
         <v>41825</v>
       </c>
-      <c r="B61" s="53" t="str">
+      <c r="B61" s="52" t="str">
         <f>Main!D63</f>
         <v>Netherlands</v>
       </c>
-      <c r="C61" s="58" t="str">
+      <c r="C61" s="57" t="str">
         <f>Main!E63</f>
         <v>Costa Rica</v>
       </c>
-      <c r="D61" s="37">
+      <c r="D61" s="35">
         <f>Main!F63/(Main!$F63+Main!$G63)*100</f>
         <v>76</v>
       </c>
-      <c r="E61" s="9">
+      <c r="E61" s="13">
         <f>Main!G63/(Main!$F63+Main!$G63)*100</f>
         <v>24</v>
       </c>
-      <c r="F61" s="37">
+      <c r="F61" s="35">
         <f>Main!I63/(Main!$I63+Main!$K63)*100</f>
         <v>85.3</v>
       </c>
-      <c r="G61" s="38">
+      <c r="G61" s="36">
         <f>Main!K63/(Main!$I63+Main!$K63)*100</f>
         <v>14.700000000000003</v>
       </c>
-      <c r="H61" s="37">
+      <c r="H61" s="35">
         <f>Main!L63</f>
         <v>82.5</v>
       </c>
-      <c r="I61" s="9">
+      <c r="I61" s="13">
         <f>Main!M63</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="J61" s="38">
+      <c r="J61" s="36">
         <f>Main!N63</f>
         <v>0.8</v>
       </c>
-      <c r="K61" s="19">
+      <c r="K61" s="18">
         <f>Main!O63</f>
         <v>74.099999999999994</v>
       </c>
-      <c r="L61" s="9">
+      <c r="L61" s="13">
         <f>Main!P63</f>
         <v>1.3</v>
       </c>
-      <c r="M61" s="64">
+      <c r="M61" s="63">
         <f>Main!Q63</f>
         <v>0.7</v>
       </c>
-      <c r="N61" s="26">
+      <c r="N61" s="24">
         <f>Main!R63</f>
         <v>3.9</v>
       </c>
-      <c r="O61" s="8">
+      <c r="O61" s="12">
         <f>Main!S63</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="P61" s="8">
+      <c r="P61" s="12">
         <f>Main!T63</f>
         <v>4.2</v>
       </c>
-      <c r="Q61" s="26">
+      <c r="Q61" s="24">
         <f>Main!U63</f>
         <v>1.6</v>
       </c>
-      <c r="R61" s="8">
+      <c r="R61" s="12">
         <f>Main!V63</f>
         <v>1.2</v>
       </c>
-      <c r="S61" s="8">
+      <c r="S61" s="12">
         <f>Main!W63</f>
         <v>1.3</v>
       </c>
-      <c r="T61" s="26">
+      <c r="T61" s="24">
         <f>Main!X63</f>
         <v>15</v>
       </c>
-      <c r="U61" s="102">
+      <c r="U61" s="101">
         <f>Main!Y63</f>
         <v>9</v>
       </c>
-      <c r="V61" s="27">
+      <c r="V61" s="25">
         <f>Main!Z63</f>
         <v>2</v>
       </c>
-      <c r="W61" s="26">
+      <c r="W61" s="24">
         <f>Main!AA63</f>
         <v>28</v>
       </c>
-      <c r="X61" s="102">
+      <c r="X61" s="101">
         <f>Main!AB63</f>
         <v>3</v>
       </c>
-      <c r="Y61" s="27">
+      <c r="Y61" s="25">
         <f>Main!AC63</f>
         <v>16</v>
       </c>
@@ -22641,103 +22735,103 @@
       </c>
     </row>
     <row r="62" spans="1:35">
-      <c r="A62" s="48">
+      <c r="A62" s="47">
         <f>Main!C64</f>
         <v>41828</v>
       </c>
-      <c r="B62" s="53" t="str">
+      <c r="B62" s="52" t="str">
         <f>Main!D64</f>
         <v>Brazil</v>
       </c>
-      <c r="C62" s="58" t="str">
+      <c r="C62" s="57" t="str">
         <f>Main!E64</f>
         <v>Germany</v>
       </c>
-      <c r="D62" s="37">
+      <c r="D62" s="35">
         <f>Main!F64/(Main!$F64+Main!$G64)*100</f>
         <v>73</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="13">
         <f>Main!G64/(Main!$F64+Main!$G64)*100</f>
         <v>27</v>
       </c>
-      <c r="F62" s="37">
+      <c r="F62" s="35">
         <f>Main!I64/(Main!$I64+Main!$K64)*100</f>
         <v>49.2</v>
       </c>
-      <c r="G62" s="38">
+      <c r="G62" s="36">
         <f>Main!K64/(Main!$I64+Main!$K64)*100</f>
         <v>50.8</v>
       </c>
-      <c r="H62" s="37">
+      <c r="H62" s="35">
         <f>Main!L64</f>
         <v>91.8</v>
       </c>
-      <c r="I62" s="9">
+      <c r="I62" s="13">
         <f>Main!M64</f>
         <v>3.4</v>
       </c>
-      <c r="J62" s="38">
+      <c r="J62" s="36">
         <f>Main!N64</f>
         <v>0.5</v>
       </c>
-      <c r="K62" s="19">
+      <c r="K62" s="18">
         <f>Main!O64</f>
         <v>88.9</v>
       </c>
-      <c r="L62" s="9">
+      <c r="L62" s="13">
         <f>Main!P64</f>
         <v>3.2</v>
       </c>
-      <c r="M62" s="64">
+      <c r="M62" s="63">
         <f>Main!Q64</f>
         <v>0.8</v>
       </c>
-      <c r="N62" s="26">
+      <c r="N62" s="24">
         <f>Main!R64</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="O62" s="8">
+      <c r="O62" s="12">
         <f>Main!S64</f>
         <v>4.8</v>
       </c>
-      <c r="P62" s="8">
+      <c r="P62" s="12">
         <f>Main!T64</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="Q62" s="26">
+      <c r="Q62" s="24">
         <f>Main!U64</f>
         <v>4.8</v>
       </c>
-      <c r="R62" s="8">
+      <c r="R62" s="12">
         <f>Main!V64</f>
         <v>4.5</v>
       </c>
-      <c r="S62" s="8">
+      <c r="S62" s="12">
         <f>Main!W64</f>
         <v>4.8</v>
       </c>
-      <c r="T62" s="26">
+      <c r="T62" s="24">
         <f>Main!X64</f>
         <v>3</v>
       </c>
-      <c r="U62" s="102">
+      <c r="U62" s="101">
         <f>Main!Y64</f>
         <v>19</v>
       </c>
-      <c r="V62" s="27">
+      <c r="V62" s="25">
         <f>Main!Z64</f>
         <v>1</v>
       </c>
-      <c r="W62" s="26">
+      <c r="W62" s="24">
         <f>Main!AA64</f>
         <v>2</v>
       </c>
-      <c r="X62" s="102">
+      <c r="X62" s="101">
         <f>Main!AB64</f>
         <v>17</v>
       </c>
-      <c r="Y62" s="27">
+      <c r="Y62" s="25">
         <f>Main!AC64</f>
         <v>1</v>
       </c>
@@ -22783,103 +22877,103 @@
       </c>
     </row>
     <row r="63" spans="1:35">
-      <c r="A63" s="48">
+      <c r="A63" s="47">
         <f>Main!C65</f>
         <v>41829</v>
       </c>
-      <c r="B63" s="53" t="str">
+      <c r="B63" s="52" t="str">
         <f>Main!D65</f>
         <v>Netherlands</v>
       </c>
-      <c r="C63" s="58" t="str">
+      <c r="C63" s="57" t="str">
         <f>Main!E65</f>
         <v>Argentina</v>
       </c>
-      <c r="D63" s="37">
+      <c r="D63" s="35">
         <f>Main!F65/(Main!$F65+Main!$G65)*100</f>
         <v>43</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E63" s="13">
         <f>Main!G65/(Main!$F65+Main!$G65)*100</f>
         <v>56.999999999999993</v>
       </c>
-      <c r="F63" s="37">
+      <c r="F63" s="35">
         <f>Main!I65/(Main!$I65+Main!$K65)*100</f>
         <v>39.299999999999997</v>
       </c>
-      <c r="G63" s="38">
+      <c r="G63" s="36">
         <f>Main!K65/(Main!$I65+Main!$K65)*100</f>
         <v>60.699999999999996</v>
       </c>
-      <c r="H63" s="37">
+      <c r="H63" s="35">
         <f>Main!L65</f>
         <v>82.5</v>
       </c>
-      <c r="I63" s="9">
+      <c r="I63" s="13">
         <f>Main!M65</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="J63" s="38">
+      <c r="J63" s="36">
         <f>Main!N65</f>
         <v>0.8</v>
       </c>
-      <c r="K63" s="19">
+      <c r="K63" s="18">
         <f>Main!O65</f>
         <v>90</v>
       </c>
-      <c r="L63" s="9">
+      <c r="L63" s="13">
         <f>Main!P65</f>
         <v>2.9</v>
       </c>
-      <c r="M63" s="64">
+      <c r="M63" s="63">
         <f>Main!Q65</f>
         <v>0.4</v>
       </c>
-      <c r="N63" s="26">
+      <c r="N63" s="24">
         <f>Main!R65</f>
         <v>3.9</v>
       </c>
-      <c r="O63" s="8">
+      <c r="O63" s="12">
         <f>Main!S65</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="P63" s="8">
+      <c r="P63" s="12">
         <f>Main!T65</f>
         <v>4.2</v>
       </c>
-      <c r="Q63" s="26">
+      <c r="Q63" s="24">
         <f>Main!U65</f>
         <v>4.8</v>
       </c>
-      <c r="R63" s="8">
+      <c r="R63" s="12">
         <f>Main!V65</f>
         <v>4.5</v>
       </c>
-      <c r="S63" s="8">
+      <c r="S63" s="12">
         <f>Main!W65</f>
         <v>4.7</v>
       </c>
-      <c r="T63" s="26">
+      <c r="T63" s="24">
         <f>Main!X65</f>
         <v>15</v>
       </c>
-      <c r="U63" s="102">
+      <c r="U63" s="101">
         <f>Main!Y65</f>
         <v>9</v>
       </c>
-      <c r="V63" s="27">
+      <c r="V63" s="25">
         <f>Main!Z65</f>
         <v>2</v>
       </c>
-      <c r="W63" s="26">
+      <c r="W63" s="24">
         <f>Main!AA65</f>
         <v>5</v>
       </c>
-      <c r="X63" s="102">
+      <c r="X63" s="101">
         <f>Main!AB65</f>
         <v>15</v>
       </c>
-      <c r="Y63" s="27">
+      <c r="Y63" s="25">
         <f>Main!AC65</f>
         <v>1</v>
       </c>
@@ -22921,6 +23015,290 @@
       </c>
       <c r="AI63" s="188" t="str">
         <f>Main!AM65</f>
+        <v>train</v>
+      </c>
+    </row>
+    <row r="64" spans="1:35">
+      <c r="A64" s="48">
+        <f>Main!C66</f>
+        <v>41832</v>
+      </c>
+      <c r="B64" s="53" t="str">
+        <f>Main!D66</f>
+        <v>Brazil</v>
+      </c>
+      <c r="C64" s="58" t="str">
+        <f>Main!E66</f>
+        <v>Netherlands</v>
+      </c>
+      <c r="D64" s="37">
+        <f>Main!F66/(Main!$F66+Main!$G66)*100</f>
+        <v>50</v>
+      </c>
+      <c r="E64" s="9">
+        <f>Main!G66/(Main!$F66+Main!$G66)*100</f>
+        <v>50</v>
+      </c>
+      <c r="F64" s="37">
+        <f>Main!I66/(Main!$I66+Main!$K66)*100</f>
+        <v>60.6</v>
+      </c>
+      <c r="G64" s="38">
+        <f>Main!K66/(Main!$I66+Main!$K66)*100</f>
+        <v>39.4</v>
+      </c>
+      <c r="H64" s="37">
+        <f>Main!L66</f>
+        <v>91.8</v>
+      </c>
+      <c r="I64" s="9">
+        <f>Main!M66</f>
+        <v>3.4</v>
+      </c>
+      <c r="J64" s="38">
+        <f>Main!N66</f>
+        <v>0.5</v>
+      </c>
+      <c r="K64" s="19">
+        <f>Main!O66</f>
+        <v>82.5</v>
+      </c>
+      <c r="L64" s="9">
+        <f>Main!P66</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M64" s="64">
+        <f>Main!Q66</f>
+        <v>0.8</v>
+      </c>
+      <c r="N64" s="26">
+        <f>Main!R66</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="O64" s="8">
+        <f>Main!S66</f>
+        <v>4.8</v>
+      </c>
+      <c r="P64" s="8">
+        <f>Main!T66</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q64" s="26">
+        <f>Main!U66</f>
+        <v>3.9</v>
+      </c>
+      <c r="R64" s="8">
+        <f>Main!V66</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S64" s="8">
+        <f>Main!W66</f>
+        <v>4.2</v>
+      </c>
+      <c r="T64" s="26">
+        <f>Main!X66</f>
+        <v>3</v>
+      </c>
+      <c r="U64" s="102">
+        <f>Main!Y66</f>
+        <v>19</v>
+      </c>
+      <c r="V64" s="27">
+        <f>Main!Z66</f>
+        <v>1</v>
+      </c>
+      <c r="W64" s="26">
+        <f>Main!AA66</f>
+        <v>15</v>
+      </c>
+      <c r="X64" s="102">
+        <f>Main!AB66</f>
+        <v>9</v>
+      </c>
+      <c r="Y64" s="27">
+        <f>Main!AC66</f>
+        <v>2</v>
+      </c>
+      <c r="Z64" s="173">
+        <f>Main!AD66</f>
+        <v>2.15</v>
+      </c>
+      <c r="AA64" s="174">
+        <f>Main!AE66</f>
+        <v>3.6</v>
+      </c>
+      <c r="AB64" s="175">
+        <f>Main!AF66</f>
+        <v>3.2</v>
+      </c>
+      <c r="AC64" s="183">
+        <f>Main!AG66</f>
+        <v>0</v>
+      </c>
+      <c r="AD64" s="184">
+        <f>Main!AH66</f>
+        <v>0</v>
+      </c>
+      <c r="AE64" s="151">
+        <f>Main!AI66</f>
+        <v>0</v>
+      </c>
+      <c r="AF64" s="156">
+        <f>Main!AJ66</f>
+        <v>0</v>
+      </c>
+      <c r="AG64" s="157">
+        <f>Main!AK66</f>
+        <v>0</v>
+      </c>
+      <c r="AH64" s="158">
+        <f>Main!AL66</f>
+        <v>0</v>
+      </c>
+      <c r="AI64" s="188" t="str">
+        <f>Main!AM66</f>
+        <v>predict</v>
+      </c>
+    </row>
+    <row r="65" spans="1:35">
+      <c r="A65" s="48">
+        <f>Main!C67</f>
+        <v>41833</v>
+      </c>
+      <c r="B65" s="53" t="str">
+        <f>Main!D67</f>
+        <v>Germany</v>
+      </c>
+      <c r="C65" s="58" t="str">
+        <f>Main!E67</f>
+        <v>Argentina</v>
+      </c>
+      <c r="D65" s="37">
+        <f>Main!F67/(Main!$F67+Main!$G67)*100</f>
+        <v>63</v>
+      </c>
+      <c r="E65" s="9">
+        <f>Main!G67/(Main!$F67+Main!$G67)*100</f>
+        <v>37</v>
+      </c>
+      <c r="F65" s="37">
+        <f>Main!I67/(Main!$I67+Main!$K67)*100</f>
+        <v>50.9</v>
+      </c>
+      <c r="G65" s="38">
+        <f>Main!K67/(Main!$I67+Main!$K67)*100</f>
+        <v>49.1</v>
+      </c>
+      <c r="H65" s="37">
+        <f>Main!L67</f>
+        <v>88.9</v>
+      </c>
+      <c r="I65" s="9">
+        <f>Main!M67</f>
+        <v>3.2</v>
+      </c>
+      <c r="J65" s="38">
+        <f>Main!N67</f>
+        <v>0.8</v>
+      </c>
+      <c r="K65" s="19">
+        <f>Main!O67</f>
+        <v>90</v>
+      </c>
+      <c r="L65" s="9">
+        <f>Main!P67</f>
+        <v>2.9</v>
+      </c>
+      <c r="M65" s="64">
+        <f>Main!Q67</f>
+        <v>0.4</v>
+      </c>
+      <c r="N65" s="26">
+        <f>Main!R67</f>
+        <v>4.8</v>
+      </c>
+      <c r="O65" s="8">
+        <f>Main!S67</f>
+        <v>4.5</v>
+      </c>
+      <c r="P65" s="8">
+        <f>Main!T67</f>
+        <v>4.8</v>
+      </c>
+      <c r="Q65" s="26">
+        <f>Main!U67</f>
+        <v>4.8</v>
+      </c>
+      <c r="R65" s="8">
+        <f>Main!V67</f>
+        <v>4.5</v>
+      </c>
+      <c r="S65" s="8">
+        <f>Main!W67</f>
+        <v>4.7</v>
+      </c>
+      <c r="T65" s="26">
+        <f>Main!X67</f>
+        <v>2</v>
+      </c>
+      <c r="U65" s="102">
+        <f>Main!Y67</f>
+        <v>17</v>
+      </c>
+      <c r="V65" s="27">
+        <f>Main!Z67</f>
+        <v>1</v>
+      </c>
+      <c r="W65" s="26">
+        <f>Main!AA67</f>
+        <v>5</v>
+      </c>
+      <c r="X65" s="102">
+        <f>Main!AB67</f>
+        <v>15</v>
+      </c>
+      <c r="Y65" s="27">
+        <f>Main!AC67</f>
+        <v>1</v>
+      </c>
+      <c r="Z65" s="173">
+        <f>Main!AD67</f>
+        <v>2.25</v>
+      </c>
+      <c r="AA65" s="174">
+        <f>Main!AE67</f>
+        <v>3.1</v>
+      </c>
+      <c r="AB65" s="175">
+        <f>Main!AF67</f>
+        <v>3.4</v>
+      </c>
+      <c r="AC65" s="183">
+        <f>Main!AG67</f>
+        <v>0</v>
+      </c>
+      <c r="AD65" s="184">
+        <f>Main!AH67</f>
+        <v>0</v>
+      </c>
+      <c r="AE65" s="151">
+        <f>Main!AI67</f>
+        <v>0</v>
+      </c>
+      <c r="AF65" s="156">
+        <f>Main!AJ67</f>
+        <v>0</v>
+      </c>
+      <c r="AG65" s="157">
+        <f>Main!AK67</f>
+        <v>0</v>
+      </c>
+      <c r="AH65" s="158">
+        <f>Main!AL67</f>
+        <v>0</v>
+      </c>
+      <c r="AI65" s="188" t="str">
+        <f>Main!AM67</f>
         <v>predict</v>
       </c>
     </row>

</xml_diff>